<commit_message>
+ add report xxbkrp.p
</commit_message>
<xml_diff>
--- a/bookmg/initial/cim.xlsx
+++ b/bookmg/initial/cim.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="2505" windowWidth="14295" windowHeight="7020" tabRatio="944" activeTab="3"/>
+    <workbookView xWindow="9555" yWindow="2505" windowWidth="14295" windowHeight="7020" tabRatio="944"/>
   </bookViews>
   <sheets>
     <sheet name="00-mgmemt.p" sheetId="8" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="283">
   <si>
     <t>mgmsgmt.p</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -780,10 +780,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>""</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>xxbkld.p</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -796,10 +792,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>''</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>图书归还</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -813,10 +805,6 @@
   </si>
   <si>
     <t>BOOK_TYPE</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOOK_STATUS</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -1210,39 +1198,185 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>书籍为不可借状态</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>书籍已被 # 借出</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不允许删除借阅记录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>书籍未被借出</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>书籍已归还不允许修改</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>书籍不存在</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不存在此日期的借书记录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxbcrp.p</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxbkrp.p</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>5/1-c</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>6/1-c</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>""</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>""</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_days</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>TO</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOK_TYPE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_bktype</t>
+  </si>
+  <si>
+    <t>v_book</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_book1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>v_avail</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>v_days</t>
-  </si>
-  <si>
-    <t>书籍为不可借状态</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>书籍已被 # 借出</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>不允许删除借阅记录</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>书籍未被借出</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>书籍已归还不允许修改</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>书籍不存在</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>不存在此日期的借书记录</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>BOOK_STATUS</t>
+  </si>
+  <si>
+    <t>BOOK_STATUS</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_bkstat</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_start1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_start</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_lendcnt</t>
+  </si>
+  <si>
+    <t>CH</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BORROW_TIMES</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>借阅次数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>次数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_bc</t>
+  </si>
+  <si>
+    <t>v_bcname</t>
+  </si>
+  <si>
+    <t>v_blstart</t>
+  </si>
+  <si>
+    <t>v_end</t>
+  </si>
+  <si>
+    <t>AVAILABLE_BRROW</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>可借</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>可</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>图书借阅报表</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>读者借阅统计</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1420,9 +1554,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
@@ -1436,6 +1567,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1733,13 +1867,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5"/>
@@ -1754,12 +1888,12 @@
     <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -1785,7 +1919,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" s="6" t="s">
         <v>133</v>
       </c>
@@ -1808,8 +1942,14 @@
       <c r="H4" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1">
+      <c r="I4" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="J4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1822,18 +1962,18 @@
       <c r="D5" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>161</v>
-      </c>
       <c r="F5" s="2">
         <v>4</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5" t="s">
+        <v>247</v>
+      </c>
+      <c r="J5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1846,17 +1986,17 @@
       <c r="D6" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>161</v>
-      </c>
       <c r="F6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" t="s">
+        <v>248</v>
+      </c>
+      <c r="J6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1869,215 +2009,267 @@
       <c r="D7" t="s">
         <v>156</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>161</v>
-      </c>
       <c r="F7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I7" t="s">
+        <v>251</v>
+      </c>
+      <c r="J7" t="s">
+        <v>252</v>
+      </c>
+      <c r="K7" t="s">
         <v>158</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="I7" t="s">
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>160</v>
-      </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E8" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" t="s">
         <v>161</v>
       </c>
-      <c r="F8" t="s">
-        <v>163</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>161</v>
-      </c>
       <c r="I8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J8" t="s">
+        <v>252</v>
+      </c>
+      <c r="K8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>160</v>
-      </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>161</v>
+        <v>281</v>
       </c>
       <c r="F9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>161</v>
+        <v>244</v>
       </c>
       <c r="I9" t="s">
+        <v>251</v>
+      </c>
+      <c r="J9" t="s">
+        <v>252</v>
+      </c>
+      <c r="K9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>160</v>
-      </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>161</v>
+        <v>282</v>
       </c>
       <c r="F10" t="s">
-        <v>150</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>161</v>
+        <v>243</v>
       </c>
       <c r="I10" t="s">
+        <v>251</v>
+      </c>
+      <c r="J10" t="s">
+        <v>252</v>
+      </c>
+      <c r="K10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>160</v>
-      </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C11">
         <v>13</v>
       </c>
       <c r="D11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" t="s">
+        <v>251</v>
+      </c>
+      <c r="J11" t="s">
+        <v>252</v>
+      </c>
+      <c r="K11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
         <v>151</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>155</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
+        <v>251</v>
+      </c>
+      <c r="J12" t="s">
+        <v>252</v>
+      </c>
+      <c r="K12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C12">
+      <c r="B13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>152</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="I13" t="s">
+        <v>251</v>
+      </c>
+      <c r="J13" t="s">
+        <v>252</v>
+      </c>
+      <c r="K13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C13">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>149</v>
+      </c>
+      <c r="F14" t="s">
+        <v>150</v>
+      </c>
+      <c r="I14" t="s">
+        <v>251</v>
+      </c>
+      <c r="J14" t="s">
+        <v>252</v>
+      </c>
+      <c r="K14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
         <v>153</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>126</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="I15" t="s">
+        <v>251</v>
+      </c>
+      <c r="J15" t="s">
+        <v>252</v>
+      </c>
+      <c r="K15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>160</v>
-      </c>
-      <c r="B14" t="s">
-        <v>160</v>
-      </c>
-      <c r="C14">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
         <v>154</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="F16" t="s">
         <v>118</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>161</v>
+      <c r="I16" t="s">
+        <v>253</v>
+      </c>
+      <c r="J16" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C983045:C1048576 C917509:C983040 C851973:C917504 C786437:C851968 C720901:C786432 C655365:C720896 C589829:C655360 C524293:C589824 C458757:C524288 C393221:C458752 C327685:C393216 C262149:C327680 C196613:C262144 C131077:C196608 C65541:C131072 C9 C5:C7 C11:C65536 SR5:SR65536 ACN5:ACN65536 AMJ5:AMJ65536 AWF5:AWF65536 BGB5:BGB65536 BPX5:BPX65536 BZT5:BZT65536 CJP5:CJP65536 CTL5:CTL65536 DDH5:DDH65536 DND5:DND65536 DWZ5:DWZ65536 EGV5:EGV65536 EQR5:EQR65536 FAN5:FAN65536 FKJ5:FKJ65536 FUF5:FUF65536 GEB5:GEB65536 GNX5:GNX65536 GXT5:GXT65536 HHP5:HHP65536 HRL5:HRL65536 IBH5:IBH65536 ILD5:ILD65536 IUZ5:IUZ65536 JEV5:JEV65536 JOR5:JOR65536 JYN5:JYN65536 KIJ5:KIJ65536 KSF5:KSF65536 LCB5:LCB65536 LLX5:LLX65536 LVT5:LVT65536 MFP5:MFP65536 MPL5:MPL65536 MZH5:MZH65536 NJD5:NJD65536 NSZ5:NSZ65536 OCV5:OCV65536 OMR5:OMR65536 OWN5:OWN65536 PGJ5:PGJ65536 PQF5:PQF65536 QAB5:QAB65536 QJX5:QJX65536 QTT5:QTT65536 RDP5:RDP65536 RNL5:RNL65536 RXH5:RXH65536 SHD5:SHD65536 SQZ5:SQZ65536 TAV5:TAV65536 TKR5:TKR65536 TUN5:TUN65536 UEJ5:UEJ65536 UOF5:UOF65536 UYB5:UYB65536 VHX5:VHX65536 VRT5:VRT65536 WBP5:WBP65536 WLL5:WLL65536 WVH5:WVH65536 IV65541:IV131072 SR65541:SR131072 ACN65541:ACN131072 AMJ65541:AMJ131072 AWF65541:AWF131072 BGB65541:BGB131072 BPX65541:BPX131072 BZT65541:BZT131072 CJP65541:CJP131072 CTL65541:CTL131072 DDH65541:DDH131072 DND65541:DND131072 DWZ65541:DWZ131072 EGV65541:EGV131072 EQR65541:EQR131072 FAN65541:FAN131072 FKJ65541:FKJ131072 FUF65541:FUF131072 GEB65541:GEB131072 GNX65541:GNX131072 GXT65541:GXT131072 HHP65541:HHP131072 HRL65541:HRL131072 IBH65541:IBH131072 ILD65541:ILD131072 IUZ65541:IUZ131072 JEV65541:JEV131072 JOR65541:JOR131072 JYN65541:JYN131072 KIJ65541:KIJ131072 KSF65541:KSF131072 LCB65541:LCB131072 LLX65541:LLX131072 LVT65541:LVT131072 MFP65541:MFP131072 MPL65541:MPL131072 MZH65541:MZH131072 NJD65541:NJD131072 NSZ65541:NSZ131072 OCV65541:OCV131072 OMR65541:OMR131072 OWN65541:OWN131072 PGJ65541:PGJ131072 PQF65541:PQF131072 QAB65541:QAB131072 QJX65541:QJX131072 QTT65541:QTT131072 RDP65541:RDP131072 RNL65541:RNL131072 RXH65541:RXH131072 SHD65541:SHD131072 SQZ65541:SQZ131072 TAV65541:TAV131072 TKR65541:TKR131072 TUN65541:TUN131072 UEJ65541:UEJ131072 UOF65541:UOF131072 UYB65541:UYB131072 VHX65541:VHX131072 VRT65541:VRT131072 WBP65541:WBP131072 WLL65541:WLL131072 WVH65541:WVH131072 IV131077:IV196608 SR131077:SR196608 ACN131077:ACN196608 AMJ131077:AMJ196608 AWF131077:AWF196608 BGB131077:BGB196608 BPX131077:BPX196608 BZT131077:BZT196608 CJP131077:CJP196608 CTL131077:CTL196608 DDH131077:DDH196608 DND131077:DND196608 DWZ131077:DWZ196608 EGV131077:EGV196608 EQR131077:EQR196608 FAN131077:FAN196608 FKJ131077:FKJ196608 FUF131077:FUF196608 GEB131077:GEB196608 GNX131077:GNX196608 GXT131077:GXT196608 HHP131077:HHP196608 HRL131077:HRL196608 IBH131077:IBH196608 ILD131077:ILD196608 IUZ131077:IUZ196608 JEV131077:JEV196608 JOR131077:JOR196608 JYN131077:JYN196608 KIJ131077:KIJ196608 KSF131077:KSF196608 LCB131077:LCB196608 LLX131077:LLX196608 LVT131077:LVT196608 MFP131077:MFP196608 MPL131077:MPL196608 MZH131077:MZH196608 NJD131077:NJD196608 NSZ131077:NSZ196608 OCV131077:OCV196608 OMR131077:OMR196608 OWN131077:OWN196608 PGJ131077:PGJ196608 PQF131077:PQF196608 QAB131077:QAB196608 QJX131077:QJX196608 QTT131077:QTT196608 RDP131077:RDP196608 RNL131077:RNL196608 RXH131077:RXH196608 SHD131077:SHD196608 SQZ131077:SQZ196608 TAV131077:TAV196608 TKR131077:TKR196608 TUN131077:TUN196608 UEJ131077:UEJ196608 UOF131077:UOF196608 UYB131077:UYB196608 VHX131077:VHX196608 VRT131077:VRT196608 WBP131077:WBP196608 WLL131077:WLL196608 WVH131077:WVH196608 IV196613:IV262144 SR196613:SR262144 ACN196613:ACN262144 AMJ196613:AMJ262144 AWF196613:AWF262144 BGB196613:BGB262144 BPX196613:BPX262144 BZT196613:BZT262144 CJP196613:CJP262144 CTL196613:CTL262144 DDH196613:DDH262144 DND196613:DND262144 DWZ196613:DWZ262144 EGV196613:EGV262144 EQR196613:EQR262144 FAN196613:FAN262144 FKJ196613:FKJ262144 FUF196613:FUF262144 GEB196613:GEB262144 GNX196613:GNX262144 GXT196613:GXT262144 HHP196613:HHP262144 HRL196613:HRL262144 IBH196613:IBH262144 ILD196613:ILD262144 IUZ196613:IUZ262144 JEV196613:JEV262144 JOR196613:JOR262144 JYN196613:JYN262144 KIJ196613:KIJ262144 KSF196613:KSF262144 LCB196613:LCB262144 LLX196613:LLX262144 LVT196613:LVT262144 MFP196613:MFP262144 MPL196613:MPL262144 MZH196613:MZH262144 NJD196613:NJD262144 NSZ196613:NSZ262144 OCV196613:OCV262144 OMR196613:OMR262144 OWN196613:OWN262144 PGJ196613:PGJ262144 PQF196613:PQF262144 QAB196613:QAB262144 QJX196613:QJX262144 QTT196613:QTT262144 RDP196613:RDP262144 RNL196613:RNL262144 RXH196613:RXH262144 SHD196613:SHD262144 SQZ196613:SQZ262144 TAV196613:TAV262144 TKR196613:TKR262144 TUN196613:TUN262144 UEJ196613:UEJ262144 UOF196613:UOF262144 UYB196613:UYB262144 VHX196613:VHX262144 VRT196613:VRT262144 WBP196613:WBP262144 WLL196613:WLL262144 WVH196613:WVH262144 IV262149:IV327680 SR262149:SR327680 ACN262149:ACN327680 AMJ262149:AMJ327680 AWF262149:AWF327680 BGB262149:BGB327680 BPX262149:BPX327680 BZT262149:BZT327680 CJP262149:CJP327680 CTL262149:CTL327680 DDH262149:DDH327680 DND262149:DND327680 DWZ262149:DWZ327680 EGV262149:EGV327680 EQR262149:EQR327680 FAN262149:FAN327680 FKJ262149:FKJ327680 FUF262149:FUF327680 GEB262149:GEB327680 GNX262149:GNX327680 GXT262149:GXT327680 HHP262149:HHP327680 HRL262149:HRL327680 IBH262149:IBH327680 ILD262149:ILD327680 IUZ262149:IUZ327680 JEV262149:JEV327680 JOR262149:JOR327680 JYN262149:JYN327680 KIJ262149:KIJ327680 KSF262149:KSF327680 LCB262149:LCB327680 LLX262149:LLX327680 LVT262149:LVT327680 MFP262149:MFP327680 MPL262149:MPL327680 MZH262149:MZH327680 NJD262149:NJD327680 NSZ262149:NSZ327680 OCV262149:OCV327680 OMR262149:OMR327680 OWN262149:OWN327680 PGJ262149:PGJ327680 PQF262149:PQF327680 QAB262149:QAB327680 QJX262149:QJX327680 QTT262149:QTT327680 RDP262149:RDP327680 RNL262149:RNL327680 RXH262149:RXH327680 SHD262149:SHD327680 SQZ262149:SQZ327680 TAV262149:TAV327680 TKR262149:TKR327680 TUN262149:TUN327680 UEJ262149:UEJ327680 UOF262149:UOF327680 UYB262149:UYB327680 VHX262149:VHX327680 VRT262149:VRT327680 WBP262149:WBP327680 WLL262149:WLL327680 WVH262149:WVH327680 IV327685:IV393216 SR327685:SR393216 ACN327685:ACN393216 AMJ327685:AMJ393216 AWF327685:AWF393216 BGB327685:BGB393216 BPX327685:BPX393216 BZT327685:BZT393216 CJP327685:CJP393216 CTL327685:CTL393216 DDH327685:DDH393216 DND327685:DND393216 DWZ327685:DWZ393216 EGV327685:EGV393216 EQR327685:EQR393216 FAN327685:FAN393216 FKJ327685:FKJ393216 FUF327685:FUF393216 GEB327685:GEB393216 GNX327685:GNX393216 GXT327685:GXT393216 HHP327685:HHP393216 HRL327685:HRL393216 IBH327685:IBH393216 ILD327685:ILD393216 IUZ327685:IUZ393216 JEV327685:JEV393216 JOR327685:JOR393216 JYN327685:JYN393216 KIJ327685:KIJ393216 KSF327685:KSF393216 LCB327685:LCB393216 LLX327685:LLX393216 LVT327685:LVT393216 MFP327685:MFP393216 MPL327685:MPL393216 MZH327685:MZH393216 NJD327685:NJD393216 NSZ327685:NSZ393216 OCV327685:OCV393216 OMR327685:OMR393216 OWN327685:OWN393216 PGJ327685:PGJ393216 PQF327685:PQF393216 QAB327685:QAB393216 QJX327685:QJX393216 QTT327685:QTT393216 RDP327685:RDP393216 RNL327685:RNL393216 RXH327685:RXH393216 SHD327685:SHD393216 SQZ327685:SQZ393216 TAV327685:TAV393216 TKR327685:TKR393216 TUN327685:TUN393216 UEJ327685:UEJ393216 UOF327685:UOF393216 UYB327685:UYB393216 VHX327685:VHX393216 VRT327685:VRT393216 WBP327685:WBP393216 WLL327685:WLL393216 WVH327685:WVH393216 IV393221:IV458752 SR393221:SR458752 ACN393221:ACN458752 AMJ393221:AMJ458752 AWF393221:AWF458752 BGB393221:BGB458752 BPX393221:BPX458752 BZT393221:BZT458752 CJP393221:CJP458752 CTL393221:CTL458752 DDH393221:DDH458752 DND393221:DND458752 DWZ393221:DWZ458752 EGV393221:EGV458752 EQR393221:EQR458752 FAN393221:FAN458752 FKJ393221:FKJ458752 FUF393221:FUF458752 GEB393221:GEB458752 GNX393221:GNX458752 GXT393221:GXT458752 HHP393221:HHP458752 HRL393221:HRL458752 IBH393221:IBH458752 ILD393221:ILD458752 IUZ393221:IUZ458752 JEV393221:JEV458752 JOR393221:JOR458752 JYN393221:JYN458752 KIJ393221:KIJ458752 KSF393221:KSF458752 LCB393221:LCB458752 LLX393221:LLX458752 LVT393221:LVT458752 MFP393221:MFP458752 MPL393221:MPL458752 MZH393221:MZH458752 NJD393221:NJD458752 NSZ393221:NSZ458752 OCV393221:OCV458752 OMR393221:OMR458752 OWN393221:OWN458752 PGJ393221:PGJ458752 PQF393221:PQF458752 QAB393221:QAB458752 QJX393221:QJX458752 QTT393221:QTT458752 RDP393221:RDP458752 RNL393221:RNL458752 RXH393221:RXH458752 SHD393221:SHD458752 SQZ393221:SQZ458752 TAV393221:TAV458752 TKR393221:TKR458752 TUN393221:TUN458752 UEJ393221:UEJ458752 UOF393221:UOF458752 UYB393221:UYB458752 VHX393221:VHX458752 VRT393221:VRT458752 WBP393221:WBP458752 WLL393221:WLL458752 WVH393221:WVH458752 IV458757:IV524288 SR458757:SR524288 ACN458757:ACN524288 AMJ458757:AMJ524288 AWF458757:AWF524288 BGB458757:BGB524288 BPX458757:BPX524288 BZT458757:BZT524288 CJP458757:CJP524288 CTL458757:CTL524288 DDH458757:DDH524288 DND458757:DND524288 DWZ458757:DWZ524288 EGV458757:EGV524288 EQR458757:EQR524288 FAN458757:FAN524288 FKJ458757:FKJ524288 FUF458757:FUF524288 GEB458757:GEB524288 GNX458757:GNX524288 GXT458757:GXT524288 HHP458757:HHP524288 HRL458757:HRL524288 IBH458757:IBH524288 ILD458757:ILD524288 IUZ458757:IUZ524288 JEV458757:JEV524288 JOR458757:JOR524288 JYN458757:JYN524288 KIJ458757:KIJ524288 KSF458757:KSF524288 LCB458757:LCB524288 LLX458757:LLX524288 LVT458757:LVT524288 MFP458757:MFP524288 MPL458757:MPL524288 MZH458757:MZH524288 NJD458757:NJD524288 NSZ458757:NSZ524288 OCV458757:OCV524288 OMR458757:OMR524288 OWN458757:OWN524288 PGJ458757:PGJ524288 PQF458757:PQF524288 QAB458757:QAB524288 QJX458757:QJX524288 QTT458757:QTT524288 RDP458757:RDP524288 RNL458757:RNL524288 RXH458757:RXH524288 SHD458757:SHD524288 SQZ458757:SQZ524288 TAV458757:TAV524288 TKR458757:TKR524288 TUN458757:TUN524288 UEJ458757:UEJ524288 UOF458757:UOF524288 UYB458757:UYB524288 VHX458757:VHX524288 VRT458757:VRT524288 WBP458757:WBP524288 WLL458757:WLL524288 WVH458757:WVH524288 IV524293:IV589824 SR524293:SR589824 ACN524293:ACN589824 AMJ524293:AMJ589824 AWF524293:AWF589824 BGB524293:BGB589824 BPX524293:BPX589824 BZT524293:BZT589824 CJP524293:CJP589824 CTL524293:CTL589824 DDH524293:DDH589824 DND524293:DND589824 DWZ524293:DWZ589824 EGV524293:EGV589824 EQR524293:EQR589824 FAN524293:FAN589824 FKJ524293:FKJ589824 FUF524293:FUF589824 GEB524293:GEB589824 GNX524293:GNX589824 GXT524293:GXT589824 HHP524293:HHP589824 HRL524293:HRL589824 IBH524293:IBH589824 ILD524293:ILD589824 IUZ524293:IUZ589824 JEV524293:JEV589824 JOR524293:JOR589824 JYN524293:JYN589824 KIJ524293:KIJ589824 KSF524293:KSF589824 LCB524293:LCB589824 LLX524293:LLX589824 LVT524293:LVT589824 MFP524293:MFP589824 MPL524293:MPL589824 MZH524293:MZH589824 NJD524293:NJD589824 NSZ524293:NSZ589824 OCV524293:OCV589824 OMR524293:OMR589824 OWN524293:OWN589824 PGJ524293:PGJ589824 PQF524293:PQF589824 QAB524293:QAB589824 QJX524293:QJX589824 QTT524293:QTT589824 RDP524293:RDP589824 RNL524293:RNL589824 RXH524293:RXH589824 SHD524293:SHD589824 SQZ524293:SQZ589824 TAV524293:TAV589824 TKR524293:TKR589824 TUN524293:TUN589824 UEJ524293:UEJ589824 UOF524293:UOF589824 UYB524293:UYB589824 VHX524293:VHX589824 VRT524293:VRT589824 WBP524293:WBP589824 WLL524293:WLL589824 WVH524293:WVH589824 IV589829:IV655360 SR589829:SR655360 ACN589829:ACN655360 AMJ589829:AMJ655360 AWF589829:AWF655360 BGB589829:BGB655360 BPX589829:BPX655360 BZT589829:BZT655360 CJP589829:CJP655360 CTL589829:CTL655360 DDH589829:DDH655360 DND589829:DND655360 DWZ589829:DWZ655360 EGV589829:EGV655360 EQR589829:EQR655360 FAN589829:FAN655360 FKJ589829:FKJ655360 FUF589829:FUF655360 GEB589829:GEB655360 GNX589829:GNX655360 GXT589829:GXT655360 HHP589829:HHP655360 HRL589829:HRL655360 IBH589829:IBH655360 ILD589829:ILD655360 IUZ589829:IUZ655360 JEV589829:JEV655360 JOR589829:JOR655360 JYN589829:JYN655360 KIJ589829:KIJ655360 KSF589829:KSF655360 LCB589829:LCB655360 LLX589829:LLX655360 LVT589829:LVT655360 MFP589829:MFP655360 MPL589829:MPL655360 MZH589829:MZH655360 NJD589829:NJD655360 NSZ589829:NSZ655360 OCV589829:OCV655360 OMR589829:OMR655360 OWN589829:OWN655360 PGJ589829:PGJ655360 PQF589829:PQF655360 QAB589829:QAB655360 QJX589829:QJX655360 QTT589829:QTT655360 RDP589829:RDP655360 RNL589829:RNL655360 RXH589829:RXH655360 SHD589829:SHD655360 SQZ589829:SQZ655360 TAV589829:TAV655360 TKR589829:TKR655360 TUN589829:TUN655360 UEJ589829:UEJ655360 UOF589829:UOF655360 UYB589829:UYB655360 VHX589829:VHX655360 VRT589829:VRT655360 WBP589829:WBP655360 WLL589829:WLL655360 WVH589829:WVH655360 IV655365:IV720896 SR655365:SR720896 ACN655365:ACN720896 AMJ655365:AMJ720896 AWF655365:AWF720896 BGB655365:BGB720896 BPX655365:BPX720896 BZT655365:BZT720896 CJP655365:CJP720896 CTL655365:CTL720896 DDH655365:DDH720896 DND655365:DND720896 DWZ655365:DWZ720896 EGV655365:EGV720896 EQR655365:EQR720896 FAN655365:FAN720896 FKJ655365:FKJ720896 FUF655365:FUF720896 GEB655365:GEB720896 GNX655365:GNX720896 GXT655365:GXT720896 HHP655365:HHP720896 HRL655365:HRL720896 IBH655365:IBH720896 ILD655365:ILD720896 IUZ655365:IUZ720896 JEV655365:JEV720896 JOR655365:JOR720896 JYN655365:JYN720896 KIJ655365:KIJ720896 KSF655365:KSF720896 LCB655365:LCB720896 LLX655365:LLX720896 LVT655365:LVT720896 MFP655365:MFP720896 MPL655365:MPL720896 MZH655365:MZH720896 NJD655365:NJD720896 NSZ655365:NSZ720896 OCV655365:OCV720896 OMR655365:OMR720896 OWN655365:OWN720896 PGJ655365:PGJ720896 PQF655365:PQF720896 QAB655365:QAB720896 QJX655365:QJX720896 QTT655365:QTT720896 RDP655365:RDP720896 RNL655365:RNL720896 RXH655365:RXH720896 SHD655365:SHD720896 SQZ655365:SQZ720896 TAV655365:TAV720896 TKR655365:TKR720896 TUN655365:TUN720896 UEJ655365:UEJ720896 UOF655365:UOF720896 UYB655365:UYB720896 VHX655365:VHX720896 VRT655365:VRT720896 WBP655365:WBP720896 WLL655365:WLL720896 WVH655365:WVH720896 IV720901:IV786432 SR720901:SR786432 ACN720901:ACN786432 AMJ720901:AMJ786432 AWF720901:AWF786432 BGB720901:BGB786432 BPX720901:BPX786432 BZT720901:BZT786432 CJP720901:CJP786432 CTL720901:CTL786432 DDH720901:DDH786432 DND720901:DND786432 DWZ720901:DWZ786432 EGV720901:EGV786432 EQR720901:EQR786432 FAN720901:FAN786432 FKJ720901:FKJ786432 FUF720901:FUF786432 GEB720901:GEB786432 GNX720901:GNX786432 GXT720901:GXT786432 HHP720901:HHP786432 HRL720901:HRL786432 IBH720901:IBH786432 ILD720901:ILD786432 IUZ720901:IUZ786432 JEV720901:JEV786432 JOR720901:JOR786432 JYN720901:JYN786432 KIJ720901:KIJ786432 KSF720901:KSF786432 LCB720901:LCB786432 LLX720901:LLX786432 LVT720901:LVT786432 MFP720901:MFP786432 MPL720901:MPL786432 MZH720901:MZH786432 NJD720901:NJD786432 NSZ720901:NSZ786432 OCV720901:OCV786432 OMR720901:OMR786432 OWN720901:OWN786432 PGJ720901:PGJ786432 PQF720901:PQF786432 QAB720901:QAB786432 QJX720901:QJX786432 QTT720901:QTT786432 RDP720901:RDP786432 RNL720901:RNL786432 RXH720901:RXH786432 SHD720901:SHD786432 SQZ720901:SQZ786432 TAV720901:TAV786432 TKR720901:TKR786432 TUN720901:TUN786432 UEJ720901:UEJ786432 UOF720901:UOF786432 UYB720901:UYB786432 VHX720901:VHX786432 VRT720901:VRT786432 WBP720901:WBP786432 WLL720901:WLL786432 WVH720901:WVH786432 IV786437:IV851968 SR786437:SR851968 ACN786437:ACN851968 AMJ786437:AMJ851968 AWF786437:AWF851968 BGB786437:BGB851968 BPX786437:BPX851968 BZT786437:BZT851968 CJP786437:CJP851968 CTL786437:CTL851968 DDH786437:DDH851968 DND786437:DND851968 DWZ786437:DWZ851968 EGV786437:EGV851968 EQR786437:EQR851968 FAN786437:FAN851968 FKJ786437:FKJ851968 FUF786437:FUF851968 GEB786437:GEB851968 GNX786437:GNX851968 GXT786437:GXT851968 HHP786437:HHP851968 HRL786437:HRL851968 IBH786437:IBH851968 ILD786437:ILD851968 IUZ786437:IUZ851968 JEV786437:JEV851968 JOR786437:JOR851968 JYN786437:JYN851968 KIJ786437:KIJ851968 KSF786437:KSF851968 LCB786437:LCB851968 LLX786437:LLX851968 LVT786437:LVT851968 MFP786437:MFP851968 MPL786437:MPL851968 MZH786437:MZH851968 NJD786437:NJD851968 NSZ786437:NSZ851968 OCV786437:OCV851968 OMR786437:OMR851968 OWN786437:OWN851968 PGJ786437:PGJ851968 PQF786437:PQF851968 QAB786437:QAB851968 QJX786437:QJX851968 QTT786437:QTT851968 RDP786437:RDP851968 RNL786437:RNL851968 RXH786437:RXH851968 SHD786437:SHD851968 SQZ786437:SQZ851968 TAV786437:TAV851968 TKR786437:TKR851968 TUN786437:TUN851968 UEJ786437:UEJ851968 UOF786437:UOF851968 UYB786437:UYB851968 VHX786437:VHX851968 VRT786437:VRT851968 WBP786437:WBP851968 WLL786437:WLL851968 WVH786437:WVH851968 IV851973:IV917504 SR851973:SR917504 ACN851973:ACN917504 AMJ851973:AMJ917504 AWF851973:AWF917504 BGB851973:BGB917504 BPX851973:BPX917504 BZT851973:BZT917504 CJP851973:CJP917504 CTL851973:CTL917504 DDH851973:DDH917504 DND851973:DND917504 DWZ851973:DWZ917504 EGV851973:EGV917504 EQR851973:EQR917504 FAN851973:FAN917504 FKJ851973:FKJ917504 FUF851973:FUF917504 GEB851973:GEB917504 GNX851973:GNX917504 GXT851973:GXT917504 HHP851973:HHP917504 HRL851973:HRL917504 IBH851973:IBH917504 ILD851973:ILD917504 IUZ851973:IUZ917504 JEV851973:JEV917504 JOR851973:JOR917504 JYN851973:JYN917504 KIJ851973:KIJ917504 KSF851973:KSF917504 LCB851973:LCB917504 LLX851973:LLX917504 LVT851973:LVT917504 MFP851973:MFP917504 MPL851973:MPL917504 MZH851973:MZH917504 NJD851973:NJD917504 NSZ851973:NSZ917504 OCV851973:OCV917504 OMR851973:OMR917504 OWN851973:OWN917504 PGJ851973:PGJ917504 PQF851973:PQF917504 QAB851973:QAB917504 QJX851973:QJX917504 QTT851973:QTT917504 RDP851973:RDP917504 RNL851973:RNL917504 RXH851973:RXH917504 SHD851973:SHD917504 SQZ851973:SQZ917504 TAV851973:TAV917504 TKR851973:TKR917504 TUN851973:TUN917504 UEJ851973:UEJ917504 UOF851973:UOF917504 UYB851973:UYB917504 VHX851973:VHX917504 VRT851973:VRT917504 WBP851973:WBP917504 WLL851973:WLL917504 WVH851973:WVH917504 IV917509:IV983040 SR917509:SR983040 ACN917509:ACN983040 AMJ917509:AMJ983040 AWF917509:AWF983040 BGB917509:BGB983040 BPX917509:BPX983040 BZT917509:BZT983040 CJP917509:CJP983040 CTL917509:CTL983040 DDH917509:DDH983040 DND917509:DND983040 DWZ917509:DWZ983040 EGV917509:EGV983040 EQR917509:EQR983040 FAN917509:FAN983040 FKJ917509:FKJ983040 FUF917509:FUF983040 GEB917509:GEB983040 GNX917509:GNX983040 GXT917509:GXT983040 HHP917509:HHP983040 HRL917509:HRL983040 IBH917509:IBH983040 ILD917509:ILD983040 IUZ917509:IUZ983040 JEV917509:JEV983040 JOR917509:JOR983040 JYN917509:JYN983040 KIJ917509:KIJ983040 KSF917509:KSF983040 LCB917509:LCB983040 LLX917509:LLX983040 LVT917509:LVT983040 MFP917509:MFP983040 MPL917509:MPL983040 MZH917509:MZH983040 NJD917509:NJD983040 NSZ917509:NSZ983040 OCV917509:OCV983040 OMR917509:OMR983040 OWN917509:OWN983040 PGJ917509:PGJ983040 PQF917509:PQF983040 QAB917509:QAB983040 QJX917509:QJX983040 QTT917509:QTT983040 RDP917509:RDP983040 RNL917509:RNL983040 RXH917509:RXH983040 SHD917509:SHD983040 SQZ917509:SQZ983040 TAV917509:TAV983040 TKR917509:TKR983040 TUN917509:TUN983040 UEJ917509:UEJ983040 UOF917509:UOF983040 UYB917509:UYB983040 VHX917509:VHX983040 VRT917509:VRT983040 WBP917509:WBP983040 WLL917509:WLL983040 WVH917509:WVH983040 IV983045:IV1048576 SR983045:SR1048576 ACN983045:ACN1048576 AMJ983045:AMJ1048576 AWF983045:AWF1048576 BGB983045:BGB1048576 BPX983045:BPX1048576 BZT983045:BZT1048576 CJP983045:CJP1048576 CTL983045:CTL1048576 DDH983045:DDH1048576 DND983045:DND1048576 DWZ983045:DWZ1048576 EGV983045:EGV1048576 EQR983045:EQR1048576 FAN983045:FAN1048576 FKJ983045:FKJ1048576 FUF983045:FUF1048576 GEB983045:GEB1048576 GNX983045:GNX1048576 GXT983045:GXT1048576 HHP983045:HHP1048576 HRL983045:HRL1048576 IBH983045:IBH1048576 ILD983045:ILD1048576 IUZ983045:IUZ1048576 JEV983045:JEV1048576 JOR983045:JOR1048576 JYN983045:JYN1048576 KIJ983045:KIJ1048576 KSF983045:KSF1048576 LCB983045:LCB1048576 LLX983045:LLX1048576 LVT983045:LVT1048576 MFP983045:MFP1048576 MPL983045:MPL1048576 MZH983045:MZH1048576 NJD983045:NJD1048576 NSZ983045:NSZ1048576 OCV983045:OCV1048576 OMR983045:OMR1048576 OWN983045:OWN1048576 PGJ983045:PGJ1048576 PQF983045:PQF1048576 QAB983045:QAB1048576 QJX983045:QJX1048576 QTT983045:QTT1048576 RDP983045:RDP1048576 RNL983045:RNL1048576 RXH983045:RXH1048576 SHD983045:SHD1048576 SQZ983045:SQZ1048576 TAV983045:TAV1048576 TKR983045:TKR1048576 TUN983045:TUN1048576 UEJ983045:UEJ1048576 UOF983045:UOF1048576 UYB983045:UYB1048576 VHX983045:VHX1048576 VRT983045:VRT1048576 WBP983045:WBP1048576 WLL983045:WLL1048576 WVH983045:WVH1048576 IV5:IV65536">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C982992:C1048576 C917456:C982987 C851920:C917451 C786384:C851915 C720848:C786379 C655312:C720843 C589776:C655307 C524240:C589771 C458704:C524235 C393168:C458699 C327632:C393163 C262096:C327627 C196560:C262091 C131024:C196555 C65488:C131019 IV65488:IV131019 SR65488:SR131019 ACN65488:ACN131019 AMJ65488:AMJ131019 AWF65488:AWF131019 BGB65488:BGB131019 BPX65488:BPX131019 BZT65488:BZT131019 CJP65488:CJP131019 CTL65488:CTL131019 DDH65488:DDH131019 DND65488:DND131019 DWZ65488:DWZ131019 EGV65488:EGV131019 EQR65488:EQR131019 FAN65488:FAN131019 FKJ65488:FKJ131019 FUF65488:FUF131019 GEB65488:GEB131019 GNX65488:GNX131019 GXT65488:GXT131019 HHP65488:HHP131019 HRL65488:HRL131019 IBH65488:IBH131019 ILD65488:ILD131019 IUZ65488:IUZ131019 JEV65488:JEV131019 JOR65488:JOR131019 JYN65488:JYN131019 KIJ65488:KIJ131019 KSF65488:KSF131019 LCB65488:LCB131019 LLX65488:LLX131019 LVT65488:LVT131019 MFP65488:MFP131019 MPL65488:MPL131019 MZH65488:MZH131019 NJD65488:NJD131019 NSZ65488:NSZ131019 OCV65488:OCV131019 OMR65488:OMR131019 OWN65488:OWN131019 PGJ65488:PGJ131019 PQF65488:PQF131019 QAB65488:QAB131019 QJX65488:QJX131019 QTT65488:QTT131019 RDP65488:RDP131019 RNL65488:RNL131019 RXH65488:RXH131019 SHD65488:SHD131019 SQZ65488:SQZ131019 TAV65488:TAV131019 TKR65488:TKR131019 TUN65488:TUN131019 UEJ65488:UEJ131019 UOF65488:UOF131019 UYB65488:UYB131019 VHX65488:VHX131019 VRT65488:VRT131019 WBP65488:WBP131019 WLL65488:WLL131019 WVH65488:WVH131019 IV131024:IV196555 SR131024:SR196555 ACN131024:ACN196555 AMJ131024:AMJ196555 AWF131024:AWF196555 BGB131024:BGB196555 BPX131024:BPX196555 BZT131024:BZT196555 CJP131024:CJP196555 CTL131024:CTL196555 DDH131024:DDH196555 DND131024:DND196555 DWZ131024:DWZ196555 EGV131024:EGV196555 EQR131024:EQR196555 FAN131024:FAN196555 FKJ131024:FKJ196555 FUF131024:FUF196555 GEB131024:GEB196555 GNX131024:GNX196555 GXT131024:GXT196555 HHP131024:HHP196555 HRL131024:HRL196555 IBH131024:IBH196555 ILD131024:ILD196555 IUZ131024:IUZ196555 JEV131024:JEV196555 JOR131024:JOR196555 JYN131024:JYN196555 KIJ131024:KIJ196555 KSF131024:KSF196555 LCB131024:LCB196555 LLX131024:LLX196555 LVT131024:LVT196555 MFP131024:MFP196555 MPL131024:MPL196555 MZH131024:MZH196555 NJD131024:NJD196555 NSZ131024:NSZ196555 OCV131024:OCV196555 OMR131024:OMR196555 OWN131024:OWN196555 PGJ131024:PGJ196555 PQF131024:PQF196555 QAB131024:QAB196555 QJX131024:QJX196555 QTT131024:QTT196555 RDP131024:RDP196555 RNL131024:RNL196555 RXH131024:RXH196555 SHD131024:SHD196555 SQZ131024:SQZ196555 TAV131024:TAV196555 TKR131024:TKR196555 TUN131024:TUN196555 UEJ131024:UEJ196555 UOF131024:UOF196555 UYB131024:UYB196555 VHX131024:VHX196555 VRT131024:VRT196555 WBP131024:WBP196555 WLL131024:WLL196555 WVH131024:WVH196555 IV196560:IV262091 SR196560:SR262091 ACN196560:ACN262091 AMJ196560:AMJ262091 AWF196560:AWF262091 BGB196560:BGB262091 BPX196560:BPX262091 BZT196560:BZT262091 CJP196560:CJP262091 CTL196560:CTL262091 DDH196560:DDH262091 DND196560:DND262091 DWZ196560:DWZ262091 EGV196560:EGV262091 EQR196560:EQR262091 FAN196560:FAN262091 FKJ196560:FKJ262091 FUF196560:FUF262091 GEB196560:GEB262091 GNX196560:GNX262091 GXT196560:GXT262091 HHP196560:HHP262091 HRL196560:HRL262091 IBH196560:IBH262091 ILD196560:ILD262091 IUZ196560:IUZ262091 JEV196560:JEV262091 JOR196560:JOR262091 JYN196560:JYN262091 KIJ196560:KIJ262091 KSF196560:KSF262091 LCB196560:LCB262091 LLX196560:LLX262091 LVT196560:LVT262091 MFP196560:MFP262091 MPL196560:MPL262091 MZH196560:MZH262091 NJD196560:NJD262091 NSZ196560:NSZ262091 OCV196560:OCV262091 OMR196560:OMR262091 OWN196560:OWN262091 PGJ196560:PGJ262091 PQF196560:PQF262091 QAB196560:QAB262091 QJX196560:QJX262091 QTT196560:QTT262091 RDP196560:RDP262091 RNL196560:RNL262091 RXH196560:RXH262091 SHD196560:SHD262091 SQZ196560:SQZ262091 TAV196560:TAV262091 TKR196560:TKR262091 TUN196560:TUN262091 UEJ196560:UEJ262091 UOF196560:UOF262091 UYB196560:UYB262091 VHX196560:VHX262091 VRT196560:VRT262091 WBP196560:WBP262091 WLL196560:WLL262091 WVH196560:WVH262091 IV262096:IV327627 SR262096:SR327627 ACN262096:ACN327627 AMJ262096:AMJ327627 AWF262096:AWF327627 BGB262096:BGB327627 BPX262096:BPX327627 BZT262096:BZT327627 CJP262096:CJP327627 CTL262096:CTL327627 DDH262096:DDH327627 DND262096:DND327627 DWZ262096:DWZ327627 EGV262096:EGV327627 EQR262096:EQR327627 FAN262096:FAN327627 FKJ262096:FKJ327627 FUF262096:FUF327627 GEB262096:GEB327627 GNX262096:GNX327627 GXT262096:GXT327627 HHP262096:HHP327627 HRL262096:HRL327627 IBH262096:IBH327627 ILD262096:ILD327627 IUZ262096:IUZ327627 JEV262096:JEV327627 JOR262096:JOR327627 JYN262096:JYN327627 KIJ262096:KIJ327627 KSF262096:KSF327627 LCB262096:LCB327627 LLX262096:LLX327627 LVT262096:LVT327627 MFP262096:MFP327627 MPL262096:MPL327627 MZH262096:MZH327627 NJD262096:NJD327627 NSZ262096:NSZ327627 OCV262096:OCV327627 OMR262096:OMR327627 OWN262096:OWN327627 PGJ262096:PGJ327627 PQF262096:PQF327627 QAB262096:QAB327627 QJX262096:QJX327627 QTT262096:QTT327627 RDP262096:RDP327627 RNL262096:RNL327627 RXH262096:RXH327627 SHD262096:SHD327627 SQZ262096:SQZ327627 TAV262096:TAV327627 TKR262096:TKR327627 TUN262096:TUN327627 UEJ262096:UEJ327627 UOF262096:UOF327627 UYB262096:UYB327627 VHX262096:VHX327627 VRT262096:VRT327627 WBP262096:WBP327627 WLL262096:WLL327627 WVH262096:WVH327627 IV327632:IV393163 SR327632:SR393163 ACN327632:ACN393163 AMJ327632:AMJ393163 AWF327632:AWF393163 BGB327632:BGB393163 BPX327632:BPX393163 BZT327632:BZT393163 CJP327632:CJP393163 CTL327632:CTL393163 DDH327632:DDH393163 DND327632:DND393163 DWZ327632:DWZ393163 EGV327632:EGV393163 EQR327632:EQR393163 FAN327632:FAN393163 FKJ327632:FKJ393163 FUF327632:FUF393163 GEB327632:GEB393163 GNX327632:GNX393163 GXT327632:GXT393163 HHP327632:HHP393163 HRL327632:HRL393163 IBH327632:IBH393163 ILD327632:ILD393163 IUZ327632:IUZ393163 JEV327632:JEV393163 JOR327632:JOR393163 JYN327632:JYN393163 KIJ327632:KIJ393163 KSF327632:KSF393163 LCB327632:LCB393163 LLX327632:LLX393163 LVT327632:LVT393163 MFP327632:MFP393163 MPL327632:MPL393163 MZH327632:MZH393163 NJD327632:NJD393163 NSZ327632:NSZ393163 OCV327632:OCV393163 OMR327632:OMR393163 OWN327632:OWN393163 PGJ327632:PGJ393163 PQF327632:PQF393163 QAB327632:QAB393163 QJX327632:QJX393163 QTT327632:QTT393163 RDP327632:RDP393163 RNL327632:RNL393163 RXH327632:RXH393163 SHD327632:SHD393163 SQZ327632:SQZ393163 TAV327632:TAV393163 TKR327632:TKR393163 TUN327632:TUN393163 UEJ327632:UEJ393163 UOF327632:UOF393163 UYB327632:UYB393163 VHX327632:VHX393163 VRT327632:VRT393163 WBP327632:WBP393163 WLL327632:WLL393163 WVH327632:WVH393163 IV393168:IV458699 SR393168:SR458699 ACN393168:ACN458699 AMJ393168:AMJ458699 AWF393168:AWF458699 BGB393168:BGB458699 BPX393168:BPX458699 BZT393168:BZT458699 CJP393168:CJP458699 CTL393168:CTL458699 DDH393168:DDH458699 DND393168:DND458699 DWZ393168:DWZ458699 EGV393168:EGV458699 EQR393168:EQR458699 FAN393168:FAN458699 FKJ393168:FKJ458699 FUF393168:FUF458699 GEB393168:GEB458699 GNX393168:GNX458699 GXT393168:GXT458699 HHP393168:HHP458699 HRL393168:HRL458699 IBH393168:IBH458699 ILD393168:ILD458699 IUZ393168:IUZ458699 JEV393168:JEV458699 JOR393168:JOR458699 JYN393168:JYN458699 KIJ393168:KIJ458699 KSF393168:KSF458699 LCB393168:LCB458699 LLX393168:LLX458699 LVT393168:LVT458699 MFP393168:MFP458699 MPL393168:MPL458699 MZH393168:MZH458699 NJD393168:NJD458699 NSZ393168:NSZ458699 OCV393168:OCV458699 OMR393168:OMR458699 OWN393168:OWN458699 PGJ393168:PGJ458699 PQF393168:PQF458699 QAB393168:QAB458699 QJX393168:QJX458699 QTT393168:QTT458699 RDP393168:RDP458699 RNL393168:RNL458699 RXH393168:RXH458699 SHD393168:SHD458699 SQZ393168:SQZ458699 TAV393168:TAV458699 TKR393168:TKR458699 TUN393168:TUN458699 UEJ393168:UEJ458699 UOF393168:UOF458699 UYB393168:UYB458699 VHX393168:VHX458699 VRT393168:VRT458699 WBP393168:WBP458699 WLL393168:WLL458699 WVH393168:WVH458699 IV458704:IV524235 SR458704:SR524235 ACN458704:ACN524235 AMJ458704:AMJ524235 AWF458704:AWF524235 BGB458704:BGB524235 BPX458704:BPX524235 BZT458704:BZT524235 CJP458704:CJP524235 CTL458704:CTL524235 DDH458704:DDH524235 DND458704:DND524235 DWZ458704:DWZ524235 EGV458704:EGV524235 EQR458704:EQR524235 FAN458704:FAN524235 FKJ458704:FKJ524235 FUF458704:FUF524235 GEB458704:GEB524235 GNX458704:GNX524235 GXT458704:GXT524235 HHP458704:HHP524235 HRL458704:HRL524235 IBH458704:IBH524235 ILD458704:ILD524235 IUZ458704:IUZ524235 JEV458704:JEV524235 JOR458704:JOR524235 JYN458704:JYN524235 KIJ458704:KIJ524235 KSF458704:KSF524235 LCB458704:LCB524235 LLX458704:LLX524235 LVT458704:LVT524235 MFP458704:MFP524235 MPL458704:MPL524235 MZH458704:MZH524235 NJD458704:NJD524235 NSZ458704:NSZ524235 OCV458704:OCV524235 OMR458704:OMR524235 OWN458704:OWN524235 PGJ458704:PGJ524235 PQF458704:PQF524235 QAB458704:QAB524235 QJX458704:QJX524235 QTT458704:QTT524235 RDP458704:RDP524235 RNL458704:RNL524235 RXH458704:RXH524235 SHD458704:SHD524235 SQZ458704:SQZ524235 TAV458704:TAV524235 TKR458704:TKR524235 TUN458704:TUN524235 UEJ458704:UEJ524235 UOF458704:UOF524235 UYB458704:UYB524235 VHX458704:VHX524235 VRT458704:VRT524235 WBP458704:WBP524235 WLL458704:WLL524235 WVH458704:WVH524235 IV524240:IV589771 SR524240:SR589771 ACN524240:ACN589771 AMJ524240:AMJ589771 AWF524240:AWF589771 BGB524240:BGB589771 BPX524240:BPX589771 BZT524240:BZT589771 CJP524240:CJP589771 CTL524240:CTL589771 DDH524240:DDH589771 DND524240:DND589771 DWZ524240:DWZ589771 EGV524240:EGV589771 EQR524240:EQR589771 FAN524240:FAN589771 FKJ524240:FKJ589771 FUF524240:FUF589771 GEB524240:GEB589771 GNX524240:GNX589771 GXT524240:GXT589771 HHP524240:HHP589771 HRL524240:HRL589771 IBH524240:IBH589771 ILD524240:ILD589771 IUZ524240:IUZ589771 JEV524240:JEV589771 JOR524240:JOR589771 JYN524240:JYN589771 KIJ524240:KIJ589771 KSF524240:KSF589771 LCB524240:LCB589771 LLX524240:LLX589771 LVT524240:LVT589771 MFP524240:MFP589771 MPL524240:MPL589771 MZH524240:MZH589771 NJD524240:NJD589771 NSZ524240:NSZ589771 OCV524240:OCV589771 OMR524240:OMR589771 OWN524240:OWN589771 PGJ524240:PGJ589771 PQF524240:PQF589771 QAB524240:QAB589771 QJX524240:QJX589771 QTT524240:QTT589771 RDP524240:RDP589771 RNL524240:RNL589771 RXH524240:RXH589771 SHD524240:SHD589771 SQZ524240:SQZ589771 TAV524240:TAV589771 TKR524240:TKR589771 TUN524240:TUN589771 UEJ524240:UEJ589771 UOF524240:UOF589771 UYB524240:UYB589771 VHX524240:VHX589771 VRT524240:VRT589771 WBP524240:WBP589771 WLL524240:WLL589771 WVH524240:WVH589771 IV589776:IV655307 SR589776:SR655307 ACN589776:ACN655307 AMJ589776:AMJ655307 AWF589776:AWF655307 BGB589776:BGB655307 BPX589776:BPX655307 BZT589776:BZT655307 CJP589776:CJP655307 CTL589776:CTL655307 DDH589776:DDH655307 DND589776:DND655307 DWZ589776:DWZ655307 EGV589776:EGV655307 EQR589776:EQR655307 FAN589776:FAN655307 FKJ589776:FKJ655307 FUF589776:FUF655307 GEB589776:GEB655307 GNX589776:GNX655307 GXT589776:GXT655307 HHP589776:HHP655307 HRL589776:HRL655307 IBH589776:IBH655307 ILD589776:ILD655307 IUZ589776:IUZ655307 JEV589776:JEV655307 JOR589776:JOR655307 JYN589776:JYN655307 KIJ589776:KIJ655307 KSF589776:KSF655307 LCB589776:LCB655307 LLX589776:LLX655307 LVT589776:LVT655307 MFP589776:MFP655307 MPL589776:MPL655307 MZH589776:MZH655307 NJD589776:NJD655307 NSZ589776:NSZ655307 OCV589776:OCV655307 OMR589776:OMR655307 OWN589776:OWN655307 PGJ589776:PGJ655307 PQF589776:PQF655307 QAB589776:QAB655307 QJX589776:QJX655307 QTT589776:QTT655307 RDP589776:RDP655307 RNL589776:RNL655307 RXH589776:RXH655307 SHD589776:SHD655307 SQZ589776:SQZ655307 TAV589776:TAV655307 TKR589776:TKR655307 TUN589776:TUN655307 UEJ589776:UEJ655307 UOF589776:UOF655307 UYB589776:UYB655307 VHX589776:VHX655307 VRT589776:VRT655307 WBP589776:WBP655307 WLL589776:WLL655307 WVH589776:WVH655307 IV655312:IV720843 SR655312:SR720843 ACN655312:ACN720843 AMJ655312:AMJ720843 AWF655312:AWF720843 BGB655312:BGB720843 BPX655312:BPX720843 BZT655312:BZT720843 CJP655312:CJP720843 CTL655312:CTL720843 DDH655312:DDH720843 DND655312:DND720843 DWZ655312:DWZ720843 EGV655312:EGV720843 EQR655312:EQR720843 FAN655312:FAN720843 FKJ655312:FKJ720843 FUF655312:FUF720843 GEB655312:GEB720843 GNX655312:GNX720843 GXT655312:GXT720843 HHP655312:HHP720843 HRL655312:HRL720843 IBH655312:IBH720843 ILD655312:ILD720843 IUZ655312:IUZ720843 JEV655312:JEV720843 JOR655312:JOR720843 JYN655312:JYN720843 KIJ655312:KIJ720843 KSF655312:KSF720843 LCB655312:LCB720843 LLX655312:LLX720843 LVT655312:LVT720843 MFP655312:MFP720843 MPL655312:MPL720843 MZH655312:MZH720843 NJD655312:NJD720843 NSZ655312:NSZ720843 OCV655312:OCV720843 OMR655312:OMR720843 OWN655312:OWN720843 PGJ655312:PGJ720843 PQF655312:PQF720843 QAB655312:QAB720843 QJX655312:QJX720843 QTT655312:QTT720843 RDP655312:RDP720843 RNL655312:RNL720843 RXH655312:RXH720843 SHD655312:SHD720843 SQZ655312:SQZ720843 TAV655312:TAV720843 TKR655312:TKR720843 TUN655312:TUN720843 UEJ655312:UEJ720843 UOF655312:UOF720843 UYB655312:UYB720843 VHX655312:VHX720843 VRT655312:VRT720843 WBP655312:WBP720843 WLL655312:WLL720843 WVH655312:WVH720843 IV720848:IV786379 SR720848:SR786379 ACN720848:ACN786379 AMJ720848:AMJ786379 AWF720848:AWF786379 BGB720848:BGB786379 BPX720848:BPX786379 BZT720848:BZT786379 CJP720848:CJP786379 CTL720848:CTL786379 DDH720848:DDH786379 DND720848:DND786379 DWZ720848:DWZ786379 EGV720848:EGV786379 EQR720848:EQR786379 FAN720848:FAN786379 FKJ720848:FKJ786379 FUF720848:FUF786379 GEB720848:GEB786379 GNX720848:GNX786379 GXT720848:GXT786379 HHP720848:HHP786379 HRL720848:HRL786379 IBH720848:IBH786379 ILD720848:ILD786379 IUZ720848:IUZ786379 JEV720848:JEV786379 JOR720848:JOR786379 JYN720848:JYN786379 KIJ720848:KIJ786379 KSF720848:KSF786379 LCB720848:LCB786379 LLX720848:LLX786379 LVT720848:LVT786379 MFP720848:MFP786379 MPL720848:MPL786379 MZH720848:MZH786379 NJD720848:NJD786379 NSZ720848:NSZ786379 OCV720848:OCV786379 OMR720848:OMR786379 OWN720848:OWN786379 PGJ720848:PGJ786379 PQF720848:PQF786379 QAB720848:QAB786379 QJX720848:QJX786379 QTT720848:QTT786379 RDP720848:RDP786379 RNL720848:RNL786379 RXH720848:RXH786379 SHD720848:SHD786379 SQZ720848:SQZ786379 TAV720848:TAV786379 TKR720848:TKR786379 TUN720848:TUN786379 UEJ720848:UEJ786379 UOF720848:UOF786379 UYB720848:UYB786379 VHX720848:VHX786379 VRT720848:VRT786379 WBP720848:WBP786379 WLL720848:WLL786379 WVH720848:WVH786379 IV786384:IV851915 SR786384:SR851915 ACN786384:ACN851915 AMJ786384:AMJ851915 AWF786384:AWF851915 BGB786384:BGB851915 BPX786384:BPX851915 BZT786384:BZT851915 CJP786384:CJP851915 CTL786384:CTL851915 DDH786384:DDH851915 DND786384:DND851915 DWZ786384:DWZ851915 EGV786384:EGV851915 EQR786384:EQR851915 FAN786384:FAN851915 FKJ786384:FKJ851915 FUF786384:FUF851915 GEB786384:GEB851915 GNX786384:GNX851915 GXT786384:GXT851915 HHP786384:HHP851915 HRL786384:HRL851915 IBH786384:IBH851915 ILD786384:ILD851915 IUZ786384:IUZ851915 JEV786384:JEV851915 JOR786384:JOR851915 JYN786384:JYN851915 KIJ786384:KIJ851915 KSF786384:KSF851915 LCB786384:LCB851915 LLX786384:LLX851915 LVT786384:LVT851915 MFP786384:MFP851915 MPL786384:MPL851915 MZH786384:MZH851915 NJD786384:NJD851915 NSZ786384:NSZ851915 OCV786384:OCV851915 OMR786384:OMR851915 OWN786384:OWN851915 PGJ786384:PGJ851915 PQF786384:PQF851915 QAB786384:QAB851915 QJX786384:QJX851915 QTT786384:QTT851915 RDP786384:RDP851915 RNL786384:RNL851915 RXH786384:RXH851915 SHD786384:SHD851915 SQZ786384:SQZ851915 TAV786384:TAV851915 TKR786384:TKR851915 TUN786384:TUN851915 UEJ786384:UEJ851915 UOF786384:UOF851915 UYB786384:UYB851915 VHX786384:VHX851915 VRT786384:VRT851915 WBP786384:WBP851915 WLL786384:WLL851915 WVH786384:WVH851915 IV851920:IV917451 SR851920:SR917451 ACN851920:ACN917451 AMJ851920:AMJ917451 AWF851920:AWF917451 BGB851920:BGB917451 BPX851920:BPX917451 BZT851920:BZT917451 CJP851920:CJP917451 CTL851920:CTL917451 DDH851920:DDH917451 DND851920:DND917451 DWZ851920:DWZ917451 EGV851920:EGV917451 EQR851920:EQR917451 FAN851920:FAN917451 FKJ851920:FKJ917451 FUF851920:FUF917451 GEB851920:GEB917451 GNX851920:GNX917451 GXT851920:GXT917451 HHP851920:HHP917451 HRL851920:HRL917451 IBH851920:IBH917451 ILD851920:ILD917451 IUZ851920:IUZ917451 JEV851920:JEV917451 JOR851920:JOR917451 JYN851920:JYN917451 KIJ851920:KIJ917451 KSF851920:KSF917451 LCB851920:LCB917451 LLX851920:LLX917451 LVT851920:LVT917451 MFP851920:MFP917451 MPL851920:MPL917451 MZH851920:MZH917451 NJD851920:NJD917451 NSZ851920:NSZ917451 OCV851920:OCV917451 OMR851920:OMR917451 OWN851920:OWN917451 PGJ851920:PGJ917451 PQF851920:PQF917451 QAB851920:QAB917451 QJX851920:QJX917451 QTT851920:QTT917451 RDP851920:RDP917451 RNL851920:RNL917451 RXH851920:RXH917451 SHD851920:SHD917451 SQZ851920:SQZ917451 TAV851920:TAV917451 TKR851920:TKR917451 TUN851920:TUN917451 UEJ851920:UEJ917451 UOF851920:UOF917451 UYB851920:UYB917451 VHX851920:VHX917451 VRT851920:VRT917451 WBP851920:WBP917451 WLL851920:WLL917451 WVH851920:WVH917451 IV917456:IV982987 SR917456:SR982987 ACN917456:ACN982987 AMJ917456:AMJ982987 AWF917456:AWF982987 BGB917456:BGB982987 BPX917456:BPX982987 BZT917456:BZT982987 CJP917456:CJP982987 CTL917456:CTL982987 DDH917456:DDH982987 DND917456:DND982987 DWZ917456:DWZ982987 EGV917456:EGV982987 EQR917456:EQR982987 FAN917456:FAN982987 FKJ917456:FKJ982987 FUF917456:FUF982987 GEB917456:GEB982987 GNX917456:GNX982987 GXT917456:GXT982987 HHP917456:HHP982987 HRL917456:HRL982987 IBH917456:IBH982987 ILD917456:ILD982987 IUZ917456:IUZ982987 JEV917456:JEV982987 JOR917456:JOR982987 JYN917456:JYN982987 KIJ917456:KIJ982987 KSF917456:KSF982987 LCB917456:LCB982987 LLX917456:LLX982987 LVT917456:LVT982987 MFP917456:MFP982987 MPL917456:MPL982987 MZH917456:MZH982987 NJD917456:NJD982987 NSZ917456:NSZ982987 OCV917456:OCV982987 OMR917456:OMR982987 OWN917456:OWN982987 PGJ917456:PGJ982987 PQF917456:PQF982987 QAB917456:QAB982987 QJX917456:QJX982987 QTT917456:QTT982987 RDP917456:RDP982987 RNL917456:RNL982987 RXH917456:RXH982987 SHD917456:SHD982987 SQZ917456:SQZ982987 TAV917456:TAV982987 TKR917456:TKR982987 TUN917456:TUN982987 UEJ917456:UEJ982987 UOF917456:UOF982987 UYB917456:UYB982987 VHX917456:VHX982987 VRT917456:VRT982987 WBP917456:WBP982987 WLL917456:WLL982987 WVH917456:WVH982987 IV982992:IV1048576 SR982992:SR1048576 ACN982992:ACN1048576 AMJ982992:AMJ1048576 AWF982992:AWF1048576 BGB982992:BGB1048576 BPX982992:BPX1048576 BZT982992:BZT1048576 CJP982992:CJP1048576 CTL982992:CTL1048576 DDH982992:DDH1048576 DND982992:DND1048576 DWZ982992:DWZ1048576 EGV982992:EGV1048576 EQR982992:EQR1048576 FAN982992:FAN1048576 FKJ982992:FKJ1048576 FUF982992:FUF1048576 GEB982992:GEB1048576 GNX982992:GNX1048576 GXT982992:GXT1048576 HHP982992:HHP1048576 HRL982992:HRL1048576 IBH982992:IBH1048576 ILD982992:ILD1048576 IUZ982992:IUZ1048576 JEV982992:JEV1048576 JOR982992:JOR1048576 JYN982992:JYN1048576 KIJ982992:KIJ1048576 KSF982992:KSF1048576 LCB982992:LCB1048576 LLX982992:LLX1048576 LVT982992:LVT1048576 MFP982992:MFP1048576 MPL982992:MPL1048576 MZH982992:MZH1048576 NJD982992:NJD1048576 NSZ982992:NSZ1048576 OCV982992:OCV1048576 OMR982992:OMR1048576 OWN982992:OWN1048576 PGJ982992:PGJ1048576 PQF982992:PQF1048576 QAB982992:QAB1048576 QJX982992:QJX1048576 QTT982992:QTT1048576 RDP982992:RDP1048576 RNL982992:RNL1048576 RXH982992:RXH1048576 SHD982992:SHD1048576 SQZ982992:SQZ1048576 TAV982992:TAV1048576 TKR982992:TKR1048576 TUN982992:TUN1048576 UEJ982992:UEJ1048576 UOF982992:UOF1048576 UYB982992:UYB1048576 VHX982992:VHX1048576 VRT982992:VRT1048576 WBP982992:WBP1048576 WLL982992:WLL1048576 WVH982992:WVH1048576 C5:C7 C17:C65483 SR5:SR65483 ACN5:ACN65483 AMJ5:AMJ65483 AWF5:AWF65483 BGB5:BGB65483 BPX5:BPX65483 BZT5:BZT65483 CJP5:CJP65483 CTL5:CTL65483 DDH5:DDH65483 DND5:DND65483 DWZ5:DWZ65483 EGV5:EGV65483 EQR5:EQR65483 FAN5:FAN65483 FKJ5:FKJ65483 FUF5:FUF65483 GEB5:GEB65483 GNX5:GNX65483 GXT5:GXT65483 HHP5:HHP65483 HRL5:HRL65483 IBH5:IBH65483 ILD5:ILD65483 IUZ5:IUZ65483 JEV5:JEV65483 JOR5:JOR65483 JYN5:JYN65483 KIJ5:KIJ65483 KSF5:KSF65483 LCB5:LCB65483 LLX5:LLX65483 LVT5:LVT65483 MFP5:MFP65483 MPL5:MPL65483 MZH5:MZH65483 NJD5:NJD65483 NSZ5:NSZ65483 OCV5:OCV65483 OMR5:OMR65483 OWN5:OWN65483 PGJ5:PGJ65483 PQF5:PQF65483 QAB5:QAB65483 QJX5:QJX65483 QTT5:QTT65483 RDP5:RDP65483 RNL5:RNL65483 RXH5:RXH65483 SHD5:SHD65483 SQZ5:SQZ65483 TAV5:TAV65483 TKR5:TKR65483 TUN5:TUN65483 UEJ5:UEJ65483 UOF5:UOF65483 UYB5:UYB65483 VHX5:VHX65483 VRT5:VRT65483 WBP5:WBP65483 WLL5:WLL65483 WVH5:WVH65483 IV5:IV65483">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="list" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B14 IT5:IT65536 A917509:A983040 A851973:A917504 A786437:A851968 A720901:A786432 A655365:A720896 A589829:A655360 A524293:A589824 A458757:A524288 A393221:A458752 A327685:A393216 A262149:A327680 A196613:A262144 A131077:A196608 A65541:A131072 A983045:A1048576 SP5:SP65536 ACL5:ACL65536 AMH5:AMH65536 AWD5:AWD65536 BFZ5:BFZ65536 BPV5:BPV65536 BZR5:BZR65536 CJN5:CJN65536 CTJ5:CTJ65536 DDF5:DDF65536 DNB5:DNB65536 DWX5:DWX65536 EGT5:EGT65536 EQP5:EQP65536 FAL5:FAL65536 FKH5:FKH65536 FUD5:FUD65536 GDZ5:GDZ65536 GNV5:GNV65536 GXR5:GXR65536 HHN5:HHN65536 HRJ5:HRJ65536 IBF5:IBF65536 ILB5:ILB65536 IUX5:IUX65536 JET5:JET65536 JOP5:JOP65536 JYL5:JYL65536 KIH5:KIH65536 KSD5:KSD65536 LBZ5:LBZ65536 LLV5:LLV65536 LVR5:LVR65536 MFN5:MFN65536 MPJ5:MPJ65536 MZF5:MZF65536 NJB5:NJB65536 NSX5:NSX65536 OCT5:OCT65536 OMP5:OMP65536 OWL5:OWL65536 PGH5:PGH65536 PQD5:PQD65536 PZZ5:PZZ65536 QJV5:QJV65536 QTR5:QTR65536 RDN5:RDN65536 RNJ5:RNJ65536 RXF5:RXF65536 SHB5:SHB65536 SQX5:SQX65536 TAT5:TAT65536 TKP5:TKP65536 TUL5:TUL65536 UEH5:UEH65536 UOD5:UOD65536 UXZ5:UXZ65536 VHV5:VHV65536 VRR5:VRR65536 WBN5:WBN65536 WLJ5:WLJ65536 WVF5:WVF65536 IT65541:IT131072 SP65541:SP131072 ACL65541:ACL131072 AMH65541:AMH131072 AWD65541:AWD131072 BFZ65541:BFZ131072 BPV65541:BPV131072 BZR65541:BZR131072 CJN65541:CJN131072 CTJ65541:CTJ131072 DDF65541:DDF131072 DNB65541:DNB131072 DWX65541:DWX131072 EGT65541:EGT131072 EQP65541:EQP131072 FAL65541:FAL131072 FKH65541:FKH131072 FUD65541:FUD131072 GDZ65541:GDZ131072 GNV65541:GNV131072 GXR65541:GXR131072 HHN65541:HHN131072 HRJ65541:HRJ131072 IBF65541:IBF131072 ILB65541:ILB131072 IUX65541:IUX131072 JET65541:JET131072 JOP65541:JOP131072 JYL65541:JYL131072 KIH65541:KIH131072 KSD65541:KSD131072 LBZ65541:LBZ131072 LLV65541:LLV131072 LVR65541:LVR131072 MFN65541:MFN131072 MPJ65541:MPJ131072 MZF65541:MZF131072 NJB65541:NJB131072 NSX65541:NSX131072 OCT65541:OCT131072 OMP65541:OMP131072 OWL65541:OWL131072 PGH65541:PGH131072 PQD65541:PQD131072 PZZ65541:PZZ131072 QJV65541:QJV131072 QTR65541:QTR131072 RDN65541:RDN131072 RNJ65541:RNJ131072 RXF65541:RXF131072 SHB65541:SHB131072 SQX65541:SQX131072 TAT65541:TAT131072 TKP65541:TKP131072 TUL65541:TUL131072 UEH65541:UEH131072 UOD65541:UOD131072 UXZ65541:UXZ131072 VHV65541:VHV131072 VRR65541:VRR131072 WBN65541:WBN131072 WLJ65541:WLJ131072 WVF65541:WVF131072 IT131077:IT196608 SP131077:SP196608 ACL131077:ACL196608 AMH131077:AMH196608 AWD131077:AWD196608 BFZ131077:BFZ196608 BPV131077:BPV196608 BZR131077:BZR196608 CJN131077:CJN196608 CTJ131077:CTJ196608 DDF131077:DDF196608 DNB131077:DNB196608 DWX131077:DWX196608 EGT131077:EGT196608 EQP131077:EQP196608 FAL131077:FAL196608 FKH131077:FKH196608 FUD131077:FUD196608 GDZ131077:GDZ196608 GNV131077:GNV196608 GXR131077:GXR196608 HHN131077:HHN196608 HRJ131077:HRJ196608 IBF131077:IBF196608 ILB131077:ILB196608 IUX131077:IUX196608 JET131077:JET196608 JOP131077:JOP196608 JYL131077:JYL196608 KIH131077:KIH196608 KSD131077:KSD196608 LBZ131077:LBZ196608 LLV131077:LLV196608 LVR131077:LVR196608 MFN131077:MFN196608 MPJ131077:MPJ196608 MZF131077:MZF196608 NJB131077:NJB196608 NSX131077:NSX196608 OCT131077:OCT196608 OMP131077:OMP196608 OWL131077:OWL196608 PGH131077:PGH196608 PQD131077:PQD196608 PZZ131077:PZZ196608 QJV131077:QJV196608 QTR131077:QTR196608 RDN131077:RDN196608 RNJ131077:RNJ196608 RXF131077:RXF196608 SHB131077:SHB196608 SQX131077:SQX196608 TAT131077:TAT196608 TKP131077:TKP196608 TUL131077:TUL196608 UEH131077:UEH196608 UOD131077:UOD196608 UXZ131077:UXZ196608 VHV131077:VHV196608 VRR131077:VRR196608 WBN131077:WBN196608 WLJ131077:WLJ196608 WVF131077:WVF196608 IT196613:IT262144 SP196613:SP262144 ACL196613:ACL262144 AMH196613:AMH262144 AWD196613:AWD262144 BFZ196613:BFZ262144 BPV196613:BPV262144 BZR196613:BZR262144 CJN196613:CJN262144 CTJ196613:CTJ262144 DDF196613:DDF262144 DNB196613:DNB262144 DWX196613:DWX262144 EGT196613:EGT262144 EQP196613:EQP262144 FAL196613:FAL262144 FKH196613:FKH262144 FUD196613:FUD262144 GDZ196613:GDZ262144 GNV196613:GNV262144 GXR196613:GXR262144 HHN196613:HHN262144 HRJ196613:HRJ262144 IBF196613:IBF262144 ILB196613:ILB262144 IUX196613:IUX262144 JET196613:JET262144 JOP196613:JOP262144 JYL196613:JYL262144 KIH196613:KIH262144 KSD196613:KSD262144 LBZ196613:LBZ262144 LLV196613:LLV262144 LVR196613:LVR262144 MFN196613:MFN262144 MPJ196613:MPJ262144 MZF196613:MZF262144 NJB196613:NJB262144 NSX196613:NSX262144 OCT196613:OCT262144 OMP196613:OMP262144 OWL196613:OWL262144 PGH196613:PGH262144 PQD196613:PQD262144 PZZ196613:PZZ262144 QJV196613:QJV262144 QTR196613:QTR262144 RDN196613:RDN262144 RNJ196613:RNJ262144 RXF196613:RXF262144 SHB196613:SHB262144 SQX196613:SQX262144 TAT196613:TAT262144 TKP196613:TKP262144 TUL196613:TUL262144 UEH196613:UEH262144 UOD196613:UOD262144 UXZ196613:UXZ262144 VHV196613:VHV262144 VRR196613:VRR262144 WBN196613:WBN262144 WLJ196613:WLJ262144 WVF196613:WVF262144 IT262149:IT327680 SP262149:SP327680 ACL262149:ACL327680 AMH262149:AMH327680 AWD262149:AWD327680 BFZ262149:BFZ327680 BPV262149:BPV327680 BZR262149:BZR327680 CJN262149:CJN327680 CTJ262149:CTJ327680 DDF262149:DDF327680 DNB262149:DNB327680 DWX262149:DWX327680 EGT262149:EGT327680 EQP262149:EQP327680 FAL262149:FAL327680 FKH262149:FKH327680 FUD262149:FUD327680 GDZ262149:GDZ327680 GNV262149:GNV327680 GXR262149:GXR327680 HHN262149:HHN327680 HRJ262149:HRJ327680 IBF262149:IBF327680 ILB262149:ILB327680 IUX262149:IUX327680 JET262149:JET327680 JOP262149:JOP327680 JYL262149:JYL327680 KIH262149:KIH327680 KSD262149:KSD327680 LBZ262149:LBZ327680 LLV262149:LLV327680 LVR262149:LVR327680 MFN262149:MFN327680 MPJ262149:MPJ327680 MZF262149:MZF327680 NJB262149:NJB327680 NSX262149:NSX327680 OCT262149:OCT327680 OMP262149:OMP327680 OWL262149:OWL327680 PGH262149:PGH327680 PQD262149:PQD327680 PZZ262149:PZZ327680 QJV262149:QJV327680 QTR262149:QTR327680 RDN262149:RDN327680 RNJ262149:RNJ327680 RXF262149:RXF327680 SHB262149:SHB327680 SQX262149:SQX327680 TAT262149:TAT327680 TKP262149:TKP327680 TUL262149:TUL327680 UEH262149:UEH327680 UOD262149:UOD327680 UXZ262149:UXZ327680 VHV262149:VHV327680 VRR262149:VRR327680 WBN262149:WBN327680 WLJ262149:WLJ327680 WVF262149:WVF327680 IT327685:IT393216 SP327685:SP393216 ACL327685:ACL393216 AMH327685:AMH393216 AWD327685:AWD393216 BFZ327685:BFZ393216 BPV327685:BPV393216 BZR327685:BZR393216 CJN327685:CJN393216 CTJ327685:CTJ393216 DDF327685:DDF393216 DNB327685:DNB393216 DWX327685:DWX393216 EGT327685:EGT393216 EQP327685:EQP393216 FAL327685:FAL393216 FKH327685:FKH393216 FUD327685:FUD393216 GDZ327685:GDZ393216 GNV327685:GNV393216 GXR327685:GXR393216 HHN327685:HHN393216 HRJ327685:HRJ393216 IBF327685:IBF393216 ILB327685:ILB393216 IUX327685:IUX393216 JET327685:JET393216 JOP327685:JOP393216 JYL327685:JYL393216 KIH327685:KIH393216 KSD327685:KSD393216 LBZ327685:LBZ393216 LLV327685:LLV393216 LVR327685:LVR393216 MFN327685:MFN393216 MPJ327685:MPJ393216 MZF327685:MZF393216 NJB327685:NJB393216 NSX327685:NSX393216 OCT327685:OCT393216 OMP327685:OMP393216 OWL327685:OWL393216 PGH327685:PGH393216 PQD327685:PQD393216 PZZ327685:PZZ393216 QJV327685:QJV393216 QTR327685:QTR393216 RDN327685:RDN393216 RNJ327685:RNJ393216 RXF327685:RXF393216 SHB327685:SHB393216 SQX327685:SQX393216 TAT327685:TAT393216 TKP327685:TKP393216 TUL327685:TUL393216 UEH327685:UEH393216 UOD327685:UOD393216 UXZ327685:UXZ393216 VHV327685:VHV393216 VRR327685:VRR393216 WBN327685:WBN393216 WLJ327685:WLJ393216 WVF327685:WVF393216 IT393221:IT458752 SP393221:SP458752 ACL393221:ACL458752 AMH393221:AMH458752 AWD393221:AWD458752 BFZ393221:BFZ458752 BPV393221:BPV458752 BZR393221:BZR458752 CJN393221:CJN458752 CTJ393221:CTJ458752 DDF393221:DDF458752 DNB393221:DNB458752 DWX393221:DWX458752 EGT393221:EGT458752 EQP393221:EQP458752 FAL393221:FAL458752 FKH393221:FKH458752 FUD393221:FUD458752 GDZ393221:GDZ458752 GNV393221:GNV458752 GXR393221:GXR458752 HHN393221:HHN458752 HRJ393221:HRJ458752 IBF393221:IBF458752 ILB393221:ILB458752 IUX393221:IUX458752 JET393221:JET458752 JOP393221:JOP458752 JYL393221:JYL458752 KIH393221:KIH458752 KSD393221:KSD458752 LBZ393221:LBZ458752 LLV393221:LLV458752 LVR393221:LVR458752 MFN393221:MFN458752 MPJ393221:MPJ458752 MZF393221:MZF458752 NJB393221:NJB458752 NSX393221:NSX458752 OCT393221:OCT458752 OMP393221:OMP458752 OWL393221:OWL458752 PGH393221:PGH458752 PQD393221:PQD458752 PZZ393221:PZZ458752 QJV393221:QJV458752 QTR393221:QTR458752 RDN393221:RDN458752 RNJ393221:RNJ458752 RXF393221:RXF458752 SHB393221:SHB458752 SQX393221:SQX458752 TAT393221:TAT458752 TKP393221:TKP458752 TUL393221:TUL458752 UEH393221:UEH458752 UOD393221:UOD458752 UXZ393221:UXZ458752 VHV393221:VHV458752 VRR393221:VRR458752 WBN393221:WBN458752 WLJ393221:WLJ458752 WVF393221:WVF458752 IT458757:IT524288 SP458757:SP524288 ACL458757:ACL524288 AMH458757:AMH524288 AWD458757:AWD524288 BFZ458757:BFZ524288 BPV458757:BPV524288 BZR458757:BZR524288 CJN458757:CJN524288 CTJ458757:CTJ524288 DDF458757:DDF524288 DNB458757:DNB524288 DWX458757:DWX524288 EGT458757:EGT524288 EQP458757:EQP524288 FAL458757:FAL524288 FKH458757:FKH524288 FUD458757:FUD524288 GDZ458757:GDZ524288 GNV458757:GNV524288 GXR458757:GXR524288 HHN458757:HHN524288 HRJ458757:HRJ524288 IBF458757:IBF524288 ILB458757:ILB524288 IUX458757:IUX524288 JET458757:JET524288 JOP458757:JOP524288 JYL458757:JYL524288 KIH458757:KIH524288 KSD458757:KSD524288 LBZ458757:LBZ524288 LLV458757:LLV524288 LVR458757:LVR524288 MFN458757:MFN524288 MPJ458757:MPJ524288 MZF458757:MZF524288 NJB458757:NJB524288 NSX458757:NSX524288 OCT458757:OCT524288 OMP458757:OMP524288 OWL458757:OWL524288 PGH458757:PGH524288 PQD458757:PQD524288 PZZ458757:PZZ524288 QJV458757:QJV524288 QTR458757:QTR524288 RDN458757:RDN524288 RNJ458757:RNJ524288 RXF458757:RXF524288 SHB458757:SHB524288 SQX458757:SQX524288 TAT458757:TAT524288 TKP458757:TKP524288 TUL458757:TUL524288 UEH458757:UEH524288 UOD458757:UOD524288 UXZ458757:UXZ524288 VHV458757:VHV524288 VRR458757:VRR524288 WBN458757:WBN524288 WLJ458757:WLJ524288 WVF458757:WVF524288 IT524293:IT589824 SP524293:SP589824 ACL524293:ACL589824 AMH524293:AMH589824 AWD524293:AWD589824 BFZ524293:BFZ589824 BPV524293:BPV589824 BZR524293:BZR589824 CJN524293:CJN589824 CTJ524293:CTJ589824 DDF524293:DDF589824 DNB524293:DNB589824 DWX524293:DWX589824 EGT524293:EGT589824 EQP524293:EQP589824 FAL524293:FAL589824 FKH524293:FKH589824 FUD524293:FUD589824 GDZ524293:GDZ589824 GNV524293:GNV589824 GXR524293:GXR589824 HHN524293:HHN589824 HRJ524293:HRJ589824 IBF524293:IBF589824 ILB524293:ILB589824 IUX524293:IUX589824 JET524293:JET589824 JOP524293:JOP589824 JYL524293:JYL589824 KIH524293:KIH589824 KSD524293:KSD589824 LBZ524293:LBZ589824 LLV524293:LLV589824 LVR524293:LVR589824 MFN524293:MFN589824 MPJ524293:MPJ589824 MZF524293:MZF589824 NJB524293:NJB589824 NSX524293:NSX589824 OCT524293:OCT589824 OMP524293:OMP589824 OWL524293:OWL589824 PGH524293:PGH589824 PQD524293:PQD589824 PZZ524293:PZZ589824 QJV524293:QJV589824 QTR524293:QTR589824 RDN524293:RDN589824 RNJ524293:RNJ589824 RXF524293:RXF589824 SHB524293:SHB589824 SQX524293:SQX589824 TAT524293:TAT589824 TKP524293:TKP589824 TUL524293:TUL589824 UEH524293:UEH589824 UOD524293:UOD589824 UXZ524293:UXZ589824 VHV524293:VHV589824 VRR524293:VRR589824 WBN524293:WBN589824 WLJ524293:WLJ589824 WVF524293:WVF589824 IT589829:IT655360 SP589829:SP655360 ACL589829:ACL655360 AMH589829:AMH655360 AWD589829:AWD655360 BFZ589829:BFZ655360 BPV589829:BPV655360 BZR589829:BZR655360 CJN589829:CJN655360 CTJ589829:CTJ655360 DDF589829:DDF655360 DNB589829:DNB655360 DWX589829:DWX655360 EGT589829:EGT655360 EQP589829:EQP655360 FAL589829:FAL655360 FKH589829:FKH655360 FUD589829:FUD655360 GDZ589829:GDZ655360 GNV589829:GNV655360 GXR589829:GXR655360 HHN589829:HHN655360 HRJ589829:HRJ655360 IBF589829:IBF655360 ILB589829:ILB655360 IUX589829:IUX655360 JET589829:JET655360 JOP589829:JOP655360 JYL589829:JYL655360 KIH589829:KIH655360 KSD589829:KSD655360 LBZ589829:LBZ655360 LLV589829:LLV655360 LVR589829:LVR655360 MFN589829:MFN655360 MPJ589829:MPJ655360 MZF589829:MZF655360 NJB589829:NJB655360 NSX589829:NSX655360 OCT589829:OCT655360 OMP589829:OMP655360 OWL589829:OWL655360 PGH589829:PGH655360 PQD589829:PQD655360 PZZ589829:PZZ655360 QJV589829:QJV655360 QTR589829:QTR655360 RDN589829:RDN655360 RNJ589829:RNJ655360 RXF589829:RXF655360 SHB589829:SHB655360 SQX589829:SQX655360 TAT589829:TAT655360 TKP589829:TKP655360 TUL589829:TUL655360 UEH589829:UEH655360 UOD589829:UOD655360 UXZ589829:UXZ655360 VHV589829:VHV655360 VRR589829:VRR655360 WBN589829:WBN655360 WLJ589829:WLJ655360 WVF589829:WVF655360 IT655365:IT720896 SP655365:SP720896 ACL655365:ACL720896 AMH655365:AMH720896 AWD655365:AWD720896 BFZ655365:BFZ720896 BPV655365:BPV720896 BZR655365:BZR720896 CJN655365:CJN720896 CTJ655365:CTJ720896 DDF655365:DDF720896 DNB655365:DNB720896 DWX655365:DWX720896 EGT655365:EGT720896 EQP655365:EQP720896 FAL655365:FAL720896 FKH655365:FKH720896 FUD655365:FUD720896 GDZ655365:GDZ720896 GNV655365:GNV720896 GXR655365:GXR720896 HHN655365:HHN720896 HRJ655365:HRJ720896 IBF655365:IBF720896 ILB655365:ILB720896 IUX655365:IUX720896 JET655365:JET720896 JOP655365:JOP720896 JYL655365:JYL720896 KIH655365:KIH720896 KSD655365:KSD720896 LBZ655365:LBZ720896 LLV655365:LLV720896 LVR655365:LVR720896 MFN655365:MFN720896 MPJ655365:MPJ720896 MZF655365:MZF720896 NJB655365:NJB720896 NSX655365:NSX720896 OCT655365:OCT720896 OMP655365:OMP720896 OWL655365:OWL720896 PGH655365:PGH720896 PQD655365:PQD720896 PZZ655365:PZZ720896 QJV655365:QJV720896 QTR655365:QTR720896 RDN655365:RDN720896 RNJ655365:RNJ720896 RXF655365:RXF720896 SHB655365:SHB720896 SQX655365:SQX720896 TAT655365:TAT720896 TKP655365:TKP720896 TUL655365:TUL720896 UEH655365:UEH720896 UOD655365:UOD720896 UXZ655365:UXZ720896 VHV655365:VHV720896 VRR655365:VRR720896 WBN655365:WBN720896 WLJ655365:WLJ720896 WVF655365:WVF720896 IT720901:IT786432 SP720901:SP786432 ACL720901:ACL786432 AMH720901:AMH786432 AWD720901:AWD786432 BFZ720901:BFZ786432 BPV720901:BPV786432 BZR720901:BZR786432 CJN720901:CJN786432 CTJ720901:CTJ786432 DDF720901:DDF786432 DNB720901:DNB786432 DWX720901:DWX786432 EGT720901:EGT786432 EQP720901:EQP786432 FAL720901:FAL786432 FKH720901:FKH786432 FUD720901:FUD786432 GDZ720901:GDZ786432 GNV720901:GNV786432 GXR720901:GXR786432 HHN720901:HHN786432 HRJ720901:HRJ786432 IBF720901:IBF786432 ILB720901:ILB786432 IUX720901:IUX786432 JET720901:JET786432 JOP720901:JOP786432 JYL720901:JYL786432 KIH720901:KIH786432 KSD720901:KSD786432 LBZ720901:LBZ786432 LLV720901:LLV786432 LVR720901:LVR786432 MFN720901:MFN786432 MPJ720901:MPJ786432 MZF720901:MZF786432 NJB720901:NJB786432 NSX720901:NSX786432 OCT720901:OCT786432 OMP720901:OMP786432 OWL720901:OWL786432 PGH720901:PGH786432 PQD720901:PQD786432 PZZ720901:PZZ786432 QJV720901:QJV786432 QTR720901:QTR786432 RDN720901:RDN786432 RNJ720901:RNJ786432 RXF720901:RXF786432 SHB720901:SHB786432 SQX720901:SQX786432 TAT720901:TAT786432 TKP720901:TKP786432 TUL720901:TUL786432 UEH720901:UEH786432 UOD720901:UOD786432 UXZ720901:UXZ786432 VHV720901:VHV786432 VRR720901:VRR786432 WBN720901:WBN786432 WLJ720901:WLJ786432 WVF720901:WVF786432 IT786437:IT851968 SP786437:SP851968 ACL786437:ACL851968 AMH786437:AMH851968 AWD786437:AWD851968 BFZ786437:BFZ851968 BPV786437:BPV851968 BZR786437:BZR851968 CJN786437:CJN851968 CTJ786437:CTJ851968 DDF786437:DDF851968 DNB786437:DNB851968 DWX786437:DWX851968 EGT786437:EGT851968 EQP786437:EQP851968 FAL786437:FAL851968 FKH786437:FKH851968 FUD786437:FUD851968 GDZ786437:GDZ851968 GNV786437:GNV851968 GXR786437:GXR851968 HHN786437:HHN851968 HRJ786437:HRJ851968 IBF786437:IBF851968 ILB786437:ILB851968 IUX786437:IUX851968 JET786437:JET851968 JOP786437:JOP851968 JYL786437:JYL851968 KIH786437:KIH851968 KSD786437:KSD851968 LBZ786437:LBZ851968 LLV786437:LLV851968 LVR786437:LVR851968 MFN786437:MFN851968 MPJ786437:MPJ851968 MZF786437:MZF851968 NJB786437:NJB851968 NSX786437:NSX851968 OCT786437:OCT851968 OMP786437:OMP851968 OWL786437:OWL851968 PGH786437:PGH851968 PQD786437:PQD851968 PZZ786437:PZZ851968 QJV786437:QJV851968 QTR786437:QTR851968 RDN786437:RDN851968 RNJ786437:RNJ851968 RXF786437:RXF851968 SHB786437:SHB851968 SQX786437:SQX851968 TAT786437:TAT851968 TKP786437:TKP851968 TUL786437:TUL851968 UEH786437:UEH851968 UOD786437:UOD851968 UXZ786437:UXZ851968 VHV786437:VHV851968 VRR786437:VRR851968 WBN786437:WBN851968 WLJ786437:WLJ851968 WVF786437:WVF851968 IT851973:IT917504 SP851973:SP917504 ACL851973:ACL917504 AMH851973:AMH917504 AWD851973:AWD917504 BFZ851973:BFZ917504 BPV851973:BPV917504 BZR851973:BZR917504 CJN851973:CJN917504 CTJ851973:CTJ917504 DDF851973:DDF917504 DNB851973:DNB917504 DWX851973:DWX917504 EGT851973:EGT917504 EQP851973:EQP917504 FAL851973:FAL917504 FKH851973:FKH917504 FUD851973:FUD917504 GDZ851973:GDZ917504 GNV851973:GNV917504 GXR851973:GXR917504 HHN851973:HHN917504 HRJ851973:HRJ917504 IBF851973:IBF917504 ILB851973:ILB917504 IUX851973:IUX917504 JET851973:JET917504 JOP851973:JOP917504 JYL851973:JYL917504 KIH851973:KIH917504 KSD851973:KSD917504 LBZ851973:LBZ917504 LLV851973:LLV917504 LVR851973:LVR917504 MFN851973:MFN917504 MPJ851973:MPJ917504 MZF851973:MZF917504 NJB851973:NJB917504 NSX851973:NSX917504 OCT851973:OCT917504 OMP851973:OMP917504 OWL851973:OWL917504 PGH851973:PGH917504 PQD851973:PQD917504 PZZ851973:PZZ917504 QJV851973:QJV917504 QTR851973:QTR917504 RDN851973:RDN917504 RNJ851973:RNJ917504 RXF851973:RXF917504 SHB851973:SHB917504 SQX851973:SQX917504 TAT851973:TAT917504 TKP851973:TKP917504 TUL851973:TUL917504 UEH851973:UEH917504 UOD851973:UOD917504 UXZ851973:UXZ917504 VHV851973:VHV917504 VRR851973:VRR917504 WBN851973:WBN917504 WLJ851973:WLJ917504 WVF851973:WVF917504 IT917509:IT983040 SP917509:SP983040 ACL917509:ACL983040 AMH917509:AMH983040 AWD917509:AWD983040 BFZ917509:BFZ983040 BPV917509:BPV983040 BZR917509:BZR983040 CJN917509:CJN983040 CTJ917509:CTJ983040 DDF917509:DDF983040 DNB917509:DNB983040 DWX917509:DWX983040 EGT917509:EGT983040 EQP917509:EQP983040 FAL917509:FAL983040 FKH917509:FKH983040 FUD917509:FUD983040 GDZ917509:GDZ983040 GNV917509:GNV983040 GXR917509:GXR983040 HHN917509:HHN983040 HRJ917509:HRJ983040 IBF917509:IBF983040 ILB917509:ILB983040 IUX917509:IUX983040 JET917509:JET983040 JOP917509:JOP983040 JYL917509:JYL983040 KIH917509:KIH983040 KSD917509:KSD983040 LBZ917509:LBZ983040 LLV917509:LLV983040 LVR917509:LVR983040 MFN917509:MFN983040 MPJ917509:MPJ983040 MZF917509:MZF983040 NJB917509:NJB983040 NSX917509:NSX983040 OCT917509:OCT983040 OMP917509:OMP983040 OWL917509:OWL983040 PGH917509:PGH983040 PQD917509:PQD983040 PZZ917509:PZZ983040 QJV917509:QJV983040 QTR917509:QTR983040 RDN917509:RDN983040 RNJ917509:RNJ983040 RXF917509:RXF983040 SHB917509:SHB983040 SQX917509:SQX983040 TAT917509:TAT983040 TKP917509:TKP983040 TUL917509:TUL983040 UEH917509:UEH983040 UOD917509:UOD983040 UXZ917509:UXZ983040 VHV917509:VHV983040 VRR917509:VRR983040 WBN917509:WBN983040 WLJ917509:WLJ983040 WVF917509:WVF983040 IT983045:IT1048576 SP983045:SP1048576 ACL983045:ACL1048576 AMH983045:AMH1048576 AWD983045:AWD1048576 BFZ983045:BFZ1048576 BPV983045:BPV1048576 BZR983045:BZR1048576 CJN983045:CJN1048576 CTJ983045:CTJ1048576 DDF983045:DDF1048576 DNB983045:DNB1048576 DWX983045:DWX1048576 EGT983045:EGT1048576 EQP983045:EQP1048576 FAL983045:FAL1048576 FKH983045:FKH1048576 FUD983045:FUD1048576 GDZ983045:GDZ1048576 GNV983045:GNV1048576 GXR983045:GXR1048576 HHN983045:HHN1048576 HRJ983045:HRJ1048576 IBF983045:IBF1048576 ILB983045:ILB1048576 IUX983045:IUX1048576 JET983045:JET1048576 JOP983045:JOP1048576 JYL983045:JYL1048576 KIH983045:KIH1048576 KSD983045:KSD1048576 LBZ983045:LBZ1048576 LLV983045:LLV1048576 LVR983045:LVR1048576 MFN983045:MFN1048576 MPJ983045:MPJ1048576 MZF983045:MZF1048576 NJB983045:NJB1048576 NSX983045:NSX1048576 OCT983045:OCT1048576 OMP983045:OMP1048576 OWL983045:OWL1048576 PGH983045:PGH1048576 PQD983045:PQD1048576 PZZ983045:PZZ1048576 QJV983045:QJV1048576 QTR983045:QTR1048576 RDN983045:RDN1048576 RNJ983045:RNJ1048576 RXF983045:RXF1048576 SHB983045:SHB1048576 SQX983045:SQX1048576 TAT983045:TAT1048576 TKP983045:TKP1048576 TUL983045:TUL1048576 UEH983045:UEH1048576 UOD983045:UOD1048576 UXZ983045:UXZ1048576 VHV983045:VHV1048576 VRR983045:VRR1048576 WBN983045:WBN1048576 WLJ983045:WLJ1048576 WVF983045:WVF1048576 A5:A65536">
+    <dataValidation type="list" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVF982992:WVF1048576 A917456:A982987 A851920:A917451 A786384:A851915 A720848:A786379 A655312:A720843 A589776:A655307 A524240:A589771 A458704:A524235 A393168:A458699 A327632:A393163 A262096:A327627 A196560:A262091 A131024:A196555 A65488:A131019 A982992:A1048576 IT65488:IT131019 SP65488:SP131019 ACL65488:ACL131019 AMH65488:AMH131019 AWD65488:AWD131019 BFZ65488:BFZ131019 BPV65488:BPV131019 BZR65488:BZR131019 CJN65488:CJN131019 CTJ65488:CTJ131019 DDF65488:DDF131019 DNB65488:DNB131019 DWX65488:DWX131019 EGT65488:EGT131019 EQP65488:EQP131019 FAL65488:FAL131019 FKH65488:FKH131019 FUD65488:FUD131019 GDZ65488:GDZ131019 GNV65488:GNV131019 GXR65488:GXR131019 HHN65488:HHN131019 HRJ65488:HRJ131019 IBF65488:IBF131019 ILB65488:ILB131019 IUX65488:IUX131019 JET65488:JET131019 JOP65488:JOP131019 JYL65488:JYL131019 KIH65488:KIH131019 KSD65488:KSD131019 LBZ65488:LBZ131019 LLV65488:LLV131019 LVR65488:LVR131019 MFN65488:MFN131019 MPJ65488:MPJ131019 MZF65488:MZF131019 NJB65488:NJB131019 NSX65488:NSX131019 OCT65488:OCT131019 OMP65488:OMP131019 OWL65488:OWL131019 PGH65488:PGH131019 PQD65488:PQD131019 PZZ65488:PZZ131019 QJV65488:QJV131019 QTR65488:QTR131019 RDN65488:RDN131019 RNJ65488:RNJ131019 RXF65488:RXF131019 SHB65488:SHB131019 SQX65488:SQX131019 TAT65488:TAT131019 TKP65488:TKP131019 TUL65488:TUL131019 UEH65488:UEH131019 UOD65488:UOD131019 UXZ65488:UXZ131019 VHV65488:VHV131019 VRR65488:VRR131019 WBN65488:WBN131019 WLJ65488:WLJ131019 WVF65488:WVF131019 IT131024:IT196555 SP131024:SP196555 ACL131024:ACL196555 AMH131024:AMH196555 AWD131024:AWD196555 BFZ131024:BFZ196555 BPV131024:BPV196555 BZR131024:BZR196555 CJN131024:CJN196555 CTJ131024:CTJ196555 DDF131024:DDF196555 DNB131024:DNB196555 DWX131024:DWX196555 EGT131024:EGT196555 EQP131024:EQP196555 FAL131024:FAL196555 FKH131024:FKH196555 FUD131024:FUD196555 GDZ131024:GDZ196555 GNV131024:GNV196555 GXR131024:GXR196555 HHN131024:HHN196555 HRJ131024:HRJ196555 IBF131024:IBF196555 ILB131024:ILB196555 IUX131024:IUX196555 JET131024:JET196555 JOP131024:JOP196555 JYL131024:JYL196555 KIH131024:KIH196555 KSD131024:KSD196555 LBZ131024:LBZ196555 LLV131024:LLV196555 LVR131024:LVR196555 MFN131024:MFN196555 MPJ131024:MPJ196555 MZF131024:MZF196555 NJB131024:NJB196555 NSX131024:NSX196555 OCT131024:OCT196555 OMP131024:OMP196555 OWL131024:OWL196555 PGH131024:PGH196555 PQD131024:PQD196555 PZZ131024:PZZ196555 QJV131024:QJV196555 QTR131024:QTR196555 RDN131024:RDN196555 RNJ131024:RNJ196555 RXF131024:RXF196555 SHB131024:SHB196555 SQX131024:SQX196555 TAT131024:TAT196555 TKP131024:TKP196555 TUL131024:TUL196555 UEH131024:UEH196555 UOD131024:UOD196555 UXZ131024:UXZ196555 VHV131024:VHV196555 VRR131024:VRR196555 WBN131024:WBN196555 WLJ131024:WLJ196555 WVF131024:WVF196555 IT196560:IT262091 SP196560:SP262091 ACL196560:ACL262091 AMH196560:AMH262091 AWD196560:AWD262091 BFZ196560:BFZ262091 BPV196560:BPV262091 BZR196560:BZR262091 CJN196560:CJN262091 CTJ196560:CTJ262091 DDF196560:DDF262091 DNB196560:DNB262091 DWX196560:DWX262091 EGT196560:EGT262091 EQP196560:EQP262091 FAL196560:FAL262091 FKH196560:FKH262091 FUD196560:FUD262091 GDZ196560:GDZ262091 GNV196560:GNV262091 GXR196560:GXR262091 HHN196560:HHN262091 HRJ196560:HRJ262091 IBF196560:IBF262091 ILB196560:ILB262091 IUX196560:IUX262091 JET196560:JET262091 JOP196560:JOP262091 JYL196560:JYL262091 KIH196560:KIH262091 KSD196560:KSD262091 LBZ196560:LBZ262091 LLV196560:LLV262091 LVR196560:LVR262091 MFN196560:MFN262091 MPJ196560:MPJ262091 MZF196560:MZF262091 NJB196560:NJB262091 NSX196560:NSX262091 OCT196560:OCT262091 OMP196560:OMP262091 OWL196560:OWL262091 PGH196560:PGH262091 PQD196560:PQD262091 PZZ196560:PZZ262091 QJV196560:QJV262091 QTR196560:QTR262091 RDN196560:RDN262091 RNJ196560:RNJ262091 RXF196560:RXF262091 SHB196560:SHB262091 SQX196560:SQX262091 TAT196560:TAT262091 TKP196560:TKP262091 TUL196560:TUL262091 UEH196560:UEH262091 UOD196560:UOD262091 UXZ196560:UXZ262091 VHV196560:VHV262091 VRR196560:VRR262091 WBN196560:WBN262091 WLJ196560:WLJ262091 WVF196560:WVF262091 IT262096:IT327627 SP262096:SP327627 ACL262096:ACL327627 AMH262096:AMH327627 AWD262096:AWD327627 BFZ262096:BFZ327627 BPV262096:BPV327627 BZR262096:BZR327627 CJN262096:CJN327627 CTJ262096:CTJ327627 DDF262096:DDF327627 DNB262096:DNB327627 DWX262096:DWX327627 EGT262096:EGT327627 EQP262096:EQP327627 FAL262096:FAL327627 FKH262096:FKH327627 FUD262096:FUD327627 GDZ262096:GDZ327627 GNV262096:GNV327627 GXR262096:GXR327627 HHN262096:HHN327627 HRJ262096:HRJ327627 IBF262096:IBF327627 ILB262096:ILB327627 IUX262096:IUX327627 JET262096:JET327627 JOP262096:JOP327627 JYL262096:JYL327627 KIH262096:KIH327627 KSD262096:KSD327627 LBZ262096:LBZ327627 LLV262096:LLV327627 LVR262096:LVR327627 MFN262096:MFN327627 MPJ262096:MPJ327627 MZF262096:MZF327627 NJB262096:NJB327627 NSX262096:NSX327627 OCT262096:OCT327627 OMP262096:OMP327627 OWL262096:OWL327627 PGH262096:PGH327627 PQD262096:PQD327627 PZZ262096:PZZ327627 QJV262096:QJV327627 QTR262096:QTR327627 RDN262096:RDN327627 RNJ262096:RNJ327627 RXF262096:RXF327627 SHB262096:SHB327627 SQX262096:SQX327627 TAT262096:TAT327627 TKP262096:TKP327627 TUL262096:TUL327627 UEH262096:UEH327627 UOD262096:UOD327627 UXZ262096:UXZ327627 VHV262096:VHV327627 VRR262096:VRR327627 WBN262096:WBN327627 WLJ262096:WLJ327627 WVF262096:WVF327627 IT327632:IT393163 SP327632:SP393163 ACL327632:ACL393163 AMH327632:AMH393163 AWD327632:AWD393163 BFZ327632:BFZ393163 BPV327632:BPV393163 BZR327632:BZR393163 CJN327632:CJN393163 CTJ327632:CTJ393163 DDF327632:DDF393163 DNB327632:DNB393163 DWX327632:DWX393163 EGT327632:EGT393163 EQP327632:EQP393163 FAL327632:FAL393163 FKH327632:FKH393163 FUD327632:FUD393163 GDZ327632:GDZ393163 GNV327632:GNV393163 GXR327632:GXR393163 HHN327632:HHN393163 HRJ327632:HRJ393163 IBF327632:IBF393163 ILB327632:ILB393163 IUX327632:IUX393163 JET327632:JET393163 JOP327632:JOP393163 JYL327632:JYL393163 KIH327632:KIH393163 KSD327632:KSD393163 LBZ327632:LBZ393163 LLV327632:LLV393163 LVR327632:LVR393163 MFN327632:MFN393163 MPJ327632:MPJ393163 MZF327632:MZF393163 NJB327632:NJB393163 NSX327632:NSX393163 OCT327632:OCT393163 OMP327632:OMP393163 OWL327632:OWL393163 PGH327632:PGH393163 PQD327632:PQD393163 PZZ327632:PZZ393163 QJV327632:QJV393163 QTR327632:QTR393163 RDN327632:RDN393163 RNJ327632:RNJ393163 RXF327632:RXF393163 SHB327632:SHB393163 SQX327632:SQX393163 TAT327632:TAT393163 TKP327632:TKP393163 TUL327632:TUL393163 UEH327632:UEH393163 UOD327632:UOD393163 UXZ327632:UXZ393163 VHV327632:VHV393163 VRR327632:VRR393163 WBN327632:WBN393163 WLJ327632:WLJ393163 WVF327632:WVF393163 IT393168:IT458699 SP393168:SP458699 ACL393168:ACL458699 AMH393168:AMH458699 AWD393168:AWD458699 BFZ393168:BFZ458699 BPV393168:BPV458699 BZR393168:BZR458699 CJN393168:CJN458699 CTJ393168:CTJ458699 DDF393168:DDF458699 DNB393168:DNB458699 DWX393168:DWX458699 EGT393168:EGT458699 EQP393168:EQP458699 FAL393168:FAL458699 FKH393168:FKH458699 FUD393168:FUD458699 GDZ393168:GDZ458699 GNV393168:GNV458699 GXR393168:GXR458699 HHN393168:HHN458699 HRJ393168:HRJ458699 IBF393168:IBF458699 ILB393168:ILB458699 IUX393168:IUX458699 JET393168:JET458699 JOP393168:JOP458699 JYL393168:JYL458699 KIH393168:KIH458699 KSD393168:KSD458699 LBZ393168:LBZ458699 LLV393168:LLV458699 LVR393168:LVR458699 MFN393168:MFN458699 MPJ393168:MPJ458699 MZF393168:MZF458699 NJB393168:NJB458699 NSX393168:NSX458699 OCT393168:OCT458699 OMP393168:OMP458699 OWL393168:OWL458699 PGH393168:PGH458699 PQD393168:PQD458699 PZZ393168:PZZ458699 QJV393168:QJV458699 QTR393168:QTR458699 RDN393168:RDN458699 RNJ393168:RNJ458699 RXF393168:RXF458699 SHB393168:SHB458699 SQX393168:SQX458699 TAT393168:TAT458699 TKP393168:TKP458699 TUL393168:TUL458699 UEH393168:UEH458699 UOD393168:UOD458699 UXZ393168:UXZ458699 VHV393168:VHV458699 VRR393168:VRR458699 WBN393168:WBN458699 WLJ393168:WLJ458699 WVF393168:WVF458699 IT458704:IT524235 SP458704:SP524235 ACL458704:ACL524235 AMH458704:AMH524235 AWD458704:AWD524235 BFZ458704:BFZ524235 BPV458704:BPV524235 BZR458704:BZR524235 CJN458704:CJN524235 CTJ458704:CTJ524235 DDF458704:DDF524235 DNB458704:DNB524235 DWX458704:DWX524235 EGT458704:EGT524235 EQP458704:EQP524235 FAL458704:FAL524235 FKH458704:FKH524235 FUD458704:FUD524235 GDZ458704:GDZ524235 GNV458704:GNV524235 GXR458704:GXR524235 HHN458704:HHN524235 HRJ458704:HRJ524235 IBF458704:IBF524235 ILB458704:ILB524235 IUX458704:IUX524235 JET458704:JET524235 JOP458704:JOP524235 JYL458704:JYL524235 KIH458704:KIH524235 KSD458704:KSD524235 LBZ458704:LBZ524235 LLV458704:LLV524235 LVR458704:LVR524235 MFN458704:MFN524235 MPJ458704:MPJ524235 MZF458704:MZF524235 NJB458704:NJB524235 NSX458704:NSX524235 OCT458704:OCT524235 OMP458704:OMP524235 OWL458704:OWL524235 PGH458704:PGH524235 PQD458704:PQD524235 PZZ458704:PZZ524235 QJV458704:QJV524235 QTR458704:QTR524235 RDN458704:RDN524235 RNJ458704:RNJ524235 RXF458704:RXF524235 SHB458704:SHB524235 SQX458704:SQX524235 TAT458704:TAT524235 TKP458704:TKP524235 TUL458704:TUL524235 UEH458704:UEH524235 UOD458704:UOD524235 UXZ458704:UXZ524235 VHV458704:VHV524235 VRR458704:VRR524235 WBN458704:WBN524235 WLJ458704:WLJ524235 WVF458704:WVF524235 IT524240:IT589771 SP524240:SP589771 ACL524240:ACL589771 AMH524240:AMH589771 AWD524240:AWD589771 BFZ524240:BFZ589771 BPV524240:BPV589771 BZR524240:BZR589771 CJN524240:CJN589771 CTJ524240:CTJ589771 DDF524240:DDF589771 DNB524240:DNB589771 DWX524240:DWX589771 EGT524240:EGT589771 EQP524240:EQP589771 FAL524240:FAL589771 FKH524240:FKH589771 FUD524240:FUD589771 GDZ524240:GDZ589771 GNV524240:GNV589771 GXR524240:GXR589771 HHN524240:HHN589771 HRJ524240:HRJ589771 IBF524240:IBF589771 ILB524240:ILB589771 IUX524240:IUX589771 JET524240:JET589771 JOP524240:JOP589771 JYL524240:JYL589771 KIH524240:KIH589771 KSD524240:KSD589771 LBZ524240:LBZ589771 LLV524240:LLV589771 LVR524240:LVR589771 MFN524240:MFN589771 MPJ524240:MPJ589771 MZF524240:MZF589771 NJB524240:NJB589771 NSX524240:NSX589771 OCT524240:OCT589771 OMP524240:OMP589771 OWL524240:OWL589771 PGH524240:PGH589771 PQD524240:PQD589771 PZZ524240:PZZ589771 QJV524240:QJV589771 QTR524240:QTR589771 RDN524240:RDN589771 RNJ524240:RNJ589771 RXF524240:RXF589771 SHB524240:SHB589771 SQX524240:SQX589771 TAT524240:TAT589771 TKP524240:TKP589771 TUL524240:TUL589771 UEH524240:UEH589771 UOD524240:UOD589771 UXZ524240:UXZ589771 VHV524240:VHV589771 VRR524240:VRR589771 WBN524240:WBN589771 WLJ524240:WLJ589771 WVF524240:WVF589771 IT589776:IT655307 SP589776:SP655307 ACL589776:ACL655307 AMH589776:AMH655307 AWD589776:AWD655307 BFZ589776:BFZ655307 BPV589776:BPV655307 BZR589776:BZR655307 CJN589776:CJN655307 CTJ589776:CTJ655307 DDF589776:DDF655307 DNB589776:DNB655307 DWX589776:DWX655307 EGT589776:EGT655307 EQP589776:EQP655307 FAL589776:FAL655307 FKH589776:FKH655307 FUD589776:FUD655307 GDZ589776:GDZ655307 GNV589776:GNV655307 GXR589776:GXR655307 HHN589776:HHN655307 HRJ589776:HRJ655307 IBF589776:IBF655307 ILB589776:ILB655307 IUX589776:IUX655307 JET589776:JET655307 JOP589776:JOP655307 JYL589776:JYL655307 KIH589776:KIH655307 KSD589776:KSD655307 LBZ589776:LBZ655307 LLV589776:LLV655307 LVR589776:LVR655307 MFN589776:MFN655307 MPJ589776:MPJ655307 MZF589776:MZF655307 NJB589776:NJB655307 NSX589776:NSX655307 OCT589776:OCT655307 OMP589776:OMP655307 OWL589776:OWL655307 PGH589776:PGH655307 PQD589776:PQD655307 PZZ589776:PZZ655307 QJV589776:QJV655307 QTR589776:QTR655307 RDN589776:RDN655307 RNJ589776:RNJ655307 RXF589776:RXF655307 SHB589776:SHB655307 SQX589776:SQX655307 TAT589776:TAT655307 TKP589776:TKP655307 TUL589776:TUL655307 UEH589776:UEH655307 UOD589776:UOD655307 UXZ589776:UXZ655307 VHV589776:VHV655307 VRR589776:VRR655307 WBN589776:WBN655307 WLJ589776:WLJ655307 WVF589776:WVF655307 IT655312:IT720843 SP655312:SP720843 ACL655312:ACL720843 AMH655312:AMH720843 AWD655312:AWD720843 BFZ655312:BFZ720843 BPV655312:BPV720843 BZR655312:BZR720843 CJN655312:CJN720843 CTJ655312:CTJ720843 DDF655312:DDF720843 DNB655312:DNB720843 DWX655312:DWX720843 EGT655312:EGT720843 EQP655312:EQP720843 FAL655312:FAL720843 FKH655312:FKH720843 FUD655312:FUD720843 GDZ655312:GDZ720843 GNV655312:GNV720843 GXR655312:GXR720843 HHN655312:HHN720843 HRJ655312:HRJ720843 IBF655312:IBF720843 ILB655312:ILB720843 IUX655312:IUX720843 JET655312:JET720843 JOP655312:JOP720843 JYL655312:JYL720843 KIH655312:KIH720843 KSD655312:KSD720843 LBZ655312:LBZ720843 LLV655312:LLV720843 LVR655312:LVR720843 MFN655312:MFN720843 MPJ655312:MPJ720843 MZF655312:MZF720843 NJB655312:NJB720843 NSX655312:NSX720843 OCT655312:OCT720843 OMP655312:OMP720843 OWL655312:OWL720843 PGH655312:PGH720843 PQD655312:PQD720843 PZZ655312:PZZ720843 QJV655312:QJV720843 QTR655312:QTR720843 RDN655312:RDN720843 RNJ655312:RNJ720843 RXF655312:RXF720843 SHB655312:SHB720843 SQX655312:SQX720843 TAT655312:TAT720843 TKP655312:TKP720843 TUL655312:TUL720843 UEH655312:UEH720843 UOD655312:UOD720843 UXZ655312:UXZ720843 VHV655312:VHV720843 VRR655312:VRR720843 WBN655312:WBN720843 WLJ655312:WLJ720843 WVF655312:WVF720843 IT720848:IT786379 SP720848:SP786379 ACL720848:ACL786379 AMH720848:AMH786379 AWD720848:AWD786379 BFZ720848:BFZ786379 BPV720848:BPV786379 BZR720848:BZR786379 CJN720848:CJN786379 CTJ720848:CTJ786379 DDF720848:DDF786379 DNB720848:DNB786379 DWX720848:DWX786379 EGT720848:EGT786379 EQP720848:EQP786379 FAL720848:FAL786379 FKH720848:FKH786379 FUD720848:FUD786379 GDZ720848:GDZ786379 GNV720848:GNV786379 GXR720848:GXR786379 HHN720848:HHN786379 HRJ720848:HRJ786379 IBF720848:IBF786379 ILB720848:ILB786379 IUX720848:IUX786379 JET720848:JET786379 JOP720848:JOP786379 JYL720848:JYL786379 KIH720848:KIH786379 KSD720848:KSD786379 LBZ720848:LBZ786379 LLV720848:LLV786379 LVR720848:LVR786379 MFN720848:MFN786379 MPJ720848:MPJ786379 MZF720848:MZF786379 NJB720848:NJB786379 NSX720848:NSX786379 OCT720848:OCT786379 OMP720848:OMP786379 OWL720848:OWL786379 PGH720848:PGH786379 PQD720848:PQD786379 PZZ720848:PZZ786379 QJV720848:QJV786379 QTR720848:QTR786379 RDN720848:RDN786379 RNJ720848:RNJ786379 RXF720848:RXF786379 SHB720848:SHB786379 SQX720848:SQX786379 TAT720848:TAT786379 TKP720848:TKP786379 TUL720848:TUL786379 UEH720848:UEH786379 UOD720848:UOD786379 UXZ720848:UXZ786379 VHV720848:VHV786379 VRR720848:VRR786379 WBN720848:WBN786379 WLJ720848:WLJ786379 WVF720848:WVF786379 IT786384:IT851915 SP786384:SP851915 ACL786384:ACL851915 AMH786384:AMH851915 AWD786384:AWD851915 BFZ786384:BFZ851915 BPV786384:BPV851915 BZR786384:BZR851915 CJN786384:CJN851915 CTJ786384:CTJ851915 DDF786384:DDF851915 DNB786384:DNB851915 DWX786384:DWX851915 EGT786384:EGT851915 EQP786384:EQP851915 FAL786384:FAL851915 FKH786384:FKH851915 FUD786384:FUD851915 GDZ786384:GDZ851915 GNV786384:GNV851915 GXR786384:GXR851915 HHN786384:HHN851915 HRJ786384:HRJ851915 IBF786384:IBF851915 ILB786384:ILB851915 IUX786384:IUX851915 JET786384:JET851915 JOP786384:JOP851915 JYL786384:JYL851915 KIH786384:KIH851915 KSD786384:KSD851915 LBZ786384:LBZ851915 LLV786384:LLV851915 LVR786384:LVR851915 MFN786384:MFN851915 MPJ786384:MPJ851915 MZF786384:MZF851915 NJB786384:NJB851915 NSX786384:NSX851915 OCT786384:OCT851915 OMP786384:OMP851915 OWL786384:OWL851915 PGH786384:PGH851915 PQD786384:PQD851915 PZZ786384:PZZ851915 QJV786384:QJV851915 QTR786384:QTR851915 RDN786384:RDN851915 RNJ786384:RNJ851915 RXF786384:RXF851915 SHB786384:SHB851915 SQX786384:SQX851915 TAT786384:TAT851915 TKP786384:TKP851915 TUL786384:TUL851915 UEH786384:UEH851915 UOD786384:UOD851915 UXZ786384:UXZ851915 VHV786384:VHV851915 VRR786384:VRR851915 WBN786384:WBN851915 WLJ786384:WLJ851915 WVF786384:WVF851915 IT851920:IT917451 SP851920:SP917451 ACL851920:ACL917451 AMH851920:AMH917451 AWD851920:AWD917451 BFZ851920:BFZ917451 BPV851920:BPV917451 BZR851920:BZR917451 CJN851920:CJN917451 CTJ851920:CTJ917451 DDF851920:DDF917451 DNB851920:DNB917451 DWX851920:DWX917451 EGT851920:EGT917451 EQP851920:EQP917451 FAL851920:FAL917451 FKH851920:FKH917451 FUD851920:FUD917451 GDZ851920:GDZ917451 GNV851920:GNV917451 GXR851920:GXR917451 HHN851920:HHN917451 HRJ851920:HRJ917451 IBF851920:IBF917451 ILB851920:ILB917451 IUX851920:IUX917451 JET851920:JET917451 JOP851920:JOP917451 JYL851920:JYL917451 KIH851920:KIH917451 KSD851920:KSD917451 LBZ851920:LBZ917451 LLV851920:LLV917451 LVR851920:LVR917451 MFN851920:MFN917451 MPJ851920:MPJ917451 MZF851920:MZF917451 NJB851920:NJB917451 NSX851920:NSX917451 OCT851920:OCT917451 OMP851920:OMP917451 OWL851920:OWL917451 PGH851920:PGH917451 PQD851920:PQD917451 PZZ851920:PZZ917451 QJV851920:QJV917451 QTR851920:QTR917451 RDN851920:RDN917451 RNJ851920:RNJ917451 RXF851920:RXF917451 SHB851920:SHB917451 SQX851920:SQX917451 TAT851920:TAT917451 TKP851920:TKP917451 TUL851920:TUL917451 UEH851920:UEH917451 UOD851920:UOD917451 UXZ851920:UXZ917451 VHV851920:VHV917451 VRR851920:VRR917451 WBN851920:WBN917451 WLJ851920:WLJ917451 WVF851920:WVF917451 IT917456:IT982987 SP917456:SP982987 ACL917456:ACL982987 AMH917456:AMH982987 AWD917456:AWD982987 BFZ917456:BFZ982987 BPV917456:BPV982987 BZR917456:BZR982987 CJN917456:CJN982987 CTJ917456:CTJ982987 DDF917456:DDF982987 DNB917456:DNB982987 DWX917456:DWX982987 EGT917456:EGT982987 EQP917456:EQP982987 FAL917456:FAL982987 FKH917456:FKH982987 FUD917456:FUD982987 GDZ917456:GDZ982987 GNV917456:GNV982987 GXR917456:GXR982987 HHN917456:HHN982987 HRJ917456:HRJ982987 IBF917456:IBF982987 ILB917456:ILB982987 IUX917456:IUX982987 JET917456:JET982987 JOP917456:JOP982987 JYL917456:JYL982987 KIH917456:KIH982987 KSD917456:KSD982987 LBZ917456:LBZ982987 LLV917456:LLV982987 LVR917456:LVR982987 MFN917456:MFN982987 MPJ917456:MPJ982987 MZF917456:MZF982987 NJB917456:NJB982987 NSX917456:NSX982987 OCT917456:OCT982987 OMP917456:OMP982987 OWL917456:OWL982987 PGH917456:PGH982987 PQD917456:PQD982987 PZZ917456:PZZ982987 QJV917456:QJV982987 QTR917456:QTR982987 RDN917456:RDN982987 RNJ917456:RNJ982987 RXF917456:RXF982987 SHB917456:SHB982987 SQX917456:SQX982987 TAT917456:TAT982987 TKP917456:TKP982987 TUL917456:TUL982987 UEH917456:UEH982987 UOD917456:UOD982987 UXZ917456:UXZ982987 VHV917456:VHV982987 VRR917456:VRR982987 WBN917456:WBN982987 WLJ917456:WLJ982987 WVF917456:WVF982987 IT982992:IT1048576 SP982992:SP1048576 ACL982992:ACL1048576 AMH982992:AMH1048576 AWD982992:AWD1048576 BFZ982992:BFZ1048576 BPV982992:BPV1048576 BZR982992:BZR1048576 CJN982992:CJN1048576 CTJ982992:CTJ1048576 DDF982992:DDF1048576 DNB982992:DNB1048576 DWX982992:DWX1048576 EGT982992:EGT1048576 EQP982992:EQP1048576 FAL982992:FAL1048576 FKH982992:FKH1048576 FUD982992:FUD1048576 GDZ982992:GDZ1048576 GNV982992:GNV1048576 GXR982992:GXR1048576 HHN982992:HHN1048576 HRJ982992:HRJ1048576 IBF982992:IBF1048576 ILB982992:ILB1048576 IUX982992:IUX1048576 JET982992:JET1048576 JOP982992:JOP1048576 JYL982992:JYL1048576 KIH982992:KIH1048576 KSD982992:KSD1048576 LBZ982992:LBZ1048576 LLV982992:LLV1048576 LVR982992:LVR1048576 MFN982992:MFN1048576 MPJ982992:MPJ1048576 MZF982992:MZF1048576 NJB982992:NJB1048576 NSX982992:NSX1048576 OCT982992:OCT1048576 OMP982992:OMP1048576 OWL982992:OWL1048576 PGH982992:PGH1048576 PQD982992:PQD1048576 PZZ982992:PZZ1048576 QJV982992:QJV1048576 QTR982992:QTR1048576 RDN982992:RDN1048576 RNJ982992:RNJ1048576 RXF982992:RXF1048576 SHB982992:SHB1048576 SQX982992:SQX1048576 TAT982992:TAT1048576 TKP982992:TKP1048576 TUL982992:TUL1048576 UEH982992:UEH1048576 UOD982992:UOD1048576 UXZ982992:UXZ1048576 VHV982992:VHV1048576 VRR982992:VRR1048576 WBN982992:WBN1048576 WLJ982992:WLJ1048576 IT5:IT65483 SP5:SP65483 ACL5:ACL65483 AMH5:AMH65483 AWD5:AWD65483 BFZ5:BFZ65483 BPV5:BPV65483 BZR5:BZR65483 CJN5:CJN65483 CTJ5:CTJ65483 DDF5:DDF65483 DNB5:DNB65483 DWX5:DWX65483 EGT5:EGT65483 EQP5:EQP65483 FAL5:FAL65483 FKH5:FKH65483 FUD5:FUD65483 GDZ5:GDZ65483 GNV5:GNV65483 GXR5:GXR65483 HHN5:HHN65483 HRJ5:HRJ65483 IBF5:IBF65483 ILB5:ILB65483 IUX5:IUX65483 JET5:JET65483 JOP5:JOP65483 JYL5:JYL65483 KIH5:KIH65483 KSD5:KSD65483 LBZ5:LBZ65483 LLV5:LLV65483 LVR5:LVR65483 MFN5:MFN65483 MPJ5:MPJ65483 MZF5:MZF65483 NJB5:NJB65483 NSX5:NSX65483 OCT5:OCT65483 OMP5:OMP65483 OWL5:OWL65483 PGH5:PGH65483 PQD5:PQD65483 PZZ5:PZZ65483 QJV5:QJV65483 QTR5:QTR65483 RDN5:RDN65483 RNJ5:RNJ65483 RXF5:RXF65483 SHB5:SHB65483 SQX5:SQX65483 TAT5:TAT65483 TKP5:TKP65483 TUL5:TUL65483 UEH5:UEH65483 UOD5:UOD65483 UXZ5:UXZ65483 VHV5:VHV65483 VRR5:VRR65483 WBN5:WBN65483 WLJ5:WLJ65483 WVF5:WVF65483 B8:B16 A5:A65483">
       <formula1>"CH,US,TW,;"</formula1>
     </dataValidation>
-    <dataValidation type="list" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVO983045:WVO1048576 JC5:JC65536 SY5:SY65536 ACU5:ACU65536 AMQ5:AMQ65536 AWM5:AWM65536 BGI5:BGI65536 BQE5:BQE65536 CAA5:CAA65536 CJW5:CJW65536 CTS5:CTS65536 DDO5:DDO65536 DNK5:DNK65536 DXG5:DXG65536 EHC5:EHC65536 EQY5:EQY65536 FAU5:FAU65536 FKQ5:FKQ65536 FUM5:FUM65536 GEI5:GEI65536 GOE5:GOE65536 GYA5:GYA65536 HHW5:HHW65536 HRS5:HRS65536 IBO5:IBO65536 ILK5:ILK65536 IVG5:IVG65536 JFC5:JFC65536 JOY5:JOY65536 JYU5:JYU65536 KIQ5:KIQ65536 KSM5:KSM65536 LCI5:LCI65536 LME5:LME65536 LWA5:LWA65536 MFW5:MFW65536 MPS5:MPS65536 MZO5:MZO65536 NJK5:NJK65536 NTG5:NTG65536 ODC5:ODC65536 OMY5:OMY65536 OWU5:OWU65536 PGQ5:PGQ65536 PQM5:PQM65536 QAI5:QAI65536 QKE5:QKE65536 QUA5:QUA65536 RDW5:RDW65536 RNS5:RNS65536 RXO5:RXO65536 SHK5:SHK65536 SRG5:SRG65536 TBC5:TBC65536 TKY5:TKY65536 TUU5:TUU65536 UEQ5:UEQ65536 UOM5:UOM65536 UYI5:UYI65536 VIE5:VIE65536 VSA5:VSA65536 WBW5:WBW65536 WLS5:WLS65536 WVO5:WVO65536 JC65541:JC131072 SY65541:SY131072 ACU65541:ACU131072 AMQ65541:AMQ131072 AWM65541:AWM131072 BGI65541:BGI131072 BQE65541:BQE131072 CAA65541:CAA131072 CJW65541:CJW131072 CTS65541:CTS131072 DDO65541:DDO131072 DNK65541:DNK131072 DXG65541:DXG131072 EHC65541:EHC131072 EQY65541:EQY131072 FAU65541:FAU131072 FKQ65541:FKQ131072 FUM65541:FUM131072 GEI65541:GEI131072 GOE65541:GOE131072 GYA65541:GYA131072 HHW65541:HHW131072 HRS65541:HRS131072 IBO65541:IBO131072 ILK65541:ILK131072 IVG65541:IVG131072 JFC65541:JFC131072 JOY65541:JOY131072 JYU65541:JYU131072 KIQ65541:KIQ131072 KSM65541:KSM131072 LCI65541:LCI131072 LME65541:LME131072 LWA65541:LWA131072 MFW65541:MFW131072 MPS65541:MPS131072 MZO65541:MZO131072 NJK65541:NJK131072 NTG65541:NTG131072 ODC65541:ODC131072 OMY65541:OMY131072 OWU65541:OWU131072 PGQ65541:PGQ131072 PQM65541:PQM131072 QAI65541:QAI131072 QKE65541:QKE131072 QUA65541:QUA131072 RDW65541:RDW131072 RNS65541:RNS131072 RXO65541:RXO131072 SHK65541:SHK131072 SRG65541:SRG131072 TBC65541:TBC131072 TKY65541:TKY131072 TUU65541:TUU131072 UEQ65541:UEQ131072 UOM65541:UOM131072 UYI65541:UYI131072 VIE65541:VIE131072 VSA65541:VSA131072 WBW65541:WBW131072 WLS65541:WLS131072 WVO65541:WVO131072 JC131077:JC196608 SY131077:SY196608 ACU131077:ACU196608 AMQ131077:AMQ196608 AWM131077:AWM196608 BGI131077:BGI196608 BQE131077:BQE196608 CAA131077:CAA196608 CJW131077:CJW196608 CTS131077:CTS196608 DDO131077:DDO196608 DNK131077:DNK196608 DXG131077:DXG196608 EHC131077:EHC196608 EQY131077:EQY196608 FAU131077:FAU196608 FKQ131077:FKQ196608 FUM131077:FUM196608 GEI131077:GEI196608 GOE131077:GOE196608 GYA131077:GYA196608 HHW131077:HHW196608 HRS131077:HRS196608 IBO131077:IBO196608 ILK131077:ILK196608 IVG131077:IVG196608 JFC131077:JFC196608 JOY131077:JOY196608 JYU131077:JYU196608 KIQ131077:KIQ196608 KSM131077:KSM196608 LCI131077:LCI196608 LME131077:LME196608 LWA131077:LWA196608 MFW131077:MFW196608 MPS131077:MPS196608 MZO131077:MZO196608 NJK131077:NJK196608 NTG131077:NTG196608 ODC131077:ODC196608 OMY131077:OMY196608 OWU131077:OWU196608 PGQ131077:PGQ196608 PQM131077:PQM196608 QAI131077:QAI196608 QKE131077:QKE196608 QUA131077:QUA196608 RDW131077:RDW196608 RNS131077:RNS196608 RXO131077:RXO196608 SHK131077:SHK196608 SRG131077:SRG196608 TBC131077:TBC196608 TKY131077:TKY196608 TUU131077:TUU196608 UEQ131077:UEQ196608 UOM131077:UOM196608 UYI131077:UYI196608 VIE131077:VIE196608 VSA131077:VSA196608 WBW131077:WBW196608 WLS131077:WLS196608 WVO131077:WVO196608 JC196613:JC262144 SY196613:SY262144 ACU196613:ACU262144 AMQ196613:AMQ262144 AWM196613:AWM262144 BGI196613:BGI262144 BQE196613:BQE262144 CAA196613:CAA262144 CJW196613:CJW262144 CTS196613:CTS262144 DDO196613:DDO262144 DNK196613:DNK262144 DXG196613:DXG262144 EHC196613:EHC262144 EQY196613:EQY262144 FAU196613:FAU262144 FKQ196613:FKQ262144 FUM196613:FUM262144 GEI196613:GEI262144 GOE196613:GOE262144 GYA196613:GYA262144 HHW196613:HHW262144 HRS196613:HRS262144 IBO196613:IBO262144 ILK196613:ILK262144 IVG196613:IVG262144 JFC196613:JFC262144 JOY196613:JOY262144 JYU196613:JYU262144 KIQ196613:KIQ262144 KSM196613:KSM262144 LCI196613:LCI262144 LME196613:LME262144 LWA196613:LWA262144 MFW196613:MFW262144 MPS196613:MPS262144 MZO196613:MZO262144 NJK196613:NJK262144 NTG196613:NTG262144 ODC196613:ODC262144 OMY196613:OMY262144 OWU196613:OWU262144 PGQ196613:PGQ262144 PQM196613:PQM262144 QAI196613:QAI262144 QKE196613:QKE262144 QUA196613:QUA262144 RDW196613:RDW262144 RNS196613:RNS262144 RXO196613:RXO262144 SHK196613:SHK262144 SRG196613:SRG262144 TBC196613:TBC262144 TKY196613:TKY262144 TUU196613:TUU262144 UEQ196613:UEQ262144 UOM196613:UOM262144 UYI196613:UYI262144 VIE196613:VIE262144 VSA196613:VSA262144 WBW196613:WBW262144 WLS196613:WLS262144 WVO196613:WVO262144 JC262149:JC327680 SY262149:SY327680 ACU262149:ACU327680 AMQ262149:AMQ327680 AWM262149:AWM327680 BGI262149:BGI327680 BQE262149:BQE327680 CAA262149:CAA327680 CJW262149:CJW327680 CTS262149:CTS327680 DDO262149:DDO327680 DNK262149:DNK327680 DXG262149:DXG327680 EHC262149:EHC327680 EQY262149:EQY327680 FAU262149:FAU327680 FKQ262149:FKQ327680 FUM262149:FUM327680 GEI262149:GEI327680 GOE262149:GOE327680 GYA262149:GYA327680 HHW262149:HHW327680 HRS262149:HRS327680 IBO262149:IBO327680 ILK262149:ILK327680 IVG262149:IVG327680 JFC262149:JFC327680 JOY262149:JOY327680 JYU262149:JYU327680 KIQ262149:KIQ327680 KSM262149:KSM327680 LCI262149:LCI327680 LME262149:LME327680 LWA262149:LWA327680 MFW262149:MFW327680 MPS262149:MPS327680 MZO262149:MZO327680 NJK262149:NJK327680 NTG262149:NTG327680 ODC262149:ODC327680 OMY262149:OMY327680 OWU262149:OWU327680 PGQ262149:PGQ327680 PQM262149:PQM327680 QAI262149:QAI327680 QKE262149:QKE327680 QUA262149:QUA327680 RDW262149:RDW327680 RNS262149:RNS327680 RXO262149:RXO327680 SHK262149:SHK327680 SRG262149:SRG327680 TBC262149:TBC327680 TKY262149:TKY327680 TUU262149:TUU327680 UEQ262149:UEQ327680 UOM262149:UOM327680 UYI262149:UYI327680 VIE262149:VIE327680 VSA262149:VSA327680 WBW262149:WBW327680 WLS262149:WLS327680 WVO262149:WVO327680 JC327685:JC393216 SY327685:SY393216 ACU327685:ACU393216 AMQ327685:AMQ393216 AWM327685:AWM393216 BGI327685:BGI393216 BQE327685:BQE393216 CAA327685:CAA393216 CJW327685:CJW393216 CTS327685:CTS393216 DDO327685:DDO393216 DNK327685:DNK393216 DXG327685:DXG393216 EHC327685:EHC393216 EQY327685:EQY393216 FAU327685:FAU393216 FKQ327685:FKQ393216 FUM327685:FUM393216 GEI327685:GEI393216 GOE327685:GOE393216 GYA327685:GYA393216 HHW327685:HHW393216 HRS327685:HRS393216 IBO327685:IBO393216 ILK327685:ILK393216 IVG327685:IVG393216 JFC327685:JFC393216 JOY327685:JOY393216 JYU327685:JYU393216 KIQ327685:KIQ393216 KSM327685:KSM393216 LCI327685:LCI393216 LME327685:LME393216 LWA327685:LWA393216 MFW327685:MFW393216 MPS327685:MPS393216 MZO327685:MZO393216 NJK327685:NJK393216 NTG327685:NTG393216 ODC327685:ODC393216 OMY327685:OMY393216 OWU327685:OWU393216 PGQ327685:PGQ393216 PQM327685:PQM393216 QAI327685:QAI393216 QKE327685:QKE393216 QUA327685:QUA393216 RDW327685:RDW393216 RNS327685:RNS393216 RXO327685:RXO393216 SHK327685:SHK393216 SRG327685:SRG393216 TBC327685:TBC393216 TKY327685:TKY393216 TUU327685:TUU393216 UEQ327685:UEQ393216 UOM327685:UOM393216 UYI327685:UYI393216 VIE327685:VIE393216 VSA327685:VSA393216 WBW327685:WBW393216 WLS327685:WLS393216 WVO327685:WVO393216 JC393221:JC458752 SY393221:SY458752 ACU393221:ACU458752 AMQ393221:AMQ458752 AWM393221:AWM458752 BGI393221:BGI458752 BQE393221:BQE458752 CAA393221:CAA458752 CJW393221:CJW458752 CTS393221:CTS458752 DDO393221:DDO458752 DNK393221:DNK458752 DXG393221:DXG458752 EHC393221:EHC458752 EQY393221:EQY458752 FAU393221:FAU458752 FKQ393221:FKQ458752 FUM393221:FUM458752 GEI393221:GEI458752 GOE393221:GOE458752 GYA393221:GYA458752 HHW393221:HHW458752 HRS393221:HRS458752 IBO393221:IBO458752 ILK393221:ILK458752 IVG393221:IVG458752 JFC393221:JFC458752 JOY393221:JOY458752 JYU393221:JYU458752 KIQ393221:KIQ458752 KSM393221:KSM458752 LCI393221:LCI458752 LME393221:LME458752 LWA393221:LWA458752 MFW393221:MFW458752 MPS393221:MPS458752 MZO393221:MZO458752 NJK393221:NJK458752 NTG393221:NTG458752 ODC393221:ODC458752 OMY393221:OMY458752 OWU393221:OWU458752 PGQ393221:PGQ458752 PQM393221:PQM458752 QAI393221:QAI458752 QKE393221:QKE458752 QUA393221:QUA458752 RDW393221:RDW458752 RNS393221:RNS458752 RXO393221:RXO458752 SHK393221:SHK458752 SRG393221:SRG458752 TBC393221:TBC458752 TKY393221:TKY458752 TUU393221:TUU458752 UEQ393221:UEQ458752 UOM393221:UOM458752 UYI393221:UYI458752 VIE393221:VIE458752 VSA393221:VSA458752 WBW393221:WBW458752 WLS393221:WLS458752 WVO393221:WVO458752 JC458757:JC524288 SY458757:SY524288 ACU458757:ACU524288 AMQ458757:AMQ524288 AWM458757:AWM524288 BGI458757:BGI524288 BQE458757:BQE524288 CAA458757:CAA524288 CJW458757:CJW524288 CTS458757:CTS524288 DDO458757:DDO524288 DNK458757:DNK524288 DXG458757:DXG524288 EHC458757:EHC524288 EQY458757:EQY524288 FAU458757:FAU524288 FKQ458757:FKQ524288 FUM458757:FUM524288 GEI458757:GEI524288 GOE458757:GOE524288 GYA458757:GYA524288 HHW458757:HHW524288 HRS458757:HRS524288 IBO458757:IBO524288 ILK458757:ILK524288 IVG458757:IVG524288 JFC458757:JFC524288 JOY458757:JOY524288 JYU458757:JYU524288 KIQ458757:KIQ524288 KSM458757:KSM524288 LCI458757:LCI524288 LME458757:LME524288 LWA458757:LWA524288 MFW458757:MFW524288 MPS458757:MPS524288 MZO458757:MZO524288 NJK458757:NJK524288 NTG458757:NTG524288 ODC458757:ODC524288 OMY458757:OMY524288 OWU458757:OWU524288 PGQ458757:PGQ524288 PQM458757:PQM524288 QAI458757:QAI524288 QKE458757:QKE524288 QUA458757:QUA524288 RDW458757:RDW524288 RNS458757:RNS524288 RXO458757:RXO524288 SHK458757:SHK524288 SRG458757:SRG524288 TBC458757:TBC524288 TKY458757:TKY524288 TUU458757:TUU524288 UEQ458757:UEQ524288 UOM458757:UOM524288 UYI458757:UYI524288 VIE458757:VIE524288 VSA458757:VSA524288 WBW458757:WBW524288 WLS458757:WLS524288 WVO458757:WVO524288 JC524293:JC589824 SY524293:SY589824 ACU524293:ACU589824 AMQ524293:AMQ589824 AWM524293:AWM589824 BGI524293:BGI589824 BQE524293:BQE589824 CAA524293:CAA589824 CJW524293:CJW589824 CTS524293:CTS589824 DDO524293:DDO589824 DNK524293:DNK589824 DXG524293:DXG589824 EHC524293:EHC589824 EQY524293:EQY589824 FAU524293:FAU589824 FKQ524293:FKQ589824 FUM524293:FUM589824 GEI524293:GEI589824 GOE524293:GOE589824 GYA524293:GYA589824 HHW524293:HHW589824 HRS524293:HRS589824 IBO524293:IBO589824 ILK524293:ILK589824 IVG524293:IVG589824 JFC524293:JFC589824 JOY524293:JOY589824 JYU524293:JYU589824 KIQ524293:KIQ589824 KSM524293:KSM589824 LCI524293:LCI589824 LME524293:LME589824 LWA524293:LWA589824 MFW524293:MFW589824 MPS524293:MPS589824 MZO524293:MZO589824 NJK524293:NJK589824 NTG524293:NTG589824 ODC524293:ODC589824 OMY524293:OMY589824 OWU524293:OWU589824 PGQ524293:PGQ589824 PQM524293:PQM589824 QAI524293:QAI589824 QKE524293:QKE589824 QUA524293:QUA589824 RDW524293:RDW589824 RNS524293:RNS589824 RXO524293:RXO589824 SHK524293:SHK589824 SRG524293:SRG589824 TBC524293:TBC589824 TKY524293:TKY589824 TUU524293:TUU589824 UEQ524293:UEQ589824 UOM524293:UOM589824 UYI524293:UYI589824 VIE524293:VIE589824 VSA524293:VSA589824 WBW524293:WBW589824 WLS524293:WLS589824 WVO524293:WVO589824 JC589829:JC655360 SY589829:SY655360 ACU589829:ACU655360 AMQ589829:AMQ655360 AWM589829:AWM655360 BGI589829:BGI655360 BQE589829:BQE655360 CAA589829:CAA655360 CJW589829:CJW655360 CTS589829:CTS655360 DDO589829:DDO655360 DNK589829:DNK655360 DXG589829:DXG655360 EHC589829:EHC655360 EQY589829:EQY655360 FAU589829:FAU655360 FKQ589829:FKQ655360 FUM589829:FUM655360 GEI589829:GEI655360 GOE589829:GOE655360 GYA589829:GYA655360 HHW589829:HHW655360 HRS589829:HRS655360 IBO589829:IBO655360 ILK589829:ILK655360 IVG589829:IVG655360 JFC589829:JFC655360 JOY589829:JOY655360 JYU589829:JYU655360 KIQ589829:KIQ655360 KSM589829:KSM655360 LCI589829:LCI655360 LME589829:LME655360 LWA589829:LWA655360 MFW589829:MFW655360 MPS589829:MPS655360 MZO589829:MZO655360 NJK589829:NJK655360 NTG589829:NTG655360 ODC589829:ODC655360 OMY589829:OMY655360 OWU589829:OWU655360 PGQ589829:PGQ655360 PQM589829:PQM655360 QAI589829:QAI655360 QKE589829:QKE655360 QUA589829:QUA655360 RDW589829:RDW655360 RNS589829:RNS655360 RXO589829:RXO655360 SHK589829:SHK655360 SRG589829:SRG655360 TBC589829:TBC655360 TKY589829:TKY655360 TUU589829:TUU655360 UEQ589829:UEQ655360 UOM589829:UOM655360 UYI589829:UYI655360 VIE589829:VIE655360 VSA589829:VSA655360 WBW589829:WBW655360 WLS589829:WLS655360 WVO589829:WVO655360 JC655365:JC720896 SY655365:SY720896 ACU655365:ACU720896 AMQ655365:AMQ720896 AWM655365:AWM720896 BGI655365:BGI720896 BQE655365:BQE720896 CAA655365:CAA720896 CJW655365:CJW720896 CTS655365:CTS720896 DDO655365:DDO720896 DNK655365:DNK720896 DXG655365:DXG720896 EHC655365:EHC720896 EQY655365:EQY720896 FAU655365:FAU720896 FKQ655365:FKQ720896 FUM655365:FUM720896 GEI655365:GEI720896 GOE655365:GOE720896 GYA655365:GYA720896 HHW655365:HHW720896 HRS655365:HRS720896 IBO655365:IBO720896 ILK655365:ILK720896 IVG655365:IVG720896 JFC655365:JFC720896 JOY655365:JOY720896 JYU655365:JYU720896 KIQ655365:KIQ720896 KSM655365:KSM720896 LCI655365:LCI720896 LME655365:LME720896 LWA655365:LWA720896 MFW655365:MFW720896 MPS655365:MPS720896 MZO655365:MZO720896 NJK655365:NJK720896 NTG655365:NTG720896 ODC655365:ODC720896 OMY655365:OMY720896 OWU655365:OWU720896 PGQ655365:PGQ720896 PQM655365:PQM720896 QAI655365:QAI720896 QKE655365:QKE720896 QUA655365:QUA720896 RDW655365:RDW720896 RNS655365:RNS720896 RXO655365:RXO720896 SHK655365:SHK720896 SRG655365:SRG720896 TBC655365:TBC720896 TKY655365:TKY720896 TUU655365:TUU720896 UEQ655365:UEQ720896 UOM655365:UOM720896 UYI655365:UYI720896 VIE655365:VIE720896 VSA655365:VSA720896 WBW655365:WBW720896 WLS655365:WLS720896 WVO655365:WVO720896 JC720901:JC786432 SY720901:SY786432 ACU720901:ACU786432 AMQ720901:AMQ786432 AWM720901:AWM786432 BGI720901:BGI786432 BQE720901:BQE786432 CAA720901:CAA786432 CJW720901:CJW786432 CTS720901:CTS786432 DDO720901:DDO786432 DNK720901:DNK786432 DXG720901:DXG786432 EHC720901:EHC786432 EQY720901:EQY786432 FAU720901:FAU786432 FKQ720901:FKQ786432 FUM720901:FUM786432 GEI720901:GEI786432 GOE720901:GOE786432 GYA720901:GYA786432 HHW720901:HHW786432 HRS720901:HRS786432 IBO720901:IBO786432 ILK720901:ILK786432 IVG720901:IVG786432 JFC720901:JFC786432 JOY720901:JOY786432 JYU720901:JYU786432 KIQ720901:KIQ786432 KSM720901:KSM786432 LCI720901:LCI786432 LME720901:LME786432 LWA720901:LWA786432 MFW720901:MFW786432 MPS720901:MPS786432 MZO720901:MZO786432 NJK720901:NJK786432 NTG720901:NTG786432 ODC720901:ODC786432 OMY720901:OMY786432 OWU720901:OWU786432 PGQ720901:PGQ786432 PQM720901:PQM786432 QAI720901:QAI786432 QKE720901:QKE786432 QUA720901:QUA786432 RDW720901:RDW786432 RNS720901:RNS786432 RXO720901:RXO786432 SHK720901:SHK786432 SRG720901:SRG786432 TBC720901:TBC786432 TKY720901:TKY786432 TUU720901:TUU786432 UEQ720901:UEQ786432 UOM720901:UOM786432 UYI720901:UYI786432 VIE720901:VIE786432 VSA720901:VSA786432 WBW720901:WBW786432 WLS720901:WLS786432 WVO720901:WVO786432 JC786437:JC851968 SY786437:SY851968 ACU786437:ACU851968 AMQ786437:AMQ851968 AWM786437:AWM851968 BGI786437:BGI851968 BQE786437:BQE851968 CAA786437:CAA851968 CJW786437:CJW851968 CTS786437:CTS851968 DDO786437:DDO851968 DNK786437:DNK851968 DXG786437:DXG851968 EHC786437:EHC851968 EQY786437:EQY851968 FAU786437:FAU851968 FKQ786437:FKQ851968 FUM786437:FUM851968 GEI786437:GEI851968 GOE786437:GOE851968 GYA786437:GYA851968 HHW786437:HHW851968 HRS786437:HRS851968 IBO786437:IBO851968 ILK786437:ILK851968 IVG786437:IVG851968 JFC786437:JFC851968 JOY786437:JOY851968 JYU786437:JYU851968 KIQ786437:KIQ851968 KSM786437:KSM851968 LCI786437:LCI851968 LME786437:LME851968 LWA786437:LWA851968 MFW786437:MFW851968 MPS786437:MPS851968 MZO786437:MZO851968 NJK786437:NJK851968 NTG786437:NTG851968 ODC786437:ODC851968 OMY786437:OMY851968 OWU786437:OWU851968 PGQ786437:PGQ851968 PQM786437:PQM851968 QAI786437:QAI851968 QKE786437:QKE851968 QUA786437:QUA851968 RDW786437:RDW851968 RNS786437:RNS851968 RXO786437:RXO851968 SHK786437:SHK851968 SRG786437:SRG851968 TBC786437:TBC851968 TKY786437:TKY851968 TUU786437:TUU851968 UEQ786437:UEQ851968 UOM786437:UOM851968 UYI786437:UYI851968 VIE786437:VIE851968 VSA786437:VSA851968 WBW786437:WBW851968 WLS786437:WLS851968 WVO786437:WVO851968 JC851973:JC917504 SY851973:SY917504 ACU851973:ACU917504 AMQ851973:AMQ917504 AWM851973:AWM917504 BGI851973:BGI917504 BQE851973:BQE917504 CAA851973:CAA917504 CJW851973:CJW917504 CTS851973:CTS917504 DDO851973:DDO917504 DNK851973:DNK917504 DXG851973:DXG917504 EHC851973:EHC917504 EQY851973:EQY917504 FAU851973:FAU917504 FKQ851973:FKQ917504 FUM851973:FUM917504 GEI851973:GEI917504 GOE851973:GOE917504 GYA851973:GYA917504 HHW851973:HHW917504 HRS851973:HRS917504 IBO851973:IBO917504 ILK851973:ILK917504 IVG851973:IVG917504 JFC851973:JFC917504 JOY851973:JOY917504 JYU851973:JYU917504 KIQ851973:KIQ917504 KSM851973:KSM917504 LCI851973:LCI917504 LME851973:LME917504 LWA851973:LWA917504 MFW851973:MFW917504 MPS851973:MPS917504 MZO851973:MZO917504 NJK851973:NJK917504 NTG851973:NTG917504 ODC851973:ODC917504 OMY851973:OMY917504 OWU851973:OWU917504 PGQ851973:PGQ917504 PQM851973:PQM917504 QAI851973:QAI917504 QKE851973:QKE917504 QUA851973:QUA917504 RDW851973:RDW917504 RNS851973:RNS917504 RXO851973:RXO917504 SHK851973:SHK917504 SRG851973:SRG917504 TBC851973:TBC917504 TKY851973:TKY917504 TUU851973:TUU917504 UEQ851973:UEQ917504 UOM851973:UOM917504 UYI851973:UYI917504 VIE851973:VIE917504 VSA851973:VSA917504 WBW851973:WBW917504 WLS851973:WLS917504 WVO851973:WVO917504 JC917509:JC983040 SY917509:SY983040 ACU917509:ACU983040 AMQ917509:AMQ983040 AWM917509:AWM983040 BGI917509:BGI983040 BQE917509:BQE983040 CAA917509:CAA983040 CJW917509:CJW983040 CTS917509:CTS983040 DDO917509:DDO983040 DNK917509:DNK983040 DXG917509:DXG983040 EHC917509:EHC983040 EQY917509:EQY983040 FAU917509:FAU983040 FKQ917509:FKQ983040 FUM917509:FUM983040 GEI917509:GEI983040 GOE917509:GOE983040 GYA917509:GYA983040 HHW917509:HHW983040 HRS917509:HRS983040 IBO917509:IBO983040 ILK917509:ILK983040 IVG917509:IVG983040 JFC917509:JFC983040 JOY917509:JOY983040 JYU917509:JYU983040 KIQ917509:KIQ983040 KSM917509:KSM983040 LCI917509:LCI983040 LME917509:LME983040 LWA917509:LWA983040 MFW917509:MFW983040 MPS917509:MPS983040 MZO917509:MZO983040 NJK917509:NJK983040 NTG917509:NTG983040 ODC917509:ODC983040 OMY917509:OMY983040 OWU917509:OWU983040 PGQ917509:PGQ983040 PQM917509:PQM983040 QAI917509:QAI983040 QKE917509:QKE983040 QUA917509:QUA983040 RDW917509:RDW983040 RNS917509:RNS983040 RXO917509:RXO983040 SHK917509:SHK983040 SRG917509:SRG983040 TBC917509:TBC983040 TKY917509:TKY983040 TUU917509:TUU983040 UEQ917509:UEQ983040 UOM917509:UOM983040 UYI917509:UYI983040 VIE917509:VIE983040 VSA917509:VSA983040 WBW917509:WBW983040 WLS917509:WLS983040 WVO917509:WVO983040 JC983045:JC1048576 SY983045:SY1048576 ACU983045:ACU1048576 AMQ983045:AMQ1048576 AWM983045:AWM1048576 BGI983045:BGI1048576 BQE983045:BQE1048576 CAA983045:CAA1048576 CJW983045:CJW1048576 CTS983045:CTS1048576 DDO983045:DDO1048576 DNK983045:DNK1048576 DXG983045:DXG1048576 EHC983045:EHC1048576 EQY983045:EQY1048576 FAU983045:FAU1048576 FKQ983045:FKQ1048576 FUM983045:FUM1048576 GEI983045:GEI1048576 GOE983045:GOE1048576 GYA983045:GYA1048576 HHW983045:HHW1048576 HRS983045:HRS1048576 IBO983045:IBO1048576 ILK983045:ILK1048576 IVG983045:IVG1048576 JFC983045:JFC1048576 JOY983045:JOY1048576 JYU983045:JYU1048576 KIQ983045:KIQ1048576 KSM983045:KSM1048576 LCI983045:LCI1048576 LME983045:LME1048576 LWA983045:LWA1048576 MFW983045:MFW1048576 MPS983045:MPS1048576 MZO983045:MZO1048576 NJK983045:NJK1048576 NTG983045:NTG1048576 ODC983045:ODC1048576 OMY983045:OMY1048576 OWU983045:OWU1048576 PGQ983045:PGQ1048576 PQM983045:PQM1048576 QAI983045:QAI1048576 QKE983045:QKE1048576 QUA983045:QUA1048576 RDW983045:RDW1048576 RNS983045:RNS1048576 RXO983045:RXO1048576 SHK983045:SHK1048576 SRG983045:SRG1048576 TBC983045:TBC1048576 TKY983045:TKY1048576 TUU983045:TUU1048576 UEQ983045:UEQ1048576 UOM983045:UOM1048576 UYI983045:UYI1048576 VIE983045:VIE1048576 VSA983045:VSA1048576 WBW983045:WBW1048576 WLS983045:WLS1048576">
+    <dataValidation type="list" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVO982992:WVO1048576 JC65488:JC131019 SY65488:SY131019 ACU65488:ACU131019 AMQ65488:AMQ131019 AWM65488:AWM131019 BGI65488:BGI131019 BQE65488:BQE131019 CAA65488:CAA131019 CJW65488:CJW131019 CTS65488:CTS131019 DDO65488:DDO131019 DNK65488:DNK131019 DXG65488:DXG131019 EHC65488:EHC131019 EQY65488:EQY131019 FAU65488:FAU131019 FKQ65488:FKQ131019 FUM65488:FUM131019 GEI65488:GEI131019 GOE65488:GOE131019 GYA65488:GYA131019 HHW65488:HHW131019 HRS65488:HRS131019 IBO65488:IBO131019 ILK65488:ILK131019 IVG65488:IVG131019 JFC65488:JFC131019 JOY65488:JOY131019 JYU65488:JYU131019 KIQ65488:KIQ131019 KSM65488:KSM131019 LCI65488:LCI131019 LME65488:LME131019 LWA65488:LWA131019 MFW65488:MFW131019 MPS65488:MPS131019 MZO65488:MZO131019 NJK65488:NJK131019 NTG65488:NTG131019 ODC65488:ODC131019 OMY65488:OMY131019 OWU65488:OWU131019 PGQ65488:PGQ131019 PQM65488:PQM131019 QAI65488:QAI131019 QKE65488:QKE131019 QUA65488:QUA131019 RDW65488:RDW131019 RNS65488:RNS131019 RXO65488:RXO131019 SHK65488:SHK131019 SRG65488:SRG131019 TBC65488:TBC131019 TKY65488:TKY131019 TUU65488:TUU131019 UEQ65488:UEQ131019 UOM65488:UOM131019 UYI65488:UYI131019 VIE65488:VIE131019 VSA65488:VSA131019 WBW65488:WBW131019 WLS65488:WLS131019 WVO65488:WVO131019 JC131024:JC196555 SY131024:SY196555 ACU131024:ACU196555 AMQ131024:AMQ196555 AWM131024:AWM196555 BGI131024:BGI196555 BQE131024:BQE196555 CAA131024:CAA196555 CJW131024:CJW196555 CTS131024:CTS196555 DDO131024:DDO196555 DNK131024:DNK196555 DXG131024:DXG196555 EHC131024:EHC196555 EQY131024:EQY196555 FAU131024:FAU196555 FKQ131024:FKQ196555 FUM131024:FUM196555 GEI131024:GEI196555 GOE131024:GOE196555 GYA131024:GYA196555 HHW131024:HHW196555 HRS131024:HRS196555 IBO131024:IBO196555 ILK131024:ILK196555 IVG131024:IVG196555 JFC131024:JFC196555 JOY131024:JOY196555 JYU131024:JYU196555 KIQ131024:KIQ196555 KSM131024:KSM196555 LCI131024:LCI196555 LME131024:LME196555 LWA131024:LWA196555 MFW131024:MFW196555 MPS131024:MPS196555 MZO131024:MZO196555 NJK131024:NJK196555 NTG131024:NTG196555 ODC131024:ODC196555 OMY131024:OMY196555 OWU131024:OWU196555 PGQ131024:PGQ196555 PQM131024:PQM196555 QAI131024:QAI196555 QKE131024:QKE196555 QUA131024:QUA196555 RDW131024:RDW196555 RNS131024:RNS196555 RXO131024:RXO196555 SHK131024:SHK196555 SRG131024:SRG196555 TBC131024:TBC196555 TKY131024:TKY196555 TUU131024:TUU196555 UEQ131024:UEQ196555 UOM131024:UOM196555 UYI131024:UYI196555 VIE131024:VIE196555 VSA131024:VSA196555 WBW131024:WBW196555 WLS131024:WLS196555 WVO131024:WVO196555 JC196560:JC262091 SY196560:SY262091 ACU196560:ACU262091 AMQ196560:AMQ262091 AWM196560:AWM262091 BGI196560:BGI262091 BQE196560:BQE262091 CAA196560:CAA262091 CJW196560:CJW262091 CTS196560:CTS262091 DDO196560:DDO262091 DNK196560:DNK262091 DXG196560:DXG262091 EHC196560:EHC262091 EQY196560:EQY262091 FAU196560:FAU262091 FKQ196560:FKQ262091 FUM196560:FUM262091 GEI196560:GEI262091 GOE196560:GOE262091 GYA196560:GYA262091 HHW196560:HHW262091 HRS196560:HRS262091 IBO196560:IBO262091 ILK196560:ILK262091 IVG196560:IVG262091 JFC196560:JFC262091 JOY196560:JOY262091 JYU196560:JYU262091 KIQ196560:KIQ262091 KSM196560:KSM262091 LCI196560:LCI262091 LME196560:LME262091 LWA196560:LWA262091 MFW196560:MFW262091 MPS196560:MPS262091 MZO196560:MZO262091 NJK196560:NJK262091 NTG196560:NTG262091 ODC196560:ODC262091 OMY196560:OMY262091 OWU196560:OWU262091 PGQ196560:PGQ262091 PQM196560:PQM262091 QAI196560:QAI262091 QKE196560:QKE262091 QUA196560:QUA262091 RDW196560:RDW262091 RNS196560:RNS262091 RXO196560:RXO262091 SHK196560:SHK262091 SRG196560:SRG262091 TBC196560:TBC262091 TKY196560:TKY262091 TUU196560:TUU262091 UEQ196560:UEQ262091 UOM196560:UOM262091 UYI196560:UYI262091 VIE196560:VIE262091 VSA196560:VSA262091 WBW196560:WBW262091 WLS196560:WLS262091 WVO196560:WVO262091 JC262096:JC327627 SY262096:SY327627 ACU262096:ACU327627 AMQ262096:AMQ327627 AWM262096:AWM327627 BGI262096:BGI327627 BQE262096:BQE327627 CAA262096:CAA327627 CJW262096:CJW327627 CTS262096:CTS327627 DDO262096:DDO327627 DNK262096:DNK327627 DXG262096:DXG327627 EHC262096:EHC327627 EQY262096:EQY327627 FAU262096:FAU327627 FKQ262096:FKQ327627 FUM262096:FUM327627 GEI262096:GEI327627 GOE262096:GOE327627 GYA262096:GYA327627 HHW262096:HHW327627 HRS262096:HRS327627 IBO262096:IBO327627 ILK262096:ILK327627 IVG262096:IVG327627 JFC262096:JFC327627 JOY262096:JOY327627 JYU262096:JYU327627 KIQ262096:KIQ327627 KSM262096:KSM327627 LCI262096:LCI327627 LME262096:LME327627 LWA262096:LWA327627 MFW262096:MFW327627 MPS262096:MPS327627 MZO262096:MZO327627 NJK262096:NJK327627 NTG262096:NTG327627 ODC262096:ODC327627 OMY262096:OMY327627 OWU262096:OWU327627 PGQ262096:PGQ327627 PQM262096:PQM327627 QAI262096:QAI327627 QKE262096:QKE327627 QUA262096:QUA327627 RDW262096:RDW327627 RNS262096:RNS327627 RXO262096:RXO327627 SHK262096:SHK327627 SRG262096:SRG327627 TBC262096:TBC327627 TKY262096:TKY327627 TUU262096:TUU327627 UEQ262096:UEQ327627 UOM262096:UOM327627 UYI262096:UYI327627 VIE262096:VIE327627 VSA262096:VSA327627 WBW262096:WBW327627 WLS262096:WLS327627 WVO262096:WVO327627 JC327632:JC393163 SY327632:SY393163 ACU327632:ACU393163 AMQ327632:AMQ393163 AWM327632:AWM393163 BGI327632:BGI393163 BQE327632:BQE393163 CAA327632:CAA393163 CJW327632:CJW393163 CTS327632:CTS393163 DDO327632:DDO393163 DNK327632:DNK393163 DXG327632:DXG393163 EHC327632:EHC393163 EQY327632:EQY393163 FAU327632:FAU393163 FKQ327632:FKQ393163 FUM327632:FUM393163 GEI327632:GEI393163 GOE327632:GOE393163 GYA327632:GYA393163 HHW327632:HHW393163 HRS327632:HRS393163 IBO327632:IBO393163 ILK327632:ILK393163 IVG327632:IVG393163 JFC327632:JFC393163 JOY327632:JOY393163 JYU327632:JYU393163 KIQ327632:KIQ393163 KSM327632:KSM393163 LCI327632:LCI393163 LME327632:LME393163 LWA327632:LWA393163 MFW327632:MFW393163 MPS327632:MPS393163 MZO327632:MZO393163 NJK327632:NJK393163 NTG327632:NTG393163 ODC327632:ODC393163 OMY327632:OMY393163 OWU327632:OWU393163 PGQ327632:PGQ393163 PQM327632:PQM393163 QAI327632:QAI393163 QKE327632:QKE393163 QUA327632:QUA393163 RDW327632:RDW393163 RNS327632:RNS393163 RXO327632:RXO393163 SHK327632:SHK393163 SRG327632:SRG393163 TBC327632:TBC393163 TKY327632:TKY393163 TUU327632:TUU393163 UEQ327632:UEQ393163 UOM327632:UOM393163 UYI327632:UYI393163 VIE327632:VIE393163 VSA327632:VSA393163 WBW327632:WBW393163 WLS327632:WLS393163 WVO327632:WVO393163 JC393168:JC458699 SY393168:SY458699 ACU393168:ACU458699 AMQ393168:AMQ458699 AWM393168:AWM458699 BGI393168:BGI458699 BQE393168:BQE458699 CAA393168:CAA458699 CJW393168:CJW458699 CTS393168:CTS458699 DDO393168:DDO458699 DNK393168:DNK458699 DXG393168:DXG458699 EHC393168:EHC458699 EQY393168:EQY458699 FAU393168:FAU458699 FKQ393168:FKQ458699 FUM393168:FUM458699 GEI393168:GEI458699 GOE393168:GOE458699 GYA393168:GYA458699 HHW393168:HHW458699 HRS393168:HRS458699 IBO393168:IBO458699 ILK393168:ILK458699 IVG393168:IVG458699 JFC393168:JFC458699 JOY393168:JOY458699 JYU393168:JYU458699 KIQ393168:KIQ458699 KSM393168:KSM458699 LCI393168:LCI458699 LME393168:LME458699 LWA393168:LWA458699 MFW393168:MFW458699 MPS393168:MPS458699 MZO393168:MZO458699 NJK393168:NJK458699 NTG393168:NTG458699 ODC393168:ODC458699 OMY393168:OMY458699 OWU393168:OWU458699 PGQ393168:PGQ458699 PQM393168:PQM458699 QAI393168:QAI458699 QKE393168:QKE458699 QUA393168:QUA458699 RDW393168:RDW458699 RNS393168:RNS458699 RXO393168:RXO458699 SHK393168:SHK458699 SRG393168:SRG458699 TBC393168:TBC458699 TKY393168:TKY458699 TUU393168:TUU458699 UEQ393168:UEQ458699 UOM393168:UOM458699 UYI393168:UYI458699 VIE393168:VIE458699 VSA393168:VSA458699 WBW393168:WBW458699 WLS393168:WLS458699 WVO393168:WVO458699 JC458704:JC524235 SY458704:SY524235 ACU458704:ACU524235 AMQ458704:AMQ524235 AWM458704:AWM524235 BGI458704:BGI524235 BQE458704:BQE524235 CAA458704:CAA524235 CJW458704:CJW524235 CTS458704:CTS524235 DDO458704:DDO524235 DNK458704:DNK524235 DXG458704:DXG524235 EHC458704:EHC524235 EQY458704:EQY524235 FAU458704:FAU524235 FKQ458704:FKQ524235 FUM458704:FUM524235 GEI458704:GEI524235 GOE458704:GOE524235 GYA458704:GYA524235 HHW458704:HHW524235 HRS458704:HRS524235 IBO458704:IBO524235 ILK458704:ILK524235 IVG458704:IVG524235 JFC458704:JFC524235 JOY458704:JOY524235 JYU458704:JYU524235 KIQ458704:KIQ524235 KSM458704:KSM524235 LCI458704:LCI524235 LME458704:LME524235 LWA458704:LWA524235 MFW458704:MFW524235 MPS458704:MPS524235 MZO458704:MZO524235 NJK458704:NJK524235 NTG458704:NTG524235 ODC458704:ODC524235 OMY458704:OMY524235 OWU458704:OWU524235 PGQ458704:PGQ524235 PQM458704:PQM524235 QAI458704:QAI524235 QKE458704:QKE524235 QUA458704:QUA524235 RDW458704:RDW524235 RNS458704:RNS524235 RXO458704:RXO524235 SHK458704:SHK524235 SRG458704:SRG524235 TBC458704:TBC524235 TKY458704:TKY524235 TUU458704:TUU524235 UEQ458704:UEQ524235 UOM458704:UOM524235 UYI458704:UYI524235 VIE458704:VIE524235 VSA458704:VSA524235 WBW458704:WBW524235 WLS458704:WLS524235 WVO458704:WVO524235 JC524240:JC589771 SY524240:SY589771 ACU524240:ACU589771 AMQ524240:AMQ589771 AWM524240:AWM589771 BGI524240:BGI589771 BQE524240:BQE589771 CAA524240:CAA589771 CJW524240:CJW589771 CTS524240:CTS589771 DDO524240:DDO589771 DNK524240:DNK589771 DXG524240:DXG589771 EHC524240:EHC589771 EQY524240:EQY589771 FAU524240:FAU589771 FKQ524240:FKQ589771 FUM524240:FUM589771 GEI524240:GEI589771 GOE524240:GOE589771 GYA524240:GYA589771 HHW524240:HHW589771 HRS524240:HRS589771 IBO524240:IBO589771 ILK524240:ILK589771 IVG524240:IVG589771 JFC524240:JFC589771 JOY524240:JOY589771 JYU524240:JYU589771 KIQ524240:KIQ589771 KSM524240:KSM589771 LCI524240:LCI589771 LME524240:LME589771 LWA524240:LWA589771 MFW524240:MFW589771 MPS524240:MPS589771 MZO524240:MZO589771 NJK524240:NJK589771 NTG524240:NTG589771 ODC524240:ODC589771 OMY524240:OMY589771 OWU524240:OWU589771 PGQ524240:PGQ589771 PQM524240:PQM589771 QAI524240:QAI589771 QKE524240:QKE589771 QUA524240:QUA589771 RDW524240:RDW589771 RNS524240:RNS589771 RXO524240:RXO589771 SHK524240:SHK589771 SRG524240:SRG589771 TBC524240:TBC589771 TKY524240:TKY589771 TUU524240:TUU589771 UEQ524240:UEQ589771 UOM524240:UOM589771 UYI524240:UYI589771 VIE524240:VIE589771 VSA524240:VSA589771 WBW524240:WBW589771 WLS524240:WLS589771 WVO524240:WVO589771 JC589776:JC655307 SY589776:SY655307 ACU589776:ACU655307 AMQ589776:AMQ655307 AWM589776:AWM655307 BGI589776:BGI655307 BQE589776:BQE655307 CAA589776:CAA655307 CJW589776:CJW655307 CTS589776:CTS655307 DDO589776:DDO655307 DNK589776:DNK655307 DXG589776:DXG655307 EHC589776:EHC655307 EQY589776:EQY655307 FAU589776:FAU655307 FKQ589776:FKQ655307 FUM589776:FUM655307 GEI589776:GEI655307 GOE589776:GOE655307 GYA589776:GYA655307 HHW589776:HHW655307 HRS589776:HRS655307 IBO589776:IBO655307 ILK589776:ILK655307 IVG589776:IVG655307 JFC589776:JFC655307 JOY589776:JOY655307 JYU589776:JYU655307 KIQ589776:KIQ655307 KSM589776:KSM655307 LCI589776:LCI655307 LME589776:LME655307 LWA589776:LWA655307 MFW589776:MFW655307 MPS589776:MPS655307 MZO589776:MZO655307 NJK589776:NJK655307 NTG589776:NTG655307 ODC589776:ODC655307 OMY589776:OMY655307 OWU589776:OWU655307 PGQ589776:PGQ655307 PQM589776:PQM655307 QAI589776:QAI655307 QKE589776:QKE655307 QUA589776:QUA655307 RDW589776:RDW655307 RNS589776:RNS655307 RXO589776:RXO655307 SHK589776:SHK655307 SRG589776:SRG655307 TBC589776:TBC655307 TKY589776:TKY655307 TUU589776:TUU655307 UEQ589776:UEQ655307 UOM589776:UOM655307 UYI589776:UYI655307 VIE589776:VIE655307 VSA589776:VSA655307 WBW589776:WBW655307 WLS589776:WLS655307 WVO589776:WVO655307 JC655312:JC720843 SY655312:SY720843 ACU655312:ACU720843 AMQ655312:AMQ720843 AWM655312:AWM720843 BGI655312:BGI720843 BQE655312:BQE720843 CAA655312:CAA720843 CJW655312:CJW720843 CTS655312:CTS720843 DDO655312:DDO720843 DNK655312:DNK720843 DXG655312:DXG720843 EHC655312:EHC720843 EQY655312:EQY720843 FAU655312:FAU720843 FKQ655312:FKQ720843 FUM655312:FUM720843 GEI655312:GEI720843 GOE655312:GOE720843 GYA655312:GYA720843 HHW655312:HHW720843 HRS655312:HRS720843 IBO655312:IBO720843 ILK655312:ILK720843 IVG655312:IVG720843 JFC655312:JFC720843 JOY655312:JOY720843 JYU655312:JYU720843 KIQ655312:KIQ720843 KSM655312:KSM720843 LCI655312:LCI720843 LME655312:LME720843 LWA655312:LWA720843 MFW655312:MFW720843 MPS655312:MPS720843 MZO655312:MZO720843 NJK655312:NJK720843 NTG655312:NTG720843 ODC655312:ODC720843 OMY655312:OMY720843 OWU655312:OWU720843 PGQ655312:PGQ720843 PQM655312:PQM720843 QAI655312:QAI720843 QKE655312:QKE720843 QUA655312:QUA720843 RDW655312:RDW720843 RNS655312:RNS720843 RXO655312:RXO720843 SHK655312:SHK720843 SRG655312:SRG720843 TBC655312:TBC720843 TKY655312:TKY720843 TUU655312:TUU720843 UEQ655312:UEQ720843 UOM655312:UOM720843 UYI655312:UYI720843 VIE655312:VIE720843 VSA655312:VSA720843 WBW655312:WBW720843 WLS655312:WLS720843 WVO655312:WVO720843 JC720848:JC786379 SY720848:SY786379 ACU720848:ACU786379 AMQ720848:AMQ786379 AWM720848:AWM786379 BGI720848:BGI786379 BQE720848:BQE786379 CAA720848:CAA786379 CJW720848:CJW786379 CTS720848:CTS786379 DDO720848:DDO786379 DNK720848:DNK786379 DXG720848:DXG786379 EHC720848:EHC786379 EQY720848:EQY786379 FAU720848:FAU786379 FKQ720848:FKQ786379 FUM720848:FUM786379 GEI720848:GEI786379 GOE720848:GOE786379 GYA720848:GYA786379 HHW720848:HHW786379 HRS720848:HRS786379 IBO720848:IBO786379 ILK720848:ILK786379 IVG720848:IVG786379 JFC720848:JFC786379 JOY720848:JOY786379 JYU720848:JYU786379 KIQ720848:KIQ786379 KSM720848:KSM786379 LCI720848:LCI786379 LME720848:LME786379 LWA720848:LWA786379 MFW720848:MFW786379 MPS720848:MPS786379 MZO720848:MZO786379 NJK720848:NJK786379 NTG720848:NTG786379 ODC720848:ODC786379 OMY720848:OMY786379 OWU720848:OWU786379 PGQ720848:PGQ786379 PQM720848:PQM786379 QAI720848:QAI786379 QKE720848:QKE786379 QUA720848:QUA786379 RDW720848:RDW786379 RNS720848:RNS786379 RXO720848:RXO786379 SHK720848:SHK786379 SRG720848:SRG786379 TBC720848:TBC786379 TKY720848:TKY786379 TUU720848:TUU786379 UEQ720848:UEQ786379 UOM720848:UOM786379 UYI720848:UYI786379 VIE720848:VIE786379 VSA720848:VSA786379 WBW720848:WBW786379 WLS720848:WLS786379 WVO720848:WVO786379 JC786384:JC851915 SY786384:SY851915 ACU786384:ACU851915 AMQ786384:AMQ851915 AWM786384:AWM851915 BGI786384:BGI851915 BQE786384:BQE851915 CAA786384:CAA851915 CJW786384:CJW851915 CTS786384:CTS851915 DDO786384:DDO851915 DNK786384:DNK851915 DXG786384:DXG851915 EHC786384:EHC851915 EQY786384:EQY851915 FAU786384:FAU851915 FKQ786384:FKQ851915 FUM786384:FUM851915 GEI786384:GEI851915 GOE786384:GOE851915 GYA786384:GYA851915 HHW786384:HHW851915 HRS786384:HRS851915 IBO786384:IBO851915 ILK786384:ILK851915 IVG786384:IVG851915 JFC786384:JFC851915 JOY786384:JOY851915 JYU786384:JYU851915 KIQ786384:KIQ851915 KSM786384:KSM851915 LCI786384:LCI851915 LME786384:LME851915 LWA786384:LWA851915 MFW786384:MFW851915 MPS786384:MPS851915 MZO786384:MZO851915 NJK786384:NJK851915 NTG786384:NTG851915 ODC786384:ODC851915 OMY786384:OMY851915 OWU786384:OWU851915 PGQ786384:PGQ851915 PQM786384:PQM851915 QAI786384:QAI851915 QKE786384:QKE851915 QUA786384:QUA851915 RDW786384:RDW851915 RNS786384:RNS851915 RXO786384:RXO851915 SHK786384:SHK851915 SRG786384:SRG851915 TBC786384:TBC851915 TKY786384:TKY851915 TUU786384:TUU851915 UEQ786384:UEQ851915 UOM786384:UOM851915 UYI786384:UYI851915 VIE786384:VIE851915 VSA786384:VSA851915 WBW786384:WBW851915 WLS786384:WLS851915 WVO786384:WVO851915 JC851920:JC917451 SY851920:SY917451 ACU851920:ACU917451 AMQ851920:AMQ917451 AWM851920:AWM917451 BGI851920:BGI917451 BQE851920:BQE917451 CAA851920:CAA917451 CJW851920:CJW917451 CTS851920:CTS917451 DDO851920:DDO917451 DNK851920:DNK917451 DXG851920:DXG917451 EHC851920:EHC917451 EQY851920:EQY917451 FAU851920:FAU917451 FKQ851920:FKQ917451 FUM851920:FUM917451 GEI851920:GEI917451 GOE851920:GOE917451 GYA851920:GYA917451 HHW851920:HHW917451 HRS851920:HRS917451 IBO851920:IBO917451 ILK851920:ILK917451 IVG851920:IVG917451 JFC851920:JFC917451 JOY851920:JOY917451 JYU851920:JYU917451 KIQ851920:KIQ917451 KSM851920:KSM917451 LCI851920:LCI917451 LME851920:LME917451 LWA851920:LWA917451 MFW851920:MFW917451 MPS851920:MPS917451 MZO851920:MZO917451 NJK851920:NJK917451 NTG851920:NTG917451 ODC851920:ODC917451 OMY851920:OMY917451 OWU851920:OWU917451 PGQ851920:PGQ917451 PQM851920:PQM917451 QAI851920:QAI917451 QKE851920:QKE917451 QUA851920:QUA917451 RDW851920:RDW917451 RNS851920:RNS917451 RXO851920:RXO917451 SHK851920:SHK917451 SRG851920:SRG917451 TBC851920:TBC917451 TKY851920:TKY917451 TUU851920:TUU917451 UEQ851920:UEQ917451 UOM851920:UOM917451 UYI851920:UYI917451 VIE851920:VIE917451 VSA851920:VSA917451 WBW851920:WBW917451 WLS851920:WLS917451 WVO851920:WVO917451 JC917456:JC982987 SY917456:SY982987 ACU917456:ACU982987 AMQ917456:AMQ982987 AWM917456:AWM982987 BGI917456:BGI982987 BQE917456:BQE982987 CAA917456:CAA982987 CJW917456:CJW982987 CTS917456:CTS982987 DDO917456:DDO982987 DNK917456:DNK982987 DXG917456:DXG982987 EHC917456:EHC982987 EQY917456:EQY982987 FAU917456:FAU982987 FKQ917456:FKQ982987 FUM917456:FUM982987 GEI917456:GEI982987 GOE917456:GOE982987 GYA917456:GYA982987 HHW917456:HHW982987 HRS917456:HRS982987 IBO917456:IBO982987 ILK917456:ILK982987 IVG917456:IVG982987 JFC917456:JFC982987 JOY917456:JOY982987 JYU917456:JYU982987 KIQ917456:KIQ982987 KSM917456:KSM982987 LCI917456:LCI982987 LME917456:LME982987 LWA917456:LWA982987 MFW917456:MFW982987 MPS917456:MPS982987 MZO917456:MZO982987 NJK917456:NJK982987 NTG917456:NTG982987 ODC917456:ODC982987 OMY917456:OMY982987 OWU917456:OWU982987 PGQ917456:PGQ982987 PQM917456:PQM982987 QAI917456:QAI982987 QKE917456:QKE982987 QUA917456:QUA982987 RDW917456:RDW982987 RNS917456:RNS982987 RXO917456:RXO982987 SHK917456:SHK982987 SRG917456:SRG982987 TBC917456:TBC982987 TKY917456:TKY982987 TUU917456:TUU982987 UEQ917456:UEQ982987 UOM917456:UOM982987 UYI917456:UYI982987 VIE917456:VIE982987 VSA917456:VSA982987 WBW917456:WBW982987 WLS917456:WLS982987 WVO917456:WVO982987 JC982992:JC1048576 SY982992:SY1048576 ACU982992:ACU1048576 AMQ982992:AMQ1048576 AWM982992:AWM1048576 BGI982992:BGI1048576 BQE982992:BQE1048576 CAA982992:CAA1048576 CJW982992:CJW1048576 CTS982992:CTS1048576 DDO982992:DDO1048576 DNK982992:DNK1048576 DXG982992:DXG1048576 EHC982992:EHC1048576 EQY982992:EQY1048576 FAU982992:FAU1048576 FKQ982992:FKQ1048576 FUM982992:FUM1048576 GEI982992:GEI1048576 GOE982992:GOE1048576 GYA982992:GYA1048576 HHW982992:HHW1048576 HRS982992:HRS1048576 IBO982992:IBO1048576 ILK982992:ILK1048576 IVG982992:IVG1048576 JFC982992:JFC1048576 JOY982992:JOY1048576 JYU982992:JYU1048576 KIQ982992:KIQ1048576 KSM982992:KSM1048576 LCI982992:LCI1048576 LME982992:LME1048576 LWA982992:LWA1048576 MFW982992:MFW1048576 MPS982992:MPS1048576 MZO982992:MZO1048576 NJK982992:NJK1048576 NTG982992:NTG1048576 ODC982992:ODC1048576 OMY982992:OMY1048576 OWU982992:OWU1048576 PGQ982992:PGQ1048576 PQM982992:PQM1048576 QAI982992:QAI1048576 QKE982992:QKE1048576 QUA982992:QUA1048576 RDW982992:RDW1048576 RNS982992:RNS1048576 RXO982992:RXO1048576 SHK982992:SHK1048576 SRG982992:SRG1048576 TBC982992:TBC1048576 TKY982992:TKY1048576 TUU982992:TUU1048576 UEQ982992:UEQ1048576 UOM982992:UOM1048576 UYI982992:UYI1048576 VIE982992:VIE1048576 VSA982992:VSA1048576 WBW982992:WBW1048576 WLS982992:WLS1048576 JC5:JC65483 SY5:SY65483 ACU5:ACU65483 AMQ5:AMQ65483 AWM5:AWM65483 BGI5:BGI65483 BQE5:BQE65483 CAA5:CAA65483 CJW5:CJW65483 CTS5:CTS65483 DDO5:DDO65483 DNK5:DNK65483 DXG5:DXG65483 EHC5:EHC65483 EQY5:EQY65483 FAU5:FAU65483 FKQ5:FKQ65483 FUM5:FUM65483 GEI5:GEI65483 GOE5:GOE65483 GYA5:GYA65483 HHW5:HHW65483 HRS5:HRS65483 IBO5:IBO65483 ILK5:ILK65483 IVG5:IVG65483 JFC5:JFC65483 JOY5:JOY65483 JYU5:JYU65483 KIQ5:KIQ65483 KSM5:KSM65483 LCI5:LCI65483 LME5:LME65483 LWA5:LWA65483 MFW5:MFW65483 MPS5:MPS65483 MZO5:MZO65483 NJK5:NJK65483 NTG5:NTG65483 ODC5:ODC65483 OMY5:OMY65483 OWU5:OWU65483 PGQ5:PGQ65483 PQM5:PQM65483 QAI5:QAI65483 QKE5:QKE65483 QUA5:QUA65483 RDW5:RDW65483 RNS5:RNS65483 RXO5:RXO65483 SHK5:SHK65483 SRG5:SRG65483 TBC5:TBC65483 TKY5:TKY65483 TUU5:TUU65483 UEQ5:UEQ65483 UOM5:UOM65483 UYI5:UYI65483 VIE5:VIE65483 VSA5:VSA65483 WBW5:WBW65483 WLS5:WLS65483 WVO5:WVO65483">
       <formula1>".,~"</formula1>
     </dataValidation>
-    <dataValidation type="list" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVP983045:WVP1048576 JD5:JD65536 SZ5:SZ65536 ACV5:ACV65536 AMR5:AMR65536 AWN5:AWN65536 BGJ5:BGJ65536 BQF5:BQF65536 CAB5:CAB65536 CJX5:CJX65536 CTT5:CTT65536 DDP5:DDP65536 DNL5:DNL65536 DXH5:DXH65536 EHD5:EHD65536 EQZ5:EQZ65536 FAV5:FAV65536 FKR5:FKR65536 FUN5:FUN65536 GEJ5:GEJ65536 GOF5:GOF65536 GYB5:GYB65536 HHX5:HHX65536 HRT5:HRT65536 IBP5:IBP65536 ILL5:ILL65536 IVH5:IVH65536 JFD5:JFD65536 JOZ5:JOZ65536 JYV5:JYV65536 KIR5:KIR65536 KSN5:KSN65536 LCJ5:LCJ65536 LMF5:LMF65536 LWB5:LWB65536 MFX5:MFX65536 MPT5:MPT65536 MZP5:MZP65536 NJL5:NJL65536 NTH5:NTH65536 ODD5:ODD65536 OMZ5:OMZ65536 OWV5:OWV65536 PGR5:PGR65536 PQN5:PQN65536 QAJ5:QAJ65536 QKF5:QKF65536 QUB5:QUB65536 RDX5:RDX65536 RNT5:RNT65536 RXP5:RXP65536 SHL5:SHL65536 SRH5:SRH65536 TBD5:TBD65536 TKZ5:TKZ65536 TUV5:TUV65536 UER5:UER65536 UON5:UON65536 UYJ5:UYJ65536 VIF5:VIF65536 VSB5:VSB65536 WBX5:WBX65536 WLT5:WLT65536 WVP5:WVP65536 JD65541:JD131072 SZ65541:SZ131072 ACV65541:ACV131072 AMR65541:AMR131072 AWN65541:AWN131072 BGJ65541:BGJ131072 BQF65541:BQF131072 CAB65541:CAB131072 CJX65541:CJX131072 CTT65541:CTT131072 DDP65541:DDP131072 DNL65541:DNL131072 DXH65541:DXH131072 EHD65541:EHD131072 EQZ65541:EQZ131072 FAV65541:FAV131072 FKR65541:FKR131072 FUN65541:FUN131072 GEJ65541:GEJ131072 GOF65541:GOF131072 GYB65541:GYB131072 HHX65541:HHX131072 HRT65541:HRT131072 IBP65541:IBP131072 ILL65541:ILL131072 IVH65541:IVH131072 JFD65541:JFD131072 JOZ65541:JOZ131072 JYV65541:JYV131072 KIR65541:KIR131072 KSN65541:KSN131072 LCJ65541:LCJ131072 LMF65541:LMF131072 LWB65541:LWB131072 MFX65541:MFX131072 MPT65541:MPT131072 MZP65541:MZP131072 NJL65541:NJL131072 NTH65541:NTH131072 ODD65541:ODD131072 OMZ65541:OMZ131072 OWV65541:OWV131072 PGR65541:PGR131072 PQN65541:PQN131072 QAJ65541:QAJ131072 QKF65541:QKF131072 QUB65541:QUB131072 RDX65541:RDX131072 RNT65541:RNT131072 RXP65541:RXP131072 SHL65541:SHL131072 SRH65541:SRH131072 TBD65541:TBD131072 TKZ65541:TKZ131072 TUV65541:TUV131072 UER65541:UER131072 UON65541:UON131072 UYJ65541:UYJ131072 VIF65541:VIF131072 VSB65541:VSB131072 WBX65541:WBX131072 WLT65541:WLT131072 WVP65541:WVP131072 JD131077:JD196608 SZ131077:SZ196608 ACV131077:ACV196608 AMR131077:AMR196608 AWN131077:AWN196608 BGJ131077:BGJ196608 BQF131077:BQF196608 CAB131077:CAB196608 CJX131077:CJX196608 CTT131077:CTT196608 DDP131077:DDP196608 DNL131077:DNL196608 DXH131077:DXH196608 EHD131077:EHD196608 EQZ131077:EQZ196608 FAV131077:FAV196608 FKR131077:FKR196608 FUN131077:FUN196608 GEJ131077:GEJ196608 GOF131077:GOF196608 GYB131077:GYB196608 HHX131077:HHX196608 HRT131077:HRT196608 IBP131077:IBP196608 ILL131077:ILL196608 IVH131077:IVH196608 JFD131077:JFD196608 JOZ131077:JOZ196608 JYV131077:JYV196608 KIR131077:KIR196608 KSN131077:KSN196608 LCJ131077:LCJ196608 LMF131077:LMF196608 LWB131077:LWB196608 MFX131077:MFX196608 MPT131077:MPT196608 MZP131077:MZP196608 NJL131077:NJL196608 NTH131077:NTH196608 ODD131077:ODD196608 OMZ131077:OMZ196608 OWV131077:OWV196608 PGR131077:PGR196608 PQN131077:PQN196608 QAJ131077:QAJ196608 QKF131077:QKF196608 QUB131077:QUB196608 RDX131077:RDX196608 RNT131077:RNT196608 RXP131077:RXP196608 SHL131077:SHL196608 SRH131077:SRH196608 TBD131077:TBD196608 TKZ131077:TKZ196608 TUV131077:TUV196608 UER131077:UER196608 UON131077:UON196608 UYJ131077:UYJ196608 VIF131077:VIF196608 VSB131077:VSB196608 WBX131077:WBX196608 WLT131077:WLT196608 WVP131077:WVP196608 JD196613:JD262144 SZ196613:SZ262144 ACV196613:ACV262144 AMR196613:AMR262144 AWN196613:AWN262144 BGJ196613:BGJ262144 BQF196613:BQF262144 CAB196613:CAB262144 CJX196613:CJX262144 CTT196613:CTT262144 DDP196613:DDP262144 DNL196613:DNL262144 DXH196613:DXH262144 EHD196613:EHD262144 EQZ196613:EQZ262144 FAV196613:FAV262144 FKR196613:FKR262144 FUN196613:FUN262144 GEJ196613:GEJ262144 GOF196613:GOF262144 GYB196613:GYB262144 HHX196613:HHX262144 HRT196613:HRT262144 IBP196613:IBP262144 ILL196613:ILL262144 IVH196613:IVH262144 JFD196613:JFD262144 JOZ196613:JOZ262144 JYV196613:JYV262144 KIR196613:KIR262144 KSN196613:KSN262144 LCJ196613:LCJ262144 LMF196613:LMF262144 LWB196613:LWB262144 MFX196613:MFX262144 MPT196613:MPT262144 MZP196613:MZP262144 NJL196613:NJL262144 NTH196613:NTH262144 ODD196613:ODD262144 OMZ196613:OMZ262144 OWV196613:OWV262144 PGR196613:PGR262144 PQN196613:PQN262144 QAJ196613:QAJ262144 QKF196613:QKF262144 QUB196613:QUB262144 RDX196613:RDX262144 RNT196613:RNT262144 RXP196613:RXP262144 SHL196613:SHL262144 SRH196613:SRH262144 TBD196613:TBD262144 TKZ196613:TKZ262144 TUV196613:TUV262144 UER196613:UER262144 UON196613:UON262144 UYJ196613:UYJ262144 VIF196613:VIF262144 VSB196613:VSB262144 WBX196613:WBX262144 WLT196613:WLT262144 WVP196613:WVP262144 JD262149:JD327680 SZ262149:SZ327680 ACV262149:ACV327680 AMR262149:AMR327680 AWN262149:AWN327680 BGJ262149:BGJ327680 BQF262149:BQF327680 CAB262149:CAB327680 CJX262149:CJX327680 CTT262149:CTT327680 DDP262149:DDP327680 DNL262149:DNL327680 DXH262149:DXH327680 EHD262149:EHD327680 EQZ262149:EQZ327680 FAV262149:FAV327680 FKR262149:FKR327680 FUN262149:FUN327680 GEJ262149:GEJ327680 GOF262149:GOF327680 GYB262149:GYB327680 HHX262149:HHX327680 HRT262149:HRT327680 IBP262149:IBP327680 ILL262149:ILL327680 IVH262149:IVH327680 JFD262149:JFD327680 JOZ262149:JOZ327680 JYV262149:JYV327680 KIR262149:KIR327680 KSN262149:KSN327680 LCJ262149:LCJ327680 LMF262149:LMF327680 LWB262149:LWB327680 MFX262149:MFX327680 MPT262149:MPT327680 MZP262149:MZP327680 NJL262149:NJL327680 NTH262149:NTH327680 ODD262149:ODD327680 OMZ262149:OMZ327680 OWV262149:OWV327680 PGR262149:PGR327680 PQN262149:PQN327680 QAJ262149:QAJ327680 QKF262149:QKF327680 QUB262149:QUB327680 RDX262149:RDX327680 RNT262149:RNT327680 RXP262149:RXP327680 SHL262149:SHL327680 SRH262149:SRH327680 TBD262149:TBD327680 TKZ262149:TKZ327680 TUV262149:TUV327680 UER262149:UER327680 UON262149:UON327680 UYJ262149:UYJ327680 VIF262149:VIF327680 VSB262149:VSB327680 WBX262149:WBX327680 WLT262149:WLT327680 WVP262149:WVP327680 JD327685:JD393216 SZ327685:SZ393216 ACV327685:ACV393216 AMR327685:AMR393216 AWN327685:AWN393216 BGJ327685:BGJ393216 BQF327685:BQF393216 CAB327685:CAB393216 CJX327685:CJX393216 CTT327685:CTT393216 DDP327685:DDP393216 DNL327685:DNL393216 DXH327685:DXH393216 EHD327685:EHD393216 EQZ327685:EQZ393216 FAV327685:FAV393216 FKR327685:FKR393216 FUN327685:FUN393216 GEJ327685:GEJ393216 GOF327685:GOF393216 GYB327685:GYB393216 HHX327685:HHX393216 HRT327685:HRT393216 IBP327685:IBP393216 ILL327685:ILL393216 IVH327685:IVH393216 JFD327685:JFD393216 JOZ327685:JOZ393216 JYV327685:JYV393216 KIR327685:KIR393216 KSN327685:KSN393216 LCJ327685:LCJ393216 LMF327685:LMF393216 LWB327685:LWB393216 MFX327685:MFX393216 MPT327685:MPT393216 MZP327685:MZP393216 NJL327685:NJL393216 NTH327685:NTH393216 ODD327685:ODD393216 OMZ327685:OMZ393216 OWV327685:OWV393216 PGR327685:PGR393216 PQN327685:PQN393216 QAJ327685:QAJ393216 QKF327685:QKF393216 QUB327685:QUB393216 RDX327685:RDX393216 RNT327685:RNT393216 RXP327685:RXP393216 SHL327685:SHL393216 SRH327685:SRH393216 TBD327685:TBD393216 TKZ327685:TKZ393216 TUV327685:TUV393216 UER327685:UER393216 UON327685:UON393216 UYJ327685:UYJ393216 VIF327685:VIF393216 VSB327685:VSB393216 WBX327685:WBX393216 WLT327685:WLT393216 WVP327685:WVP393216 JD393221:JD458752 SZ393221:SZ458752 ACV393221:ACV458752 AMR393221:AMR458752 AWN393221:AWN458752 BGJ393221:BGJ458752 BQF393221:BQF458752 CAB393221:CAB458752 CJX393221:CJX458752 CTT393221:CTT458752 DDP393221:DDP458752 DNL393221:DNL458752 DXH393221:DXH458752 EHD393221:EHD458752 EQZ393221:EQZ458752 FAV393221:FAV458752 FKR393221:FKR458752 FUN393221:FUN458752 GEJ393221:GEJ458752 GOF393221:GOF458752 GYB393221:GYB458752 HHX393221:HHX458752 HRT393221:HRT458752 IBP393221:IBP458752 ILL393221:ILL458752 IVH393221:IVH458752 JFD393221:JFD458752 JOZ393221:JOZ458752 JYV393221:JYV458752 KIR393221:KIR458752 KSN393221:KSN458752 LCJ393221:LCJ458752 LMF393221:LMF458752 LWB393221:LWB458752 MFX393221:MFX458752 MPT393221:MPT458752 MZP393221:MZP458752 NJL393221:NJL458752 NTH393221:NTH458752 ODD393221:ODD458752 OMZ393221:OMZ458752 OWV393221:OWV458752 PGR393221:PGR458752 PQN393221:PQN458752 QAJ393221:QAJ458752 QKF393221:QKF458752 QUB393221:QUB458752 RDX393221:RDX458752 RNT393221:RNT458752 RXP393221:RXP458752 SHL393221:SHL458752 SRH393221:SRH458752 TBD393221:TBD458752 TKZ393221:TKZ458752 TUV393221:TUV458752 UER393221:UER458752 UON393221:UON458752 UYJ393221:UYJ458752 VIF393221:VIF458752 VSB393221:VSB458752 WBX393221:WBX458752 WLT393221:WLT458752 WVP393221:WVP458752 JD458757:JD524288 SZ458757:SZ524288 ACV458757:ACV524288 AMR458757:AMR524288 AWN458757:AWN524288 BGJ458757:BGJ524288 BQF458757:BQF524288 CAB458757:CAB524288 CJX458757:CJX524288 CTT458757:CTT524288 DDP458757:DDP524288 DNL458757:DNL524288 DXH458757:DXH524288 EHD458757:EHD524288 EQZ458757:EQZ524288 FAV458757:FAV524288 FKR458757:FKR524288 FUN458757:FUN524288 GEJ458757:GEJ524288 GOF458757:GOF524288 GYB458757:GYB524288 HHX458757:HHX524288 HRT458757:HRT524288 IBP458757:IBP524288 ILL458757:ILL524288 IVH458757:IVH524288 JFD458757:JFD524288 JOZ458757:JOZ524288 JYV458757:JYV524288 KIR458757:KIR524288 KSN458757:KSN524288 LCJ458757:LCJ524288 LMF458757:LMF524288 LWB458757:LWB524288 MFX458757:MFX524288 MPT458757:MPT524288 MZP458757:MZP524288 NJL458757:NJL524288 NTH458757:NTH524288 ODD458757:ODD524288 OMZ458757:OMZ524288 OWV458757:OWV524288 PGR458757:PGR524288 PQN458757:PQN524288 QAJ458757:QAJ524288 QKF458757:QKF524288 QUB458757:QUB524288 RDX458757:RDX524288 RNT458757:RNT524288 RXP458757:RXP524288 SHL458757:SHL524288 SRH458757:SRH524288 TBD458757:TBD524288 TKZ458757:TKZ524288 TUV458757:TUV524288 UER458757:UER524288 UON458757:UON524288 UYJ458757:UYJ524288 VIF458757:VIF524288 VSB458757:VSB524288 WBX458757:WBX524288 WLT458757:WLT524288 WVP458757:WVP524288 JD524293:JD589824 SZ524293:SZ589824 ACV524293:ACV589824 AMR524293:AMR589824 AWN524293:AWN589824 BGJ524293:BGJ589824 BQF524293:BQF589824 CAB524293:CAB589824 CJX524293:CJX589824 CTT524293:CTT589824 DDP524293:DDP589824 DNL524293:DNL589824 DXH524293:DXH589824 EHD524293:EHD589824 EQZ524293:EQZ589824 FAV524293:FAV589824 FKR524293:FKR589824 FUN524293:FUN589824 GEJ524293:GEJ589824 GOF524293:GOF589824 GYB524293:GYB589824 HHX524293:HHX589824 HRT524293:HRT589824 IBP524293:IBP589824 ILL524293:ILL589824 IVH524293:IVH589824 JFD524293:JFD589824 JOZ524293:JOZ589824 JYV524293:JYV589824 KIR524293:KIR589824 KSN524293:KSN589824 LCJ524293:LCJ589824 LMF524293:LMF589824 LWB524293:LWB589824 MFX524293:MFX589824 MPT524293:MPT589824 MZP524293:MZP589824 NJL524293:NJL589824 NTH524293:NTH589824 ODD524293:ODD589824 OMZ524293:OMZ589824 OWV524293:OWV589824 PGR524293:PGR589824 PQN524293:PQN589824 QAJ524293:QAJ589824 QKF524293:QKF589824 QUB524293:QUB589824 RDX524293:RDX589824 RNT524293:RNT589824 RXP524293:RXP589824 SHL524293:SHL589824 SRH524293:SRH589824 TBD524293:TBD589824 TKZ524293:TKZ589824 TUV524293:TUV589824 UER524293:UER589824 UON524293:UON589824 UYJ524293:UYJ589824 VIF524293:VIF589824 VSB524293:VSB589824 WBX524293:WBX589824 WLT524293:WLT589824 WVP524293:WVP589824 JD589829:JD655360 SZ589829:SZ655360 ACV589829:ACV655360 AMR589829:AMR655360 AWN589829:AWN655360 BGJ589829:BGJ655360 BQF589829:BQF655360 CAB589829:CAB655360 CJX589829:CJX655360 CTT589829:CTT655360 DDP589829:DDP655360 DNL589829:DNL655360 DXH589829:DXH655360 EHD589829:EHD655360 EQZ589829:EQZ655360 FAV589829:FAV655360 FKR589829:FKR655360 FUN589829:FUN655360 GEJ589829:GEJ655360 GOF589829:GOF655360 GYB589829:GYB655360 HHX589829:HHX655360 HRT589829:HRT655360 IBP589829:IBP655360 ILL589829:ILL655360 IVH589829:IVH655360 JFD589829:JFD655360 JOZ589829:JOZ655360 JYV589829:JYV655360 KIR589829:KIR655360 KSN589829:KSN655360 LCJ589829:LCJ655360 LMF589829:LMF655360 LWB589829:LWB655360 MFX589829:MFX655360 MPT589829:MPT655360 MZP589829:MZP655360 NJL589829:NJL655360 NTH589829:NTH655360 ODD589829:ODD655360 OMZ589829:OMZ655360 OWV589829:OWV655360 PGR589829:PGR655360 PQN589829:PQN655360 QAJ589829:QAJ655360 QKF589829:QKF655360 QUB589829:QUB655360 RDX589829:RDX655360 RNT589829:RNT655360 RXP589829:RXP655360 SHL589829:SHL655360 SRH589829:SRH655360 TBD589829:TBD655360 TKZ589829:TKZ655360 TUV589829:TUV655360 UER589829:UER655360 UON589829:UON655360 UYJ589829:UYJ655360 VIF589829:VIF655360 VSB589829:VSB655360 WBX589829:WBX655360 WLT589829:WLT655360 WVP589829:WVP655360 JD655365:JD720896 SZ655365:SZ720896 ACV655365:ACV720896 AMR655365:AMR720896 AWN655365:AWN720896 BGJ655365:BGJ720896 BQF655365:BQF720896 CAB655365:CAB720896 CJX655365:CJX720896 CTT655365:CTT720896 DDP655365:DDP720896 DNL655365:DNL720896 DXH655365:DXH720896 EHD655365:EHD720896 EQZ655365:EQZ720896 FAV655365:FAV720896 FKR655365:FKR720896 FUN655365:FUN720896 GEJ655365:GEJ720896 GOF655365:GOF720896 GYB655365:GYB720896 HHX655365:HHX720896 HRT655365:HRT720896 IBP655365:IBP720896 ILL655365:ILL720896 IVH655365:IVH720896 JFD655365:JFD720896 JOZ655365:JOZ720896 JYV655365:JYV720896 KIR655365:KIR720896 KSN655365:KSN720896 LCJ655365:LCJ720896 LMF655365:LMF720896 LWB655365:LWB720896 MFX655365:MFX720896 MPT655365:MPT720896 MZP655365:MZP720896 NJL655365:NJL720896 NTH655365:NTH720896 ODD655365:ODD720896 OMZ655365:OMZ720896 OWV655365:OWV720896 PGR655365:PGR720896 PQN655365:PQN720896 QAJ655365:QAJ720896 QKF655365:QKF720896 QUB655365:QUB720896 RDX655365:RDX720896 RNT655365:RNT720896 RXP655365:RXP720896 SHL655365:SHL720896 SRH655365:SRH720896 TBD655365:TBD720896 TKZ655365:TKZ720896 TUV655365:TUV720896 UER655365:UER720896 UON655365:UON720896 UYJ655365:UYJ720896 VIF655365:VIF720896 VSB655365:VSB720896 WBX655365:WBX720896 WLT655365:WLT720896 WVP655365:WVP720896 JD720901:JD786432 SZ720901:SZ786432 ACV720901:ACV786432 AMR720901:AMR786432 AWN720901:AWN786432 BGJ720901:BGJ786432 BQF720901:BQF786432 CAB720901:CAB786432 CJX720901:CJX786432 CTT720901:CTT786432 DDP720901:DDP786432 DNL720901:DNL786432 DXH720901:DXH786432 EHD720901:EHD786432 EQZ720901:EQZ786432 FAV720901:FAV786432 FKR720901:FKR786432 FUN720901:FUN786432 GEJ720901:GEJ786432 GOF720901:GOF786432 GYB720901:GYB786432 HHX720901:HHX786432 HRT720901:HRT786432 IBP720901:IBP786432 ILL720901:ILL786432 IVH720901:IVH786432 JFD720901:JFD786432 JOZ720901:JOZ786432 JYV720901:JYV786432 KIR720901:KIR786432 KSN720901:KSN786432 LCJ720901:LCJ786432 LMF720901:LMF786432 LWB720901:LWB786432 MFX720901:MFX786432 MPT720901:MPT786432 MZP720901:MZP786432 NJL720901:NJL786432 NTH720901:NTH786432 ODD720901:ODD786432 OMZ720901:OMZ786432 OWV720901:OWV786432 PGR720901:PGR786432 PQN720901:PQN786432 QAJ720901:QAJ786432 QKF720901:QKF786432 QUB720901:QUB786432 RDX720901:RDX786432 RNT720901:RNT786432 RXP720901:RXP786432 SHL720901:SHL786432 SRH720901:SRH786432 TBD720901:TBD786432 TKZ720901:TKZ786432 TUV720901:TUV786432 UER720901:UER786432 UON720901:UON786432 UYJ720901:UYJ786432 VIF720901:VIF786432 VSB720901:VSB786432 WBX720901:WBX786432 WLT720901:WLT786432 WVP720901:WVP786432 JD786437:JD851968 SZ786437:SZ851968 ACV786437:ACV851968 AMR786437:AMR851968 AWN786437:AWN851968 BGJ786437:BGJ851968 BQF786437:BQF851968 CAB786437:CAB851968 CJX786437:CJX851968 CTT786437:CTT851968 DDP786437:DDP851968 DNL786437:DNL851968 DXH786437:DXH851968 EHD786437:EHD851968 EQZ786437:EQZ851968 FAV786437:FAV851968 FKR786437:FKR851968 FUN786437:FUN851968 GEJ786437:GEJ851968 GOF786437:GOF851968 GYB786437:GYB851968 HHX786437:HHX851968 HRT786437:HRT851968 IBP786437:IBP851968 ILL786437:ILL851968 IVH786437:IVH851968 JFD786437:JFD851968 JOZ786437:JOZ851968 JYV786437:JYV851968 KIR786437:KIR851968 KSN786437:KSN851968 LCJ786437:LCJ851968 LMF786437:LMF851968 LWB786437:LWB851968 MFX786437:MFX851968 MPT786437:MPT851968 MZP786437:MZP851968 NJL786437:NJL851968 NTH786437:NTH851968 ODD786437:ODD851968 OMZ786437:OMZ851968 OWV786437:OWV851968 PGR786437:PGR851968 PQN786437:PQN851968 QAJ786437:QAJ851968 QKF786437:QKF851968 QUB786437:QUB851968 RDX786437:RDX851968 RNT786437:RNT851968 RXP786437:RXP851968 SHL786437:SHL851968 SRH786437:SRH851968 TBD786437:TBD851968 TKZ786437:TKZ851968 TUV786437:TUV851968 UER786437:UER851968 UON786437:UON851968 UYJ786437:UYJ851968 VIF786437:VIF851968 VSB786437:VSB851968 WBX786437:WBX851968 WLT786437:WLT851968 WVP786437:WVP851968 JD851973:JD917504 SZ851973:SZ917504 ACV851973:ACV917504 AMR851973:AMR917504 AWN851973:AWN917504 BGJ851973:BGJ917504 BQF851973:BQF917504 CAB851973:CAB917504 CJX851973:CJX917504 CTT851973:CTT917504 DDP851973:DDP917504 DNL851973:DNL917504 DXH851973:DXH917504 EHD851973:EHD917504 EQZ851973:EQZ917504 FAV851973:FAV917504 FKR851973:FKR917504 FUN851973:FUN917504 GEJ851973:GEJ917504 GOF851973:GOF917504 GYB851973:GYB917504 HHX851973:HHX917504 HRT851973:HRT917504 IBP851973:IBP917504 ILL851973:ILL917504 IVH851973:IVH917504 JFD851973:JFD917504 JOZ851973:JOZ917504 JYV851973:JYV917504 KIR851973:KIR917504 KSN851973:KSN917504 LCJ851973:LCJ917504 LMF851973:LMF917504 LWB851973:LWB917504 MFX851973:MFX917504 MPT851973:MPT917504 MZP851973:MZP917504 NJL851973:NJL917504 NTH851973:NTH917504 ODD851973:ODD917504 OMZ851973:OMZ917504 OWV851973:OWV917504 PGR851973:PGR917504 PQN851973:PQN917504 QAJ851973:QAJ917504 QKF851973:QKF917504 QUB851973:QUB917504 RDX851973:RDX917504 RNT851973:RNT917504 RXP851973:RXP917504 SHL851973:SHL917504 SRH851973:SRH917504 TBD851973:TBD917504 TKZ851973:TKZ917504 TUV851973:TUV917504 UER851973:UER917504 UON851973:UON917504 UYJ851973:UYJ917504 VIF851973:VIF917504 VSB851973:VSB917504 WBX851973:WBX917504 WLT851973:WLT917504 WVP851973:WVP917504 JD917509:JD983040 SZ917509:SZ983040 ACV917509:ACV983040 AMR917509:AMR983040 AWN917509:AWN983040 BGJ917509:BGJ983040 BQF917509:BQF983040 CAB917509:CAB983040 CJX917509:CJX983040 CTT917509:CTT983040 DDP917509:DDP983040 DNL917509:DNL983040 DXH917509:DXH983040 EHD917509:EHD983040 EQZ917509:EQZ983040 FAV917509:FAV983040 FKR917509:FKR983040 FUN917509:FUN983040 GEJ917509:GEJ983040 GOF917509:GOF983040 GYB917509:GYB983040 HHX917509:HHX983040 HRT917509:HRT983040 IBP917509:IBP983040 ILL917509:ILL983040 IVH917509:IVH983040 JFD917509:JFD983040 JOZ917509:JOZ983040 JYV917509:JYV983040 KIR917509:KIR983040 KSN917509:KSN983040 LCJ917509:LCJ983040 LMF917509:LMF983040 LWB917509:LWB983040 MFX917509:MFX983040 MPT917509:MPT983040 MZP917509:MZP983040 NJL917509:NJL983040 NTH917509:NTH983040 ODD917509:ODD983040 OMZ917509:OMZ983040 OWV917509:OWV983040 PGR917509:PGR983040 PQN917509:PQN983040 QAJ917509:QAJ983040 QKF917509:QKF983040 QUB917509:QUB983040 RDX917509:RDX983040 RNT917509:RNT983040 RXP917509:RXP983040 SHL917509:SHL983040 SRH917509:SRH983040 TBD917509:TBD983040 TKZ917509:TKZ983040 TUV917509:TUV983040 UER917509:UER983040 UON917509:UON983040 UYJ917509:UYJ983040 VIF917509:VIF983040 VSB917509:VSB983040 WBX917509:WBX983040 WLT917509:WLT983040 WVP917509:WVP983040 JD983045:JD1048576 SZ983045:SZ1048576 ACV983045:ACV1048576 AMR983045:AMR1048576 AWN983045:AWN1048576 BGJ983045:BGJ1048576 BQF983045:BQF1048576 CAB983045:CAB1048576 CJX983045:CJX1048576 CTT983045:CTT1048576 DDP983045:DDP1048576 DNL983045:DNL1048576 DXH983045:DXH1048576 EHD983045:EHD1048576 EQZ983045:EQZ1048576 FAV983045:FAV1048576 FKR983045:FKR1048576 FUN983045:FUN1048576 GEJ983045:GEJ1048576 GOF983045:GOF1048576 GYB983045:GYB1048576 HHX983045:HHX1048576 HRT983045:HRT1048576 IBP983045:IBP1048576 ILL983045:ILL1048576 IVH983045:IVH1048576 JFD983045:JFD1048576 JOZ983045:JOZ1048576 JYV983045:JYV1048576 KIR983045:KIR1048576 KSN983045:KSN1048576 LCJ983045:LCJ1048576 LMF983045:LMF1048576 LWB983045:LWB1048576 MFX983045:MFX1048576 MPT983045:MPT1048576 MZP983045:MZP1048576 NJL983045:NJL1048576 NTH983045:NTH1048576 ODD983045:ODD1048576 OMZ983045:OMZ1048576 OWV983045:OWV1048576 PGR983045:PGR1048576 PQN983045:PQN1048576 QAJ983045:QAJ1048576 QKF983045:QKF1048576 QUB983045:QUB1048576 RDX983045:RDX1048576 RNT983045:RNT1048576 RXP983045:RXP1048576 SHL983045:SHL1048576 SRH983045:SRH1048576 TBD983045:TBD1048576 TKZ983045:TKZ1048576 TUV983045:TUV1048576 UER983045:UER1048576 UON983045:UON1048576 UYJ983045:UYJ1048576 VIF983045:VIF1048576 VSB983045:VSB1048576 WBX983045:WBX1048576 WLT983045:WLT1048576">
+    <dataValidation type="list" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVP982992:WVP1048576 JD65488:JD131019 SZ65488:SZ131019 ACV65488:ACV131019 AMR65488:AMR131019 AWN65488:AWN131019 BGJ65488:BGJ131019 BQF65488:BQF131019 CAB65488:CAB131019 CJX65488:CJX131019 CTT65488:CTT131019 DDP65488:DDP131019 DNL65488:DNL131019 DXH65488:DXH131019 EHD65488:EHD131019 EQZ65488:EQZ131019 FAV65488:FAV131019 FKR65488:FKR131019 FUN65488:FUN131019 GEJ65488:GEJ131019 GOF65488:GOF131019 GYB65488:GYB131019 HHX65488:HHX131019 HRT65488:HRT131019 IBP65488:IBP131019 ILL65488:ILL131019 IVH65488:IVH131019 JFD65488:JFD131019 JOZ65488:JOZ131019 JYV65488:JYV131019 KIR65488:KIR131019 KSN65488:KSN131019 LCJ65488:LCJ131019 LMF65488:LMF131019 LWB65488:LWB131019 MFX65488:MFX131019 MPT65488:MPT131019 MZP65488:MZP131019 NJL65488:NJL131019 NTH65488:NTH131019 ODD65488:ODD131019 OMZ65488:OMZ131019 OWV65488:OWV131019 PGR65488:PGR131019 PQN65488:PQN131019 QAJ65488:QAJ131019 QKF65488:QKF131019 QUB65488:QUB131019 RDX65488:RDX131019 RNT65488:RNT131019 RXP65488:RXP131019 SHL65488:SHL131019 SRH65488:SRH131019 TBD65488:TBD131019 TKZ65488:TKZ131019 TUV65488:TUV131019 UER65488:UER131019 UON65488:UON131019 UYJ65488:UYJ131019 VIF65488:VIF131019 VSB65488:VSB131019 WBX65488:WBX131019 WLT65488:WLT131019 WVP65488:WVP131019 JD131024:JD196555 SZ131024:SZ196555 ACV131024:ACV196555 AMR131024:AMR196555 AWN131024:AWN196555 BGJ131024:BGJ196555 BQF131024:BQF196555 CAB131024:CAB196555 CJX131024:CJX196555 CTT131024:CTT196555 DDP131024:DDP196555 DNL131024:DNL196555 DXH131024:DXH196555 EHD131024:EHD196555 EQZ131024:EQZ196555 FAV131024:FAV196555 FKR131024:FKR196555 FUN131024:FUN196555 GEJ131024:GEJ196555 GOF131024:GOF196555 GYB131024:GYB196555 HHX131024:HHX196555 HRT131024:HRT196555 IBP131024:IBP196555 ILL131024:ILL196555 IVH131024:IVH196555 JFD131024:JFD196555 JOZ131024:JOZ196555 JYV131024:JYV196555 KIR131024:KIR196555 KSN131024:KSN196555 LCJ131024:LCJ196555 LMF131024:LMF196555 LWB131024:LWB196555 MFX131024:MFX196555 MPT131024:MPT196555 MZP131024:MZP196555 NJL131024:NJL196555 NTH131024:NTH196555 ODD131024:ODD196555 OMZ131024:OMZ196555 OWV131024:OWV196555 PGR131024:PGR196555 PQN131024:PQN196555 QAJ131024:QAJ196555 QKF131024:QKF196555 QUB131024:QUB196555 RDX131024:RDX196555 RNT131024:RNT196555 RXP131024:RXP196555 SHL131024:SHL196555 SRH131024:SRH196555 TBD131024:TBD196555 TKZ131024:TKZ196555 TUV131024:TUV196555 UER131024:UER196555 UON131024:UON196555 UYJ131024:UYJ196555 VIF131024:VIF196555 VSB131024:VSB196555 WBX131024:WBX196555 WLT131024:WLT196555 WVP131024:WVP196555 JD196560:JD262091 SZ196560:SZ262091 ACV196560:ACV262091 AMR196560:AMR262091 AWN196560:AWN262091 BGJ196560:BGJ262091 BQF196560:BQF262091 CAB196560:CAB262091 CJX196560:CJX262091 CTT196560:CTT262091 DDP196560:DDP262091 DNL196560:DNL262091 DXH196560:DXH262091 EHD196560:EHD262091 EQZ196560:EQZ262091 FAV196560:FAV262091 FKR196560:FKR262091 FUN196560:FUN262091 GEJ196560:GEJ262091 GOF196560:GOF262091 GYB196560:GYB262091 HHX196560:HHX262091 HRT196560:HRT262091 IBP196560:IBP262091 ILL196560:ILL262091 IVH196560:IVH262091 JFD196560:JFD262091 JOZ196560:JOZ262091 JYV196560:JYV262091 KIR196560:KIR262091 KSN196560:KSN262091 LCJ196560:LCJ262091 LMF196560:LMF262091 LWB196560:LWB262091 MFX196560:MFX262091 MPT196560:MPT262091 MZP196560:MZP262091 NJL196560:NJL262091 NTH196560:NTH262091 ODD196560:ODD262091 OMZ196560:OMZ262091 OWV196560:OWV262091 PGR196560:PGR262091 PQN196560:PQN262091 QAJ196560:QAJ262091 QKF196560:QKF262091 QUB196560:QUB262091 RDX196560:RDX262091 RNT196560:RNT262091 RXP196560:RXP262091 SHL196560:SHL262091 SRH196560:SRH262091 TBD196560:TBD262091 TKZ196560:TKZ262091 TUV196560:TUV262091 UER196560:UER262091 UON196560:UON262091 UYJ196560:UYJ262091 VIF196560:VIF262091 VSB196560:VSB262091 WBX196560:WBX262091 WLT196560:WLT262091 WVP196560:WVP262091 JD262096:JD327627 SZ262096:SZ327627 ACV262096:ACV327627 AMR262096:AMR327627 AWN262096:AWN327627 BGJ262096:BGJ327627 BQF262096:BQF327627 CAB262096:CAB327627 CJX262096:CJX327627 CTT262096:CTT327627 DDP262096:DDP327627 DNL262096:DNL327627 DXH262096:DXH327627 EHD262096:EHD327627 EQZ262096:EQZ327627 FAV262096:FAV327627 FKR262096:FKR327627 FUN262096:FUN327627 GEJ262096:GEJ327627 GOF262096:GOF327627 GYB262096:GYB327627 HHX262096:HHX327627 HRT262096:HRT327627 IBP262096:IBP327627 ILL262096:ILL327627 IVH262096:IVH327627 JFD262096:JFD327627 JOZ262096:JOZ327627 JYV262096:JYV327627 KIR262096:KIR327627 KSN262096:KSN327627 LCJ262096:LCJ327627 LMF262096:LMF327627 LWB262096:LWB327627 MFX262096:MFX327627 MPT262096:MPT327627 MZP262096:MZP327627 NJL262096:NJL327627 NTH262096:NTH327627 ODD262096:ODD327627 OMZ262096:OMZ327627 OWV262096:OWV327627 PGR262096:PGR327627 PQN262096:PQN327627 QAJ262096:QAJ327627 QKF262096:QKF327627 QUB262096:QUB327627 RDX262096:RDX327627 RNT262096:RNT327627 RXP262096:RXP327627 SHL262096:SHL327627 SRH262096:SRH327627 TBD262096:TBD327627 TKZ262096:TKZ327627 TUV262096:TUV327627 UER262096:UER327627 UON262096:UON327627 UYJ262096:UYJ327627 VIF262096:VIF327627 VSB262096:VSB327627 WBX262096:WBX327627 WLT262096:WLT327627 WVP262096:WVP327627 JD327632:JD393163 SZ327632:SZ393163 ACV327632:ACV393163 AMR327632:AMR393163 AWN327632:AWN393163 BGJ327632:BGJ393163 BQF327632:BQF393163 CAB327632:CAB393163 CJX327632:CJX393163 CTT327632:CTT393163 DDP327632:DDP393163 DNL327632:DNL393163 DXH327632:DXH393163 EHD327632:EHD393163 EQZ327632:EQZ393163 FAV327632:FAV393163 FKR327632:FKR393163 FUN327632:FUN393163 GEJ327632:GEJ393163 GOF327632:GOF393163 GYB327632:GYB393163 HHX327632:HHX393163 HRT327632:HRT393163 IBP327632:IBP393163 ILL327632:ILL393163 IVH327632:IVH393163 JFD327632:JFD393163 JOZ327632:JOZ393163 JYV327632:JYV393163 KIR327632:KIR393163 KSN327632:KSN393163 LCJ327632:LCJ393163 LMF327632:LMF393163 LWB327632:LWB393163 MFX327632:MFX393163 MPT327632:MPT393163 MZP327632:MZP393163 NJL327632:NJL393163 NTH327632:NTH393163 ODD327632:ODD393163 OMZ327632:OMZ393163 OWV327632:OWV393163 PGR327632:PGR393163 PQN327632:PQN393163 QAJ327632:QAJ393163 QKF327632:QKF393163 QUB327632:QUB393163 RDX327632:RDX393163 RNT327632:RNT393163 RXP327632:RXP393163 SHL327632:SHL393163 SRH327632:SRH393163 TBD327632:TBD393163 TKZ327632:TKZ393163 TUV327632:TUV393163 UER327632:UER393163 UON327632:UON393163 UYJ327632:UYJ393163 VIF327632:VIF393163 VSB327632:VSB393163 WBX327632:WBX393163 WLT327632:WLT393163 WVP327632:WVP393163 JD393168:JD458699 SZ393168:SZ458699 ACV393168:ACV458699 AMR393168:AMR458699 AWN393168:AWN458699 BGJ393168:BGJ458699 BQF393168:BQF458699 CAB393168:CAB458699 CJX393168:CJX458699 CTT393168:CTT458699 DDP393168:DDP458699 DNL393168:DNL458699 DXH393168:DXH458699 EHD393168:EHD458699 EQZ393168:EQZ458699 FAV393168:FAV458699 FKR393168:FKR458699 FUN393168:FUN458699 GEJ393168:GEJ458699 GOF393168:GOF458699 GYB393168:GYB458699 HHX393168:HHX458699 HRT393168:HRT458699 IBP393168:IBP458699 ILL393168:ILL458699 IVH393168:IVH458699 JFD393168:JFD458699 JOZ393168:JOZ458699 JYV393168:JYV458699 KIR393168:KIR458699 KSN393168:KSN458699 LCJ393168:LCJ458699 LMF393168:LMF458699 LWB393168:LWB458699 MFX393168:MFX458699 MPT393168:MPT458699 MZP393168:MZP458699 NJL393168:NJL458699 NTH393168:NTH458699 ODD393168:ODD458699 OMZ393168:OMZ458699 OWV393168:OWV458699 PGR393168:PGR458699 PQN393168:PQN458699 QAJ393168:QAJ458699 QKF393168:QKF458699 QUB393168:QUB458699 RDX393168:RDX458699 RNT393168:RNT458699 RXP393168:RXP458699 SHL393168:SHL458699 SRH393168:SRH458699 TBD393168:TBD458699 TKZ393168:TKZ458699 TUV393168:TUV458699 UER393168:UER458699 UON393168:UON458699 UYJ393168:UYJ458699 VIF393168:VIF458699 VSB393168:VSB458699 WBX393168:WBX458699 WLT393168:WLT458699 WVP393168:WVP458699 JD458704:JD524235 SZ458704:SZ524235 ACV458704:ACV524235 AMR458704:AMR524235 AWN458704:AWN524235 BGJ458704:BGJ524235 BQF458704:BQF524235 CAB458704:CAB524235 CJX458704:CJX524235 CTT458704:CTT524235 DDP458704:DDP524235 DNL458704:DNL524235 DXH458704:DXH524235 EHD458704:EHD524235 EQZ458704:EQZ524235 FAV458704:FAV524235 FKR458704:FKR524235 FUN458704:FUN524235 GEJ458704:GEJ524235 GOF458704:GOF524235 GYB458704:GYB524235 HHX458704:HHX524235 HRT458704:HRT524235 IBP458704:IBP524235 ILL458704:ILL524235 IVH458704:IVH524235 JFD458704:JFD524235 JOZ458704:JOZ524235 JYV458704:JYV524235 KIR458704:KIR524235 KSN458704:KSN524235 LCJ458704:LCJ524235 LMF458704:LMF524235 LWB458704:LWB524235 MFX458704:MFX524235 MPT458704:MPT524235 MZP458704:MZP524235 NJL458704:NJL524235 NTH458704:NTH524235 ODD458704:ODD524235 OMZ458704:OMZ524235 OWV458704:OWV524235 PGR458704:PGR524235 PQN458704:PQN524235 QAJ458704:QAJ524235 QKF458704:QKF524235 QUB458704:QUB524235 RDX458704:RDX524235 RNT458704:RNT524235 RXP458704:RXP524235 SHL458704:SHL524235 SRH458704:SRH524235 TBD458704:TBD524235 TKZ458704:TKZ524235 TUV458704:TUV524235 UER458704:UER524235 UON458704:UON524235 UYJ458704:UYJ524235 VIF458704:VIF524235 VSB458704:VSB524235 WBX458704:WBX524235 WLT458704:WLT524235 WVP458704:WVP524235 JD524240:JD589771 SZ524240:SZ589771 ACV524240:ACV589771 AMR524240:AMR589771 AWN524240:AWN589771 BGJ524240:BGJ589771 BQF524240:BQF589771 CAB524240:CAB589771 CJX524240:CJX589771 CTT524240:CTT589771 DDP524240:DDP589771 DNL524240:DNL589771 DXH524240:DXH589771 EHD524240:EHD589771 EQZ524240:EQZ589771 FAV524240:FAV589771 FKR524240:FKR589771 FUN524240:FUN589771 GEJ524240:GEJ589771 GOF524240:GOF589771 GYB524240:GYB589771 HHX524240:HHX589771 HRT524240:HRT589771 IBP524240:IBP589771 ILL524240:ILL589771 IVH524240:IVH589771 JFD524240:JFD589771 JOZ524240:JOZ589771 JYV524240:JYV589771 KIR524240:KIR589771 KSN524240:KSN589771 LCJ524240:LCJ589771 LMF524240:LMF589771 LWB524240:LWB589771 MFX524240:MFX589771 MPT524240:MPT589771 MZP524240:MZP589771 NJL524240:NJL589771 NTH524240:NTH589771 ODD524240:ODD589771 OMZ524240:OMZ589771 OWV524240:OWV589771 PGR524240:PGR589771 PQN524240:PQN589771 QAJ524240:QAJ589771 QKF524240:QKF589771 QUB524240:QUB589771 RDX524240:RDX589771 RNT524240:RNT589771 RXP524240:RXP589771 SHL524240:SHL589771 SRH524240:SRH589771 TBD524240:TBD589771 TKZ524240:TKZ589771 TUV524240:TUV589771 UER524240:UER589771 UON524240:UON589771 UYJ524240:UYJ589771 VIF524240:VIF589771 VSB524240:VSB589771 WBX524240:WBX589771 WLT524240:WLT589771 WVP524240:WVP589771 JD589776:JD655307 SZ589776:SZ655307 ACV589776:ACV655307 AMR589776:AMR655307 AWN589776:AWN655307 BGJ589776:BGJ655307 BQF589776:BQF655307 CAB589776:CAB655307 CJX589776:CJX655307 CTT589776:CTT655307 DDP589776:DDP655307 DNL589776:DNL655307 DXH589776:DXH655307 EHD589776:EHD655307 EQZ589776:EQZ655307 FAV589776:FAV655307 FKR589776:FKR655307 FUN589776:FUN655307 GEJ589776:GEJ655307 GOF589776:GOF655307 GYB589776:GYB655307 HHX589776:HHX655307 HRT589776:HRT655307 IBP589776:IBP655307 ILL589776:ILL655307 IVH589776:IVH655307 JFD589776:JFD655307 JOZ589776:JOZ655307 JYV589776:JYV655307 KIR589776:KIR655307 KSN589776:KSN655307 LCJ589776:LCJ655307 LMF589776:LMF655307 LWB589776:LWB655307 MFX589776:MFX655307 MPT589776:MPT655307 MZP589776:MZP655307 NJL589776:NJL655307 NTH589776:NTH655307 ODD589776:ODD655307 OMZ589776:OMZ655307 OWV589776:OWV655307 PGR589776:PGR655307 PQN589776:PQN655307 QAJ589776:QAJ655307 QKF589776:QKF655307 QUB589776:QUB655307 RDX589776:RDX655307 RNT589776:RNT655307 RXP589776:RXP655307 SHL589776:SHL655307 SRH589776:SRH655307 TBD589776:TBD655307 TKZ589776:TKZ655307 TUV589776:TUV655307 UER589776:UER655307 UON589776:UON655307 UYJ589776:UYJ655307 VIF589776:VIF655307 VSB589776:VSB655307 WBX589776:WBX655307 WLT589776:WLT655307 WVP589776:WVP655307 JD655312:JD720843 SZ655312:SZ720843 ACV655312:ACV720843 AMR655312:AMR720843 AWN655312:AWN720843 BGJ655312:BGJ720843 BQF655312:BQF720843 CAB655312:CAB720843 CJX655312:CJX720843 CTT655312:CTT720843 DDP655312:DDP720843 DNL655312:DNL720843 DXH655312:DXH720843 EHD655312:EHD720843 EQZ655312:EQZ720843 FAV655312:FAV720843 FKR655312:FKR720843 FUN655312:FUN720843 GEJ655312:GEJ720843 GOF655312:GOF720843 GYB655312:GYB720843 HHX655312:HHX720843 HRT655312:HRT720843 IBP655312:IBP720843 ILL655312:ILL720843 IVH655312:IVH720843 JFD655312:JFD720843 JOZ655312:JOZ720843 JYV655312:JYV720843 KIR655312:KIR720843 KSN655312:KSN720843 LCJ655312:LCJ720843 LMF655312:LMF720843 LWB655312:LWB720843 MFX655312:MFX720843 MPT655312:MPT720843 MZP655312:MZP720843 NJL655312:NJL720843 NTH655312:NTH720843 ODD655312:ODD720843 OMZ655312:OMZ720843 OWV655312:OWV720843 PGR655312:PGR720843 PQN655312:PQN720843 QAJ655312:QAJ720843 QKF655312:QKF720843 QUB655312:QUB720843 RDX655312:RDX720843 RNT655312:RNT720843 RXP655312:RXP720843 SHL655312:SHL720843 SRH655312:SRH720843 TBD655312:TBD720843 TKZ655312:TKZ720843 TUV655312:TUV720843 UER655312:UER720843 UON655312:UON720843 UYJ655312:UYJ720843 VIF655312:VIF720843 VSB655312:VSB720843 WBX655312:WBX720843 WLT655312:WLT720843 WVP655312:WVP720843 JD720848:JD786379 SZ720848:SZ786379 ACV720848:ACV786379 AMR720848:AMR786379 AWN720848:AWN786379 BGJ720848:BGJ786379 BQF720848:BQF786379 CAB720848:CAB786379 CJX720848:CJX786379 CTT720848:CTT786379 DDP720848:DDP786379 DNL720848:DNL786379 DXH720848:DXH786379 EHD720848:EHD786379 EQZ720848:EQZ786379 FAV720848:FAV786379 FKR720848:FKR786379 FUN720848:FUN786379 GEJ720848:GEJ786379 GOF720848:GOF786379 GYB720848:GYB786379 HHX720848:HHX786379 HRT720848:HRT786379 IBP720848:IBP786379 ILL720848:ILL786379 IVH720848:IVH786379 JFD720848:JFD786379 JOZ720848:JOZ786379 JYV720848:JYV786379 KIR720848:KIR786379 KSN720848:KSN786379 LCJ720848:LCJ786379 LMF720848:LMF786379 LWB720848:LWB786379 MFX720848:MFX786379 MPT720848:MPT786379 MZP720848:MZP786379 NJL720848:NJL786379 NTH720848:NTH786379 ODD720848:ODD786379 OMZ720848:OMZ786379 OWV720848:OWV786379 PGR720848:PGR786379 PQN720848:PQN786379 QAJ720848:QAJ786379 QKF720848:QKF786379 QUB720848:QUB786379 RDX720848:RDX786379 RNT720848:RNT786379 RXP720848:RXP786379 SHL720848:SHL786379 SRH720848:SRH786379 TBD720848:TBD786379 TKZ720848:TKZ786379 TUV720848:TUV786379 UER720848:UER786379 UON720848:UON786379 UYJ720848:UYJ786379 VIF720848:VIF786379 VSB720848:VSB786379 WBX720848:WBX786379 WLT720848:WLT786379 WVP720848:WVP786379 JD786384:JD851915 SZ786384:SZ851915 ACV786384:ACV851915 AMR786384:AMR851915 AWN786384:AWN851915 BGJ786384:BGJ851915 BQF786384:BQF851915 CAB786384:CAB851915 CJX786384:CJX851915 CTT786384:CTT851915 DDP786384:DDP851915 DNL786384:DNL851915 DXH786384:DXH851915 EHD786384:EHD851915 EQZ786384:EQZ851915 FAV786384:FAV851915 FKR786384:FKR851915 FUN786384:FUN851915 GEJ786384:GEJ851915 GOF786384:GOF851915 GYB786384:GYB851915 HHX786384:HHX851915 HRT786384:HRT851915 IBP786384:IBP851915 ILL786384:ILL851915 IVH786384:IVH851915 JFD786384:JFD851915 JOZ786384:JOZ851915 JYV786384:JYV851915 KIR786384:KIR851915 KSN786384:KSN851915 LCJ786384:LCJ851915 LMF786384:LMF851915 LWB786384:LWB851915 MFX786384:MFX851915 MPT786384:MPT851915 MZP786384:MZP851915 NJL786384:NJL851915 NTH786384:NTH851915 ODD786384:ODD851915 OMZ786384:OMZ851915 OWV786384:OWV851915 PGR786384:PGR851915 PQN786384:PQN851915 QAJ786384:QAJ851915 QKF786384:QKF851915 QUB786384:QUB851915 RDX786384:RDX851915 RNT786384:RNT851915 RXP786384:RXP851915 SHL786384:SHL851915 SRH786384:SRH851915 TBD786384:TBD851915 TKZ786384:TKZ851915 TUV786384:TUV851915 UER786384:UER851915 UON786384:UON851915 UYJ786384:UYJ851915 VIF786384:VIF851915 VSB786384:VSB851915 WBX786384:WBX851915 WLT786384:WLT851915 WVP786384:WVP851915 JD851920:JD917451 SZ851920:SZ917451 ACV851920:ACV917451 AMR851920:AMR917451 AWN851920:AWN917451 BGJ851920:BGJ917451 BQF851920:BQF917451 CAB851920:CAB917451 CJX851920:CJX917451 CTT851920:CTT917451 DDP851920:DDP917451 DNL851920:DNL917451 DXH851920:DXH917451 EHD851920:EHD917451 EQZ851920:EQZ917451 FAV851920:FAV917451 FKR851920:FKR917451 FUN851920:FUN917451 GEJ851920:GEJ917451 GOF851920:GOF917451 GYB851920:GYB917451 HHX851920:HHX917451 HRT851920:HRT917451 IBP851920:IBP917451 ILL851920:ILL917451 IVH851920:IVH917451 JFD851920:JFD917451 JOZ851920:JOZ917451 JYV851920:JYV917451 KIR851920:KIR917451 KSN851920:KSN917451 LCJ851920:LCJ917451 LMF851920:LMF917451 LWB851920:LWB917451 MFX851920:MFX917451 MPT851920:MPT917451 MZP851920:MZP917451 NJL851920:NJL917451 NTH851920:NTH917451 ODD851920:ODD917451 OMZ851920:OMZ917451 OWV851920:OWV917451 PGR851920:PGR917451 PQN851920:PQN917451 QAJ851920:QAJ917451 QKF851920:QKF917451 QUB851920:QUB917451 RDX851920:RDX917451 RNT851920:RNT917451 RXP851920:RXP917451 SHL851920:SHL917451 SRH851920:SRH917451 TBD851920:TBD917451 TKZ851920:TKZ917451 TUV851920:TUV917451 UER851920:UER917451 UON851920:UON917451 UYJ851920:UYJ917451 VIF851920:VIF917451 VSB851920:VSB917451 WBX851920:WBX917451 WLT851920:WLT917451 WVP851920:WVP917451 JD917456:JD982987 SZ917456:SZ982987 ACV917456:ACV982987 AMR917456:AMR982987 AWN917456:AWN982987 BGJ917456:BGJ982987 BQF917456:BQF982987 CAB917456:CAB982987 CJX917456:CJX982987 CTT917456:CTT982987 DDP917456:DDP982987 DNL917456:DNL982987 DXH917456:DXH982987 EHD917456:EHD982987 EQZ917456:EQZ982987 FAV917456:FAV982987 FKR917456:FKR982987 FUN917456:FUN982987 GEJ917456:GEJ982987 GOF917456:GOF982987 GYB917456:GYB982987 HHX917456:HHX982987 HRT917456:HRT982987 IBP917456:IBP982987 ILL917456:ILL982987 IVH917456:IVH982987 JFD917456:JFD982987 JOZ917456:JOZ982987 JYV917456:JYV982987 KIR917456:KIR982987 KSN917456:KSN982987 LCJ917456:LCJ982987 LMF917456:LMF982987 LWB917456:LWB982987 MFX917456:MFX982987 MPT917456:MPT982987 MZP917456:MZP982987 NJL917456:NJL982987 NTH917456:NTH982987 ODD917456:ODD982987 OMZ917456:OMZ982987 OWV917456:OWV982987 PGR917456:PGR982987 PQN917456:PQN982987 QAJ917456:QAJ982987 QKF917456:QKF982987 QUB917456:QUB982987 RDX917456:RDX982987 RNT917456:RNT982987 RXP917456:RXP982987 SHL917456:SHL982987 SRH917456:SRH982987 TBD917456:TBD982987 TKZ917456:TKZ982987 TUV917456:TUV982987 UER917456:UER982987 UON917456:UON982987 UYJ917456:UYJ982987 VIF917456:VIF982987 VSB917456:VSB982987 WBX917456:WBX982987 WLT917456:WLT982987 WVP917456:WVP982987 JD982992:JD1048576 SZ982992:SZ1048576 ACV982992:ACV1048576 AMR982992:AMR1048576 AWN982992:AWN1048576 BGJ982992:BGJ1048576 BQF982992:BQF1048576 CAB982992:CAB1048576 CJX982992:CJX1048576 CTT982992:CTT1048576 DDP982992:DDP1048576 DNL982992:DNL1048576 DXH982992:DXH1048576 EHD982992:EHD1048576 EQZ982992:EQZ1048576 FAV982992:FAV1048576 FKR982992:FKR1048576 FUN982992:FUN1048576 GEJ982992:GEJ1048576 GOF982992:GOF1048576 GYB982992:GYB1048576 HHX982992:HHX1048576 HRT982992:HRT1048576 IBP982992:IBP1048576 ILL982992:ILL1048576 IVH982992:IVH1048576 JFD982992:JFD1048576 JOZ982992:JOZ1048576 JYV982992:JYV1048576 KIR982992:KIR1048576 KSN982992:KSN1048576 LCJ982992:LCJ1048576 LMF982992:LMF1048576 LWB982992:LWB1048576 MFX982992:MFX1048576 MPT982992:MPT1048576 MZP982992:MZP1048576 NJL982992:NJL1048576 NTH982992:NTH1048576 ODD982992:ODD1048576 OMZ982992:OMZ1048576 OWV982992:OWV1048576 PGR982992:PGR1048576 PQN982992:PQN1048576 QAJ982992:QAJ1048576 QKF982992:QKF1048576 QUB982992:QUB1048576 RDX982992:RDX1048576 RNT982992:RNT1048576 RXP982992:RXP1048576 SHL982992:SHL1048576 SRH982992:SRH1048576 TBD982992:TBD1048576 TKZ982992:TKZ1048576 TUV982992:TUV1048576 UER982992:UER1048576 UON982992:UON1048576 UYJ982992:UYJ1048576 VIF982992:VIF1048576 VSB982992:VSB1048576 WBX982992:WBX1048576 WLT982992:WLT1048576 JD5:JD65483 SZ5:SZ65483 ACV5:ACV65483 AMR5:AMR65483 AWN5:AWN65483 BGJ5:BGJ65483 BQF5:BQF65483 CAB5:CAB65483 CJX5:CJX65483 CTT5:CTT65483 DDP5:DDP65483 DNL5:DNL65483 DXH5:DXH65483 EHD5:EHD65483 EQZ5:EQZ65483 FAV5:FAV65483 FKR5:FKR65483 FUN5:FUN65483 GEJ5:GEJ65483 GOF5:GOF65483 GYB5:GYB65483 HHX5:HHX65483 HRT5:HRT65483 IBP5:IBP65483 ILL5:ILL65483 IVH5:IVH65483 JFD5:JFD65483 JOZ5:JOZ65483 JYV5:JYV65483 KIR5:KIR65483 KSN5:KSN65483 LCJ5:LCJ65483 LMF5:LMF65483 LWB5:LWB65483 MFX5:MFX65483 MPT5:MPT65483 MZP5:MZP65483 NJL5:NJL65483 NTH5:NTH65483 ODD5:ODD65483 OMZ5:OMZ65483 OWV5:OWV65483 PGR5:PGR65483 PQN5:PQN65483 QAJ5:QAJ65483 QKF5:QKF65483 QUB5:QUB65483 RDX5:RDX65483 RNT5:RNT65483 RXP5:RXP65483 SHL5:SHL65483 SRH5:SRH65483 TBD5:TBD65483 TKZ5:TKZ65483 TUV5:TUV65483 UER5:UER65483 UON5:UON65483 UYJ5:UYJ65483 VIF5:VIF65483 VSB5:VSB65483 WBX5:WBX65483 WLT5:WLT65483 WVP5:WVP65483">
       <formula1>"~"</formula1>
     </dataValidation>
-    <dataValidation type="list" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVN983045:WVN1048576 JB5:JB65536 SX5:SX65536 ACT5:ACT65536 AMP5:AMP65536 AWL5:AWL65536 BGH5:BGH65536 BQD5:BQD65536 BZZ5:BZZ65536 CJV5:CJV65536 CTR5:CTR65536 DDN5:DDN65536 DNJ5:DNJ65536 DXF5:DXF65536 EHB5:EHB65536 EQX5:EQX65536 FAT5:FAT65536 FKP5:FKP65536 FUL5:FUL65536 GEH5:GEH65536 GOD5:GOD65536 GXZ5:GXZ65536 HHV5:HHV65536 HRR5:HRR65536 IBN5:IBN65536 ILJ5:ILJ65536 IVF5:IVF65536 JFB5:JFB65536 JOX5:JOX65536 JYT5:JYT65536 KIP5:KIP65536 KSL5:KSL65536 LCH5:LCH65536 LMD5:LMD65536 LVZ5:LVZ65536 MFV5:MFV65536 MPR5:MPR65536 MZN5:MZN65536 NJJ5:NJJ65536 NTF5:NTF65536 ODB5:ODB65536 OMX5:OMX65536 OWT5:OWT65536 PGP5:PGP65536 PQL5:PQL65536 QAH5:QAH65536 QKD5:QKD65536 QTZ5:QTZ65536 RDV5:RDV65536 RNR5:RNR65536 RXN5:RXN65536 SHJ5:SHJ65536 SRF5:SRF65536 TBB5:TBB65536 TKX5:TKX65536 TUT5:TUT65536 UEP5:UEP65536 UOL5:UOL65536 UYH5:UYH65536 VID5:VID65536 VRZ5:VRZ65536 WBV5:WBV65536 WLR5:WLR65536 WVN5:WVN65536 JB65541:JB131072 SX65541:SX131072 ACT65541:ACT131072 AMP65541:AMP131072 AWL65541:AWL131072 BGH65541:BGH131072 BQD65541:BQD131072 BZZ65541:BZZ131072 CJV65541:CJV131072 CTR65541:CTR131072 DDN65541:DDN131072 DNJ65541:DNJ131072 DXF65541:DXF131072 EHB65541:EHB131072 EQX65541:EQX131072 FAT65541:FAT131072 FKP65541:FKP131072 FUL65541:FUL131072 GEH65541:GEH131072 GOD65541:GOD131072 GXZ65541:GXZ131072 HHV65541:HHV131072 HRR65541:HRR131072 IBN65541:IBN131072 ILJ65541:ILJ131072 IVF65541:IVF131072 JFB65541:JFB131072 JOX65541:JOX131072 JYT65541:JYT131072 KIP65541:KIP131072 KSL65541:KSL131072 LCH65541:LCH131072 LMD65541:LMD131072 LVZ65541:LVZ131072 MFV65541:MFV131072 MPR65541:MPR131072 MZN65541:MZN131072 NJJ65541:NJJ131072 NTF65541:NTF131072 ODB65541:ODB131072 OMX65541:OMX131072 OWT65541:OWT131072 PGP65541:PGP131072 PQL65541:PQL131072 QAH65541:QAH131072 QKD65541:QKD131072 QTZ65541:QTZ131072 RDV65541:RDV131072 RNR65541:RNR131072 RXN65541:RXN131072 SHJ65541:SHJ131072 SRF65541:SRF131072 TBB65541:TBB131072 TKX65541:TKX131072 TUT65541:TUT131072 UEP65541:UEP131072 UOL65541:UOL131072 UYH65541:UYH131072 VID65541:VID131072 VRZ65541:VRZ131072 WBV65541:WBV131072 WLR65541:WLR131072 WVN65541:WVN131072 JB131077:JB196608 SX131077:SX196608 ACT131077:ACT196608 AMP131077:AMP196608 AWL131077:AWL196608 BGH131077:BGH196608 BQD131077:BQD196608 BZZ131077:BZZ196608 CJV131077:CJV196608 CTR131077:CTR196608 DDN131077:DDN196608 DNJ131077:DNJ196608 DXF131077:DXF196608 EHB131077:EHB196608 EQX131077:EQX196608 FAT131077:FAT196608 FKP131077:FKP196608 FUL131077:FUL196608 GEH131077:GEH196608 GOD131077:GOD196608 GXZ131077:GXZ196608 HHV131077:HHV196608 HRR131077:HRR196608 IBN131077:IBN196608 ILJ131077:ILJ196608 IVF131077:IVF196608 JFB131077:JFB196608 JOX131077:JOX196608 JYT131077:JYT196608 KIP131077:KIP196608 KSL131077:KSL196608 LCH131077:LCH196608 LMD131077:LMD196608 LVZ131077:LVZ196608 MFV131077:MFV196608 MPR131077:MPR196608 MZN131077:MZN196608 NJJ131077:NJJ196608 NTF131077:NTF196608 ODB131077:ODB196608 OMX131077:OMX196608 OWT131077:OWT196608 PGP131077:PGP196608 PQL131077:PQL196608 QAH131077:QAH196608 QKD131077:QKD196608 QTZ131077:QTZ196608 RDV131077:RDV196608 RNR131077:RNR196608 RXN131077:RXN196608 SHJ131077:SHJ196608 SRF131077:SRF196608 TBB131077:TBB196608 TKX131077:TKX196608 TUT131077:TUT196608 UEP131077:UEP196608 UOL131077:UOL196608 UYH131077:UYH196608 VID131077:VID196608 VRZ131077:VRZ196608 WBV131077:WBV196608 WLR131077:WLR196608 WVN131077:WVN196608 JB196613:JB262144 SX196613:SX262144 ACT196613:ACT262144 AMP196613:AMP262144 AWL196613:AWL262144 BGH196613:BGH262144 BQD196613:BQD262144 BZZ196613:BZZ262144 CJV196613:CJV262144 CTR196613:CTR262144 DDN196613:DDN262144 DNJ196613:DNJ262144 DXF196613:DXF262144 EHB196613:EHB262144 EQX196613:EQX262144 FAT196613:FAT262144 FKP196613:FKP262144 FUL196613:FUL262144 GEH196613:GEH262144 GOD196613:GOD262144 GXZ196613:GXZ262144 HHV196613:HHV262144 HRR196613:HRR262144 IBN196613:IBN262144 ILJ196613:ILJ262144 IVF196613:IVF262144 JFB196613:JFB262144 JOX196613:JOX262144 JYT196613:JYT262144 KIP196613:KIP262144 KSL196613:KSL262144 LCH196613:LCH262144 LMD196613:LMD262144 LVZ196613:LVZ262144 MFV196613:MFV262144 MPR196613:MPR262144 MZN196613:MZN262144 NJJ196613:NJJ262144 NTF196613:NTF262144 ODB196613:ODB262144 OMX196613:OMX262144 OWT196613:OWT262144 PGP196613:PGP262144 PQL196613:PQL262144 QAH196613:QAH262144 QKD196613:QKD262144 QTZ196613:QTZ262144 RDV196613:RDV262144 RNR196613:RNR262144 RXN196613:RXN262144 SHJ196613:SHJ262144 SRF196613:SRF262144 TBB196613:TBB262144 TKX196613:TKX262144 TUT196613:TUT262144 UEP196613:UEP262144 UOL196613:UOL262144 UYH196613:UYH262144 VID196613:VID262144 VRZ196613:VRZ262144 WBV196613:WBV262144 WLR196613:WLR262144 WVN196613:WVN262144 JB262149:JB327680 SX262149:SX327680 ACT262149:ACT327680 AMP262149:AMP327680 AWL262149:AWL327680 BGH262149:BGH327680 BQD262149:BQD327680 BZZ262149:BZZ327680 CJV262149:CJV327680 CTR262149:CTR327680 DDN262149:DDN327680 DNJ262149:DNJ327680 DXF262149:DXF327680 EHB262149:EHB327680 EQX262149:EQX327680 FAT262149:FAT327680 FKP262149:FKP327680 FUL262149:FUL327680 GEH262149:GEH327680 GOD262149:GOD327680 GXZ262149:GXZ327680 HHV262149:HHV327680 HRR262149:HRR327680 IBN262149:IBN327680 ILJ262149:ILJ327680 IVF262149:IVF327680 JFB262149:JFB327680 JOX262149:JOX327680 JYT262149:JYT327680 KIP262149:KIP327680 KSL262149:KSL327680 LCH262149:LCH327680 LMD262149:LMD327680 LVZ262149:LVZ327680 MFV262149:MFV327680 MPR262149:MPR327680 MZN262149:MZN327680 NJJ262149:NJJ327680 NTF262149:NTF327680 ODB262149:ODB327680 OMX262149:OMX327680 OWT262149:OWT327680 PGP262149:PGP327680 PQL262149:PQL327680 QAH262149:QAH327680 QKD262149:QKD327680 QTZ262149:QTZ327680 RDV262149:RDV327680 RNR262149:RNR327680 RXN262149:RXN327680 SHJ262149:SHJ327680 SRF262149:SRF327680 TBB262149:TBB327680 TKX262149:TKX327680 TUT262149:TUT327680 UEP262149:UEP327680 UOL262149:UOL327680 UYH262149:UYH327680 VID262149:VID327680 VRZ262149:VRZ327680 WBV262149:WBV327680 WLR262149:WLR327680 WVN262149:WVN327680 JB327685:JB393216 SX327685:SX393216 ACT327685:ACT393216 AMP327685:AMP393216 AWL327685:AWL393216 BGH327685:BGH393216 BQD327685:BQD393216 BZZ327685:BZZ393216 CJV327685:CJV393216 CTR327685:CTR393216 DDN327685:DDN393216 DNJ327685:DNJ393216 DXF327685:DXF393216 EHB327685:EHB393216 EQX327685:EQX393216 FAT327685:FAT393216 FKP327685:FKP393216 FUL327685:FUL393216 GEH327685:GEH393216 GOD327685:GOD393216 GXZ327685:GXZ393216 HHV327685:HHV393216 HRR327685:HRR393216 IBN327685:IBN393216 ILJ327685:ILJ393216 IVF327685:IVF393216 JFB327685:JFB393216 JOX327685:JOX393216 JYT327685:JYT393216 KIP327685:KIP393216 KSL327685:KSL393216 LCH327685:LCH393216 LMD327685:LMD393216 LVZ327685:LVZ393216 MFV327685:MFV393216 MPR327685:MPR393216 MZN327685:MZN393216 NJJ327685:NJJ393216 NTF327685:NTF393216 ODB327685:ODB393216 OMX327685:OMX393216 OWT327685:OWT393216 PGP327685:PGP393216 PQL327685:PQL393216 QAH327685:QAH393216 QKD327685:QKD393216 QTZ327685:QTZ393216 RDV327685:RDV393216 RNR327685:RNR393216 RXN327685:RXN393216 SHJ327685:SHJ393216 SRF327685:SRF393216 TBB327685:TBB393216 TKX327685:TKX393216 TUT327685:TUT393216 UEP327685:UEP393216 UOL327685:UOL393216 UYH327685:UYH393216 VID327685:VID393216 VRZ327685:VRZ393216 WBV327685:WBV393216 WLR327685:WLR393216 WVN327685:WVN393216 JB393221:JB458752 SX393221:SX458752 ACT393221:ACT458752 AMP393221:AMP458752 AWL393221:AWL458752 BGH393221:BGH458752 BQD393221:BQD458752 BZZ393221:BZZ458752 CJV393221:CJV458752 CTR393221:CTR458752 DDN393221:DDN458752 DNJ393221:DNJ458752 DXF393221:DXF458752 EHB393221:EHB458752 EQX393221:EQX458752 FAT393221:FAT458752 FKP393221:FKP458752 FUL393221:FUL458752 GEH393221:GEH458752 GOD393221:GOD458752 GXZ393221:GXZ458752 HHV393221:HHV458752 HRR393221:HRR458752 IBN393221:IBN458752 ILJ393221:ILJ458752 IVF393221:IVF458752 JFB393221:JFB458752 JOX393221:JOX458752 JYT393221:JYT458752 KIP393221:KIP458752 KSL393221:KSL458752 LCH393221:LCH458752 LMD393221:LMD458752 LVZ393221:LVZ458752 MFV393221:MFV458752 MPR393221:MPR458752 MZN393221:MZN458752 NJJ393221:NJJ458752 NTF393221:NTF458752 ODB393221:ODB458752 OMX393221:OMX458752 OWT393221:OWT458752 PGP393221:PGP458752 PQL393221:PQL458752 QAH393221:QAH458752 QKD393221:QKD458752 QTZ393221:QTZ458752 RDV393221:RDV458752 RNR393221:RNR458752 RXN393221:RXN458752 SHJ393221:SHJ458752 SRF393221:SRF458752 TBB393221:TBB458752 TKX393221:TKX458752 TUT393221:TUT458752 UEP393221:UEP458752 UOL393221:UOL458752 UYH393221:UYH458752 VID393221:VID458752 VRZ393221:VRZ458752 WBV393221:WBV458752 WLR393221:WLR458752 WVN393221:WVN458752 JB458757:JB524288 SX458757:SX524288 ACT458757:ACT524288 AMP458757:AMP524288 AWL458757:AWL524288 BGH458757:BGH524288 BQD458757:BQD524288 BZZ458757:BZZ524288 CJV458757:CJV524288 CTR458757:CTR524288 DDN458757:DDN524288 DNJ458757:DNJ524288 DXF458757:DXF524288 EHB458757:EHB524288 EQX458757:EQX524288 FAT458757:FAT524288 FKP458757:FKP524288 FUL458757:FUL524288 GEH458757:GEH524288 GOD458757:GOD524288 GXZ458757:GXZ524288 HHV458757:HHV524288 HRR458757:HRR524288 IBN458757:IBN524288 ILJ458757:ILJ524288 IVF458757:IVF524288 JFB458757:JFB524288 JOX458757:JOX524288 JYT458757:JYT524288 KIP458757:KIP524288 KSL458757:KSL524288 LCH458757:LCH524288 LMD458757:LMD524288 LVZ458757:LVZ524288 MFV458757:MFV524288 MPR458757:MPR524288 MZN458757:MZN524288 NJJ458757:NJJ524288 NTF458757:NTF524288 ODB458757:ODB524288 OMX458757:OMX524288 OWT458757:OWT524288 PGP458757:PGP524288 PQL458757:PQL524288 QAH458757:QAH524288 QKD458757:QKD524288 QTZ458757:QTZ524288 RDV458757:RDV524288 RNR458757:RNR524288 RXN458757:RXN524288 SHJ458757:SHJ524288 SRF458757:SRF524288 TBB458757:TBB524288 TKX458757:TKX524288 TUT458757:TUT524288 UEP458757:UEP524288 UOL458757:UOL524288 UYH458757:UYH524288 VID458757:VID524288 VRZ458757:VRZ524288 WBV458757:WBV524288 WLR458757:WLR524288 WVN458757:WVN524288 JB524293:JB589824 SX524293:SX589824 ACT524293:ACT589824 AMP524293:AMP589824 AWL524293:AWL589824 BGH524293:BGH589824 BQD524293:BQD589824 BZZ524293:BZZ589824 CJV524293:CJV589824 CTR524293:CTR589824 DDN524293:DDN589824 DNJ524293:DNJ589824 DXF524293:DXF589824 EHB524293:EHB589824 EQX524293:EQX589824 FAT524293:FAT589824 FKP524293:FKP589824 FUL524293:FUL589824 GEH524293:GEH589824 GOD524293:GOD589824 GXZ524293:GXZ589824 HHV524293:HHV589824 HRR524293:HRR589824 IBN524293:IBN589824 ILJ524293:ILJ589824 IVF524293:IVF589824 JFB524293:JFB589824 JOX524293:JOX589824 JYT524293:JYT589824 KIP524293:KIP589824 KSL524293:KSL589824 LCH524293:LCH589824 LMD524293:LMD589824 LVZ524293:LVZ589824 MFV524293:MFV589824 MPR524293:MPR589824 MZN524293:MZN589824 NJJ524293:NJJ589824 NTF524293:NTF589824 ODB524293:ODB589824 OMX524293:OMX589824 OWT524293:OWT589824 PGP524293:PGP589824 PQL524293:PQL589824 QAH524293:QAH589824 QKD524293:QKD589824 QTZ524293:QTZ589824 RDV524293:RDV589824 RNR524293:RNR589824 RXN524293:RXN589824 SHJ524293:SHJ589824 SRF524293:SRF589824 TBB524293:TBB589824 TKX524293:TKX589824 TUT524293:TUT589824 UEP524293:UEP589824 UOL524293:UOL589824 UYH524293:UYH589824 VID524293:VID589824 VRZ524293:VRZ589824 WBV524293:WBV589824 WLR524293:WLR589824 WVN524293:WVN589824 JB589829:JB655360 SX589829:SX655360 ACT589829:ACT655360 AMP589829:AMP655360 AWL589829:AWL655360 BGH589829:BGH655360 BQD589829:BQD655360 BZZ589829:BZZ655360 CJV589829:CJV655360 CTR589829:CTR655360 DDN589829:DDN655360 DNJ589829:DNJ655360 DXF589829:DXF655360 EHB589829:EHB655360 EQX589829:EQX655360 FAT589829:FAT655360 FKP589829:FKP655360 FUL589829:FUL655360 GEH589829:GEH655360 GOD589829:GOD655360 GXZ589829:GXZ655360 HHV589829:HHV655360 HRR589829:HRR655360 IBN589829:IBN655360 ILJ589829:ILJ655360 IVF589829:IVF655360 JFB589829:JFB655360 JOX589829:JOX655360 JYT589829:JYT655360 KIP589829:KIP655360 KSL589829:KSL655360 LCH589829:LCH655360 LMD589829:LMD655360 LVZ589829:LVZ655360 MFV589829:MFV655360 MPR589829:MPR655360 MZN589829:MZN655360 NJJ589829:NJJ655360 NTF589829:NTF655360 ODB589829:ODB655360 OMX589829:OMX655360 OWT589829:OWT655360 PGP589829:PGP655360 PQL589829:PQL655360 QAH589829:QAH655360 QKD589829:QKD655360 QTZ589829:QTZ655360 RDV589829:RDV655360 RNR589829:RNR655360 RXN589829:RXN655360 SHJ589829:SHJ655360 SRF589829:SRF655360 TBB589829:TBB655360 TKX589829:TKX655360 TUT589829:TUT655360 UEP589829:UEP655360 UOL589829:UOL655360 UYH589829:UYH655360 VID589829:VID655360 VRZ589829:VRZ655360 WBV589829:WBV655360 WLR589829:WLR655360 WVN589829:WVN655360 JB655365:JB720896 SX655365:SX720896 ACT655365:ACT720896 AMP655365:AMP720896 AWL655365:AWL720896 BGH655365:BGH720896 BQD655365:BQD720896 BZZ655365:BZZ720896 CJV655365:CJV720896 CTR655365:CTR720896 DDN655365:DDN720896 DNJ655365:DNJ720896 DXF655365:DXF720896 EHB655365:EHB720896 EQX655365:EQX720896 FAT655365:FAT720896 FKP655365:FKP720896 FUL655365:FUL720896 GEH655365:GEH720896 GOD655365:GOD720896 GXZ655365:GXZ720896 HHV655365:HHV720896 HRR655365:HRR720896 IBN655365:IBN720896 ILJ655365:ILJ720896 IVF655365:IVF720896 JFB655365:JFB720896 JOX655365:JOX720896 JYT655365:JYT720896 KIP655365:KIP720896 KSL655365:KSL720896 LCH655365:LCH720896 LMD655365:LMD720896 LVZ655365:LVZ720896 MFV655365:MFV720896 MPR655365:MPR720896 MZN655365:MZN720896 NJJ655365:NJJ720896 NTF655365:NTF720896 ODB655365:ODB720896 OMX655365:OMX720896 OWT655365:OWT720896 PGP655365:PGP720896 PQL655365:PQL720896 QAH655365:QAH720896 QKD655365:QKD720896 QTZ655365:QTZ720896 RDV655365:RDV720896 RNR655365:RNR720896 RXN655365:RXN720896 SHJ655365:SHJ720896 SRF655365:SRF720896 TBB655365:TBB720896 TKX655365:TKX720896 TUT655365:TUT720896 UEP655365:UEP720896 UOL655365:UOL720896 UYH655365:UYH720896 VID655365:VID720896 VRZ655365:VRZ720896 WBV655365:WBV720896 WLR655365:WLR720896 WVN655365:WVN720896 JB720901:JB786432 SX720901:SX786432 ACT720901:ACT786432 AMP720901:AMP786432 AWL720901:AWL786432 BGH720901:BGH786432 BQD720901:BQD786432 BZZ720901:BZZ786432 CJV720901:CJV786432 CTR720901:CTR786432 DDN720901:DDN786432 DNJ720901:DNJ786432 DXF720901:DXF786432 EHB720901:EHB786432 EQX720901:EQX786432 FAT720901:FAT786432 FKP720901:FKP786432 FUL720901:FUL786432 GEH720901:GEH786432 GOD720901:GOD786432 GXZ720901:GXZ786432 HHV720901:HHV786432 HRR720901:HRR786432 IBN720901:IBN786432 ILJ720901:ILJ786432 IVF720901:IVF786432 JFB720901:JFB786432 JOX720901:JOX786432 JYT720901:JYT786432 KIP720901:KIP786432 KSL720901:KSL786432 LCH720901:LCH786432 LMD720901:LMD786432 LVZ720901:LVZ786432 MFV720901:MFV786432 MPR720901:MPR786432 MZN720901:MZN786432 NJJ720901:NJJ786432 NTF720901:NTF786432 ODB720901:ODB786432 OMX720901:OMX786432 OWT720901:OWT786432 PGP720901:PGP786432 PQL720901:PQL786432 QAH720901:QAH786432 QKD720901:QKD786432 QTZ720901:QTZ786432 RDV720901:RDV786432 RNR720901:RNR786432 RXN720901:RXN786432 SHJ720901:SHJ786432 SRF720901:SRF786432 TBB720901:TBB786432 TKX720901:TKX786432 TUT720901:TUT786432 UEP720901:UEP786432 UOL720901:UOL786432 UYH720901:UYH786432 VID720901:VID786432 VRZ720901:VRZ786432 WBV720901:WBV786432 WLR720901:WLR786432 WVN720901:WVN786432 JB786437:JB851968 SX786437:SX851968 ACT786437:ACT851968 AMP786437:AMP851968 AWL786437:AWL851968 BGH786437:BGH851968 BQD786437:BQD851968 BZZ786437:BZZ851968 CJV786437:CJV851968 CTR786437:CTR851968 DDN786437:DDN851968 DNJ786437:DNJ851968 DXF786437:DXF851968 EHB786437:EHB851968 EQX786437:EQX851968 FAT786437:FAT851968 FKP786437:FKP851968 FUL786437:FUL851968 GEH786437:GEH851968 GOD786437:GOD851968 GXZ786437:GXZ851968 HHV786437:HHV851968 HRR786437:HRR851968 IBN786437:IBN851968 ILJ786437:ILJ851968 IVF786437:IVF851968 JFB786437:JFB851968 JOX786437:JOX851968 JYT786437:JYT851968 KIP786437:KIP851968 KSL786437:KSL851968 LCH786437:LCH851968 LMD786437:LMD851968 LVZ786437:LVZ851968 MFV786437:MFV851968 MPR786437:MPR851968 MZN786437:MZN851968 NJJ786437:NJJ851968 NTF786437:NTF851968 ODB786437:ODB851968 OMX786437:OMX851968 OWT786437:OWT851968 PGP786437:PGP851968 PQL786437:PQL851968 QAH786437:QAH851968 QKD786437:QKD851968 QTZ786437:QTZ851968 RDV786437:RDV851968 RNR786437:RNR851968 RXN786437:RXN851968 SHJ786437:SHJ851968 SRF786437:SRF851968 TBB786437:TBB851968 TKX786437:TKX851968 TUT786437:TUT851968 UEP786437:UEP851968 UOL786437:UOL851968 UYH786437:UYH851968 VID786437:VID851968 VRZ786437:VRZ851968 WBV786437:WBV851968 WLR786437:WLR851968 WVN786437:WVN851968 JB851973:JB917504 SX851973:SX917504 ACT851973:ACT917504 AMP851973:AMP917504 AWL851973:AWL917504 BGH851973:BGH917504 BQD851973:BQD917504 BZZ851973:BZZ917504 CJV851973:CJV917504 CTR851973:CTR917504 DDN851973:DDN917504 DNJ851973:DNJ917504 DXF851973:DXF917504 EHB851973:EHB917504 EQX851973:EQX917504 FAT851973:FAT917504 FKP851973:FKP917504 FUL851973:FUL917504 GEH851973:GEH917504 GOD851973:GOD917504 GXZ851973:GXZ917504 HHV851973:HHV917504 HRR851973:HRR917504 IBN851973:IBN917504 ILJ851973:ILJ917504 IVF851973:IVF917504 JFB851973:JFB917504 JOX851973:JOX917504 JYT851973:JYT917504 KIP851973:KIP917504 KSL851973:KSL917504 LCH851973:LCH917504 LMD851973:LMD917504 LVZ851973:LVZ917504 MFV851973:MFV917504 MPR851973:MPR917504 MZN851973:MZN917504 NJJ851973:NJJ917504 NTF851973:NTF917504 ODB851973:ODB917504 OMX851973:OMX917504 OWT851973:OWT917504 PGP851973:PGP917504 PQL851973:PQL917504 QAH851973:QAH917504 QKD851973:QKD917504 QTZ851973:QTZ917504 RDV851973:RDV917504 RNR851973:RNR917504 RXN851973:RXN917504 SHJ851973:SHJ917504 SRF851973:SRF917504 TBB851973:TBB917504 TKX851973:TKX917504 TUT851973:TUT917504 UEP851973:UEP917504 UOL851973:UOL917504 UYH851973:UYH917504 VID851973:VID917504 VRZ851973:VRZ917504 WBV851973:WBV917504 WLR851973:WLR917504 WVN851973:WVN917504 JB917509:JB983040 SX917509:SX983040 ACT917509:ACT983040 AMP917509:AMP983040 AWL917509:AWL983040 BGH917509:BGH983040 BQD917509:BQD983040 BZZ917509:BZZ983040 CJV917509:CJV983040 CTR917509:CTR983040 DDN917509:DDN983040 DNJ917509:DNJ983040 DXF917509:DXF983040 EHB917509:EHB983040 EQX917509:EQX983040 FAT917509:FAT983040 FKP917509:FKP983040 FUL917509:FUL983040 GEH917509:GEH983040 GOD917509:GOD983040 GXZ917509:GXZ983040 HHV917509:HHV983040 HRR917509:HRR983040 IBN917509:IBN983040 ILJ917509:ILJ983040 IVF917509:IVF983040 JFB917509:JFB983040 JOX917509:JOX983040 JYT917509:JYT983040 KIP917509:KIP983040 KSL917509:KSL983040 LCH917509:LCH983040 LMD917509:LMD983040 LVZ917509:LVZ983040 MFV917509:MFV983040 MPR917509:MPR983040 MZN917509:MZN983040 NJJ917509:NJJ983040 NTF917509:NTF983040 ODB917509:ODB983040 OMX917509:OMX983040 OWT917509:OWT983040 PGP917509:PGP983040 PQL917509:PQL983040 QAH917509:QAH983040 QKD917509:QKD983040 QTZ917509:QTZ983040 RDV917509:RDV983040 RNR917509:RNR983040 RXN917509:RXN983040 SHJ917509:SHJ983040 SRF917509:SRF983040 TBB917509:TBB983040 TKX917509:TKX983040 TUT917509:TUT983040 UEP917509:UEP983040 UOL917509:UOL983040 UYH917509:UYH983040 VID917509:VID983040 VRZ917509:VRZ983040 WBV917509:WBV983040 WLR917509:WLR983040 WVN917509:WVN983040 JB983045:JB1048576 SX983045:SX1048576 ACT983045:ACT1048576 AMP983045:AMP1048576 AWL983045:AWL1048576 BGH983045:BGH1048576 BQD983045:BQD1048576 BZZ983045:BZZ1048576 CJV983045:CJV1048576 CTR983045:CTR1048576 DDN983045:DDN1048576 DNJ983045:DNJ1048576 DXF983045:DXF1048576 EHB983045:EHB1048576 EQX983045:EQX1048576 FAT983045:FAT1048576 FKP983045:FKP1048576 FUL983045:FUL1048576 GEH983045:GEH1048576 GOD983045:GOD1048576 GXZ983045:GXZ1048576 HHV983045:HHV1048576 HRR983045:HRR1048576 IBN983045:IBN1048576 ILJ983045:ILJ1048576 IVF983045:IVF1048576 JFB983045:JFB1048576 JOX983045:JOX1048576 JYT983045:JYT1048576 KIP983045:KIP1048576 KSL983045:KSL1048576 LCH983045:LCH1048576 LMD983045:LMD1048576 LVZ983045:LVZ1048576 MFV983045:MFV1048576 MPR983045:MPR1048576 MZN983045:MZN1048576 NJJ983045:NJJ1048576 NTF983045:NTF1048576 ODB983045:ODB1048576 OMX983045:OMX1048576 OWT983045:OWT1048576 PGP983045:PGP1048576 PQL983045:PQL1048576 QAH983045:QAH1048576 QKD983045:QKD1048576 QTZ983045:QTZ1048576 RDV983045:RDV1048576 RNR983045:RNR1048576 RXN983045:RXN1048576 SHJ983045:SHJ1048576 SRF983045:SRF1048576 TBB983045:TBB1048576 TKX983045:TKX1048576 TUT983045:TUT1048576 UEP983045:UEP1048576 UOL983045:UOL1048576 UYH983045:UYH1048576 VID983045:VID1048576 VRZ983045:VRZ1048576 WBV983045:WBV1048576 WLR983045:WLR1048576">
+    <dataValidation type="list" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVN982992:WVN1048576 JB65488:JB131019 SX65488:SX131019 ACT65488:ACT131019 AMP65488:AMP131019 AWL65488:AWL131019 BGH65488:BGH131019 BQD65488:BQD131019 BZZ65488:BZZ131019 CJV65488:CJV131019 CTR65488:CTR131019 DDN65488:DDN131019 DNJ65488:DNJ131019 DXF65488:DXF131019 EHB65488:EHB131019 EQX65488:EQX131019 FAT65488:FAT131019 FKP65488:FKP131019 FUL65488:FUL131019 GEH65488:GEH131019 GOD65488:GOD131019 GXZ65488:GXZ131019 HHV65488:HHV131019 HRR65488:HRR131019 IBN65488:IBN131019 ILJ65488:ILJ131019 IVF65488:IVF131019 JFB65488:JFB131019 JOX65488:JOX131019 JYT65488:JYT131019 KIP65488:KIP131019 KSL65488:KSL131019 LCH65488:LCH131019 LMD65488:LMD131019 LVZ65488:LVZ131019 MFV65488:MFV131019 MPR65488:MPR131019 MZN65488:MZN131019 NJJ65488:NJJ131019 NTF65488:NTF131019 ODB65488:ODB131019 OMX65488:OMX131019 OWT65488:OWT131019 PGP65488:PGP131019 PQL65488:PQL131019 QAH65488:QAH131019 QKD65488:QKD131019 QTZ65488:QTZ131019 RDV65488:RDV131019 RNR65488:RNR131019 RXN65488:RXN131019 SHJ65488:SHJ131019 SRF65488:SRF131019 TBB65488:TBB131019 TKX65488:TKX131019 TUT65488:TUT131019 UEP65488:UEP131019 UOL65488:UOL131019 UYH65488:UYH131019 VID65488:VID131019 VRZ65488:VRZ131019 WBV65488:WBV131019 WLR65488:WLR131019 WVN65488:WVN131019 JB131024:JB196555 SX131024:SX196555 ACT131024:ACT196555 AMP131024:AMP196555 AWL131024:AWL196555 BGH131024:BGH196555 BQD131024:BQD196555 BZZ131024:BZZ196555 CJV131024:CJV196555 CTR131024:CTR196555 DDN131024:DDN196555 DNJ131024:DNJ196555 DXF131024:DXF196555 EHB131024:EHB196555 EQX131024:EQX196555 FAT131024:FAT196555 FKP131024:FKP196555 FUL131024:FUL196555 GEH131024:GEH196555 GOD131024:GOD196555 GXZ131024:GXZ196555 HHV131024:HHV196555 HRR131024:HRR196555 IBN131024:IBN196555 ILJ131024:ILJ196555 IVF131024:IVF196555 JFB131024:JFB196555 JOX131024:JOX196555 JYT131024:JYT196555 KIP131024:KIP196555 KSL131024:KSL196555 LCH131024:LCH196555 LMD131024:LMD196555 LVZ131024:LVZ196555 MFV131024:MFV196555 MPR131024:MPR196555 MZN131024:MZN196555 NJJ131024:NJJ196555 NTF131024:NTF196555 ODB131024:ODB196555 OMX131024:OMX196555 OWT131024:OWT196555 PGP131024:PGP196555 PQL131024:PQL196555 QAH131024:QAH196555 QKD131024:QKD196555 QTZ131024:QTZ196555 RDV131024:RDV196555 RNR131024:RNR196555 RXN131024:RXN196555 SHJ131024:SHJ196555 SRF131024:SRF196555 TBB131024:TBB196555 TKX131024:TKX196555 TUT131024:TUT196555 UEP131024:UEP196555 UOL131024:UOL196555 UYH131024:UYH196555 VID131024:VID196555 VRZ131024:VRZ196555 WBV131024:WBV196555 WLR131024:WLR196555 WVN131024:WVN196555 JB196560:JB262091 SX196560:SX262091 ACT196560:ACT262091 AMP196560:AMP262091 AWL196560:AWL262091 BGH196560:BGH262091 BQD196560:BQD262091 BZZ196560:BZZ262091 CJV196560:CJV262091 CTR196560:CTR262091 DDN196560:DDN262091 DNJ196560:DNJ262091 DXF196560:DXF262091 EHB196560:EHB262091 EQX196560:EQX262091 FAT196560:FAT262091 FKP196560:FKP262091 FUL196560:FUL262091 GEH196560:GEH262091 GOD196560:GOD262091 GXZ196560:GXZ262091 HHV196560:HHV262091 HRR196560:HRR262091 IBN196560:IBN262091 ILJ196560:ILJ262091 IVF196560:IVF262091 JFB196560:JFB262091 JOX196560:JOX262091 JYT196560:JYT262091 KIP196560:KIP262091 KSL196560:KSL262091 LCH196560:LCH262091 LMD196560:LMD262091 LVZ196560:LVZ262091 MFV196560:MFV262091 MPR196560:MPR262091 MZN196560:MZN262091 NJJ196560:NJJ262091 NTF196560:NTF262091 ODB196560:ODB262091 OMX196560:OMX262091 OWT196560:OWT262091 PGP196560:PGP262091 PQL196560:PQL262091 QAH196560:QAH262091 QKD196560:QKD262091 QTZ196560:QTZ262091 RDV196560:RDV262091 RNR196560:RNR262091 RXN196560:RXN262091 SHJ196560:SHJ262091 SRF196560:SRF262091 TBB196560:TBB262091 TKX196560:TKX262091 TUT196560:TUT262091 UEP196560:UEP262091 UOL196560:UOL262091 UYH196560:UYH262091 VID196560:VID262091 VRZ196560:VRZ262091 WBV196560:WBV262091 WLR196560:WLR262091 WVN196560:WVN262091 JB262096:JB327627 SX262096:SX327627 ACT262096:ACT327627 AMP262096:AMP327627 AWL262096:AWL327627 BGH262096:BGH327627 BQD262096:BQD327627 BZZ262096:BZZ327627 CJV262096:CJV327627 CTR262096:CTR327627 DDN262096:DDN327627 DNJ262096:DNJ327627 DXF262096:DXF327627 EHB262096:EHB327627 EQX262096:EQX327627 FAT262096:FAT327627 FKP262096:FKP327627 FUL262096:FUL327627 GEH262096:GEH327627 GOD262096:GOD327627 GXZ262096:GXZ327627 HHV262096:HHV327627 HRR262096:HRR327627 IBN262096:IBN327627 ILJ262096:ILJ327627 IVF262096:IVF327627 JFB262096:JFB327627 JOX262096:JOX327627 JYT262096:JYT327627 KIP262096:KIP327627 KSL262096:KSL327627 LCH262096:LCH327627 LMD262096:LMD327627 LVZ262096:LVZ327627 MFV262096:MFV327627 MPR262096:MPR327627 MZN262096:MZN327627 NJJ262096:NJJ327627 NTF262096:NTF327627 ODB262096:ODB327627 OMX262096:OMX327627 OWT262096:OWT327627 PGP262096:PGP327627 PQL262096:PQL327627 QAH262096:QAH327627 QKD262096:QKD327627 QTZ262096:QTZ327627 RDV262096:RDV327627 RNR262096:RNR327627 RXN262096:RXN327627 SHJ262096:SHJ327627 SRF262096:SRF327627 TBB262096:TBB327627 TKX262096:TKX327627 TUT262096:TUT327627 UEP262096:UEP327627 UOL262096:UOL327627 UYH262096:UYH327627 VID262096:VID327627 VRZ262096:VRZ327627 WBV262096:WBV327627 WLR262096:WLR327627 WVN262096:WVN327627 JB327632:JB393163 SX327632:SX393163 ACT327632:ACT393163 AMP327632:AMP393163 AWL327632:AWL393163 BGH327632:BGH393163 BQD327632:BQD393163 BZZ327632:BZZ393163 CJV327632:CJV393163 CTR327632:CTR393163 DDN327632:DDN393163 DNJ327632:DNJ393163 DXF327632:DXF393163 EHB327632:EHB393163 EQX327632:EQX393163 FAT327632:FAT393163 FKP327632:FKP393163 FUL327632:FUL393163 GEH327632:GEH393163 GOD327632:GOD393163 GXZ327632:GXZ393163 HHV327632:HHV393163 HRR327632:HRR393163 IBN327632:IBN393163 ILJ327632:ILJ393163 IVF327632:IVF393163 JFB327632:JFB393163 JOX327632:JOX393163 JYT327632:JYT393163 KIP327632:KIP393163 KSL327632:KSL393163 LCH327632:LCH393163 LMD327632:LMD393163 LVZ327632:LVZ393163 MFV327632:MFV393163 MPR327632:MPR393163 MZN327632:MZN393163 NJJ327632:NJJ393163 NTF327632:NTF393163 ODB327632:ODB393163 OMX327632:OMX393163 OWT327632:OWT393163 PGP327632:PGP393163 PQL327632:PQL393163 QAH327632:QAH393163 QKD327632:QKD393163 QTZ327632:QTZ393163 RDV327632:RDV393163 RNR327632:RNR393163 RXN327632:RXN393163 SHJ327632:SHJ393163 SRF327632:SRF393163 TBB327632:TBB393163 TKX327632:TKX393163 TUT327632:TUT393163 UEP327632:UEP393163 UOL327632:UOL393163 UYH327632:UYH393163 VID327632:VID393163 VRZ327632:VRZ393163 WBV327632:WBV393163 WLR327632:WLR393163 WVN327632:WVN393163 JB393168:JB458699 SX393168:SX458699 ACT393168:ACT458699 AMP393168:AMP458699 AWL393168:AWL458699 BGH393168:BGH458699 BQD393168:BQD458699 BZZ393168:BZZ458699 CJV393168:CJV458699 CTR393168:CTR458699 DDN393168:DDN458699 DNJ393168:DNJ458699 DXF393168:DXF458699 EHB393168:EHB458699 EQX393168:EQX458699 FAT393168:FAT458699 FKP393168:FKP458699 FUL393168:FUL458699 GEH393168:GEH458699 GOD393168:GOD458699 GXZ393168:GXZ458699 HHV393168:HHV458699 HRR393168:HRR458699 IBN393168:IBN458699 ILJ393168:ILJ458699 IVF393168:IVF458699 JFB393168:JFB458699 JOX393168:JOX458699 JYT393168:JYT458699 KIP393168:KIP458699 KSL393168:KSL458699 LCH393168:LCH458699 LMD393168:LMD458699 LVZ393168:LVZ458699 MFV393168:MFV458699 MPR393168:MPR458699 MZN393168:MZN458699 NJJ393168:NJJ458699 NTF393168:NTF458699 ODB393168:ODB458699 OMX393168:OMX458699 OWT393168:OWT458699 PGP393168:PGP458699 PQL393168:PQL458699 QAH393168:QAH458699 QKD393168:QKD458699 QTZ393168:QTZ458699 RDV393168:RDV458699 RNR393168:RNR458699 RXN393168:RXN458699 SHJ393168:SHJ458699 SRF393168:SRF458699 TBB393168:TBB458699 TKX393168:TKX458699 TUT393168:TUT458699 UEP393168:UEP458699 UOL393168:UOL458699 UYH393168:UYH458699 VID393168:VID458699 VRZ393168:VRZ458699 WBV393168:WBV458699 WLR393168:WLR458699 WVN393168:WVN458699 JB458704:JB524235 SX458704:SX524235 ACT458704:ACT524235 AMP458704:AMP524235 AWL458704:AWL524235 BGH458704:BGH524235 BQD458704:BQD524235 BZZ458704:BZZ524235 CJV458704:CJV524235 CTR458704:CTR524235 DDN458704:DDN524235 DNJ458704:DNJ524235 DXF458704:DXF524235 EHB458704:EHB524235 EQX458704:EQX524235 FAT458704:FAT524235 FKP458704:FKP524235 FUL458704:FUL524235 GEH458704:GEH524235 GOD458704:GOD524235 GXZ458704:GXZ524235 HHV458704:HHV524235 HRR458704:HRR524235 IBN458704:IBN524235 ILJ458704:ILJ524235 IVF458704:IVF524235 JFB458704:JFB524235 JOX458704:JOX524235 JYT458704:JYT524235 KIP458704:KIP524235 KSL458704:KSL524235 LCH458704:LCH524235 LMD458704:LMD524235 LVZ458704:LVZ524235 MFV458704:MFV524235 MPR458704:MPR524235 MZN458704:MZN524235 NJJ458704:NJJ524235 NTF458704:NTF524235 ODB458704:ODB524235 OMX458704:OMX524235 OWT458704:OWT524235 PGP458704:PGP524235 PQL458704:PQL524235 QAH458704:QAH524235 QKD458704:QKD524235 QTZ458704:QTZ524235 RDV458704:RDV524235 RNR458704:RNR524235 RXN458704:RXN524235 SHJ458704:SHJ524235 SRF458704:SRF524235 TBB458704:TBB524235 TKX458704:TKX524235 TUT458704:TUT524235 UEP458704:UEP524235 UOL458704:UOL524235 UYH458704:UYH524235 VID458704:VID524235 VRZ458704:VRZ524235 WBV458704:WBV524235 WLR458704:WLR524235 WVN458704:WVN524235 JB524240:JB589771 SX524240:SX589771 ACT524240:ACT589771 AMP524240:AMP589771 AWL524240:AWL589771 BGH524240:BGH589771 BQD524240:BQD589771 BZZ524240:BZZ589771 CJV524240:CJV589771 CTR524240:CTR589771 DDN524240:DDN589771 DNJ524240:DNJ589771 DXF524240:DXF589771 EHB524240:EHB589771 EQX524240:EQX589771 FAT524240:FAT589771 FKP524240:FKP589771 FUL524240:FUL589771 GEH524240:GEH589771 GOD524240:GOD589771 GXZ524240:GXZ589771 HHV524240:HHV589771 HRR524240:HRR589771 IBN524240:IBN589771 ILJ524240:ILJ589771 IVF524240:IVF589771 JFB524240:JFB589771 JOX524240:JOX589771 JYT524240:JYT589771 KIP524240:KIP589771 KSL524240:KSL589771 LCH524240:LCH589771 LMD524240:LMD589771 LVZ524240:LVZ589771 MFV524240:MFV589771 MPR524240:MPR589771 MZN524240:MZN589771 NJJ524240:NJJ589771 NTF524240:NTF589771 ODB524240:ODB589771 OMX524240:OMX589771 OWT524240:OWT589771 PGP524240:PGP589771 PQL524240:PQL589771 QAH524240:QAH589771 QKD524240:QKD589771 QTZ524240:QTZ589771 RDV524240:RDV589771 RNR524240:RNR589771 RXN524240:RXN589771 SHJ524240:SHJ589771 SRF524240:SRF589771 TBB524240:TBB589771 TKX524240:TKX589771 TUT524240:TUT589771 UEP524240:UEP589771 UOL524240:UOL589771 UYH524240:UYH589771 VID524240:VID589771 VRZ524240:VRZ589771 WBV524240:WBV589771 WLR524240:WLR589771 WVN524240:WVN589771 JB589776:JB655307 SX589776:SX655307 ACT589776:ACT655307 AMP589776:AMP655307 AWL589776:AWL655307 BGH589776:BGH655307 BQD589776:BQD655307 BZZ589776:BZZ655307 CJV589776:CJV655307 CTR589776:CTR655307 DDN589776:DDN655307 DNJ589776:DNJ655307 DXF589776:DXF655307 EHB589776:EHB655307 EQX589776:EQX655307 FAT589776:FAT655307 FKP589776:FKP655307 FUL589776:FUL655307 GEH589776:GEH655307 GOD589776:GOD655307 GXZ589776:GXZ655307 HHV589776:HHV655307 HRR589776:HRR655307 IBN589776:IBN655307 ILJ589776:ILJ655307 IVF589776:IVF655307 JFB589776:JFB655307 JOX589776:JOX655307 JYT589776:JYT655307 KIP589776:KIP655307 KSL589776:KSL655307 LCH589776:LCH655307 LMD589776:LMD655307 LVZ589776:LVZ655307 MFV589776:MFV655307 MPR589776:MPR655307 MZN589776:MZN655307 NJJ589776:NJJ655307 NTF589776:NTF655307 ODB589776:ODB655307 OMX589776:OMX655307 OWT589776:OWT655307 PGP589776:PGP655307 PQL589776:PQL655307 QAH589776:QAH655307 QKD589776:QKD655307 QTZ589776:QTZ655307 RDV589776:RDV655307 RNR589776:RNR655307 RXN589776:RXN655307 SHJ589776:SHJ655307 SRF589776:SRF655307 TBB589776:TBB655307 TKX589776:TKX655307 TUT589776:TUT655307 UEP589776:UEP655307 UOL589776:UOL655307 UYH589776:UYH655307 VID589776:VID655307 VRZ589776:VRZ655307 WBV589776:WBV655307 WLR589776:WLR655307 WVN589776:WVN655307 JB655312:JB720843 SX655312:SX720843 ACT655312:ACT720843 AMP655312:AMP720843 AWL655312:AWL720843 BGH655312:BGH720843 BQD655312:BQD720843 BZZ655312:BZZ720843 CJV655312:CJV720843 CTR655312:CTR720843 DDN655312:DDN720843 DNJ655312:DNJ720843 DXF655312:DXF720843 EHB655312:EHB720843 EQX655312:EQX720843 FAT655312:FAT720843 FKP655312:FKP720843 FUL655312:FUL720843 GEH655312:GEH720843 GOD655312:GOD720843 GXZ655312:GXZ720843 HHV655312:HHV720843 HRR655312:HRR720843 IBN655312:IBN720843 ILJ655312:ILJ720843 IVF655312:IVF720843 JFB655312:JFB720843 JOX655312:JOX720843 JYT655312:JYT720843 KIP655312:KIP720843 KSL655312:KSL720843 LCH655312:LCH720843 LMD655312:LMD720843 LVZ655312:LVZ720843 MFV655312:MFV720843 MPR655312:MPR720843 MZN655312:MZN720843 NJJ655312:NJJ720843 NTF655312:NTF720843 ODB655312:ODB720843 OMX655312:OMX720843 OWT655312:OWT720843 PGP655312:PGP720843 PQL655312:PQL720843 QAH655312:QAH720843 QKD655312:QKD720843 QTZ655312:QTZ720843 RDV655312:RDV720843 RNR655312:RNR720843 RXN655312:RXN720843 SHJ655312:SHJ720843 SRF655312:SRF720843 TBB655312:TBB720843 TKX655312:TKX720843 TUT655312:TUT720843 UEP655312:UEP720843 UOL655312:UOL720843 UYH655312:UYH720843 VID655312:VID720843 VRZ655312:VRZ720843 WBV655312:WBV720843 WLR655312:WLR720843 WVN655312:WVN720843 JB720848:JB786379 SX720848:SX786379 ACT720848:ACT786379 AMP720848:AMP786379 AWL720848:AWL786379 BGH720848:BGH786379 BQD720848:BQD786379 BZZ720848:BZZ786379 CJV720848:CJV786379 CTR720848:CTR786379 DDN720848:DDN786379 DNJ720848:DNJ786379 DXF720848:DXF786379 EHB720848:EHB786379 EQX720848:EQX786379 FAT720848:FAT786379 FKP720848:FKP786379 FUL720848:FUL786379 GEH720848:GEH786379 GOD720848:GOD786379 GXZ720848:GXZ786379 HHV720848:HHV786379 HRR720848:HRR786379 IBN720848:IBN786379 ILJ720848:ILJ786379 IVF720848:IVF786379 JFB720848:JFB786379 JOX720848:JOX786379 JYT720848:JYT786379 KIP720848:KIP786379 KSL720848:KSL786379 LCH720848:LCH786379 LMD720848:LMD786379 LVZ720848:LVZ786379 MFV720848:MFV786379 MPR720848:MPR786379 MZN720848:MZN786379 NJJ720848:NJJ786379 NTF720848:NTF786379 ODB720848:ODB786379 OMX720848:OMX786379 OWT720848:OWT786379 PGP720848:PGP786379 PQL720848:PQL786379 QAH720848:QAH786379 QKD720848:QKD786379 QTZ720848:QTZ786379 RDV720848:RDV786379 RNR720848:RNR786379 RXN720848:RXN786379 SHJ720848:SHJ786379 SRF720848:SRF786379 TBB720848:TBB786379 TKX720848:TKX786379 TUT720848:TUT786379 UEP720848:UEP786379 UOL720848:UOL786379 UYH720848:UYH786379 VID720848:VID786379 VRZ720848:VRZ786379 WBV720848:WBV786379 WLR720848:WLR786379 WVN720848:WVN786379 JB786384:JB851915 SX786384:SX851915 ACT786384:ACT851915 AMP786384:AMP851915 AWL786384:AWL851915 BGH786384:BGH851915 BQD786384:BQD851915 BZZ786384:BZZ851915 CJV786384:CJV851915 CTR786384:CTR851915 DDN786384:DDN851915 DNJ786384:DNJ851915 DXF786384:DXF851915 EHB786384:EHB851915 EQX786384:EQX851915 FAT786384:FAT851915 FKP786384:FKP851915 FUL786384:FUL851915 GEH786384:GEH851915 GOD786384:GOD851915 GXZ786384:GXZ851915 HHV786384:HHV851915 HRR786384:HRR851915 IBN786384:IBN851915 ILJ786384:ILJ851915 IVF786384:IVF851915 JFB786384:JFB851915 JOX786384:JOX851915 JYT786384:JYT851915 KIP786384:KIP851915 KSL786384:KSL851915 LCH786384:LCH851915 LMD786384:LMD851915 LVZ786384:LVZ851915 MFV786384:MFV851915 MPR786384:MPR851915 MZN786384:MZN851915 NJJ786384:NJJ851915 NTF786384:NTF851915 ODB786384:ODB851915 OMX786384:OMX851915 OWT786384:OWT851915 PGP786384:PGP851915 PQL786384:PQL851915 QAH786384:QAH851915 QKD786384:QKD851915 QTZ786384:QTZ851915 RDV786384:RDV851915 RNR786384:RNR851915 RXN786384:RXN851915 SHJ786384:SHJ851915 SRF786384:SRF851915 TBB786384:TBB851915 TKX786384:TKX851915 TUT786384:TUT851915 UEP786384:UEP851915 UOL786384:UOL851915 UYH786384:UYH851915 VID786384:VID851915 VRZ786384:VRZ851915 WBV786384:WBV851915 WLR786384:WLR851915 WVN786384:WVN851915 JB851920:JB917451 SX851920:SX917451 ACT851920:ACT917451 AMP851920:AMP917451 AWL851920:AWL917451 BGH851920:BGH917451 BQD851920:BQD917451 BZZ851920:BZZ917451 CJV851920:CJV917451 CTR851920:CTR917451 DDN851920:DDN917451 DNJ851920:DNJ917451 DXF851920:DXF917451 EHB851920:EHB917451 EQX851920:EQX917451 FAT851920:FAT917451 FKP851920:FKP917451 FUL851920:FUL917451 GEH851920:GEH917451 GOD851920:GOD917451 GXZ851920:GXZ917451 HHV851920:HHV917451 HRR851920:HRR917451 IBN851920:IBN917451 ILJ851920:ILJ917451 IVF851920:IVF917451 JFB851920:JFB917451 JOX851920:JOX917451 JYT851920:JYT917451 KIP851920:KIP917451 KSL851920:KSL917451 LCH851920:LCH917451 LMD851920:LMD917451 LVZ851920:LVZ917451 MFV851920:MFV917451 MPR851920:MPR917451 MZN851920:MZN917451 NJJ851920:NJJ917451 NTF851920:NTF917451 ODB851920:ODB917451 OMX851920:OMX917451 OWT851920:OWT917451 PGP851920:PGP917451 PQL851920:PQL917451 QAH851920:QAH917451 QKD851920:QKD917451 QTZ851920:QTZ917451 RDV851920:RDV917451 RNR851920:RNR917451 RXN851920:RXN917451 SHJ851920:SHJ917451 SRF851920:SRF917451 TBB851920:TBB917451 TKX851920:TKX917451 TUT851920:TUT917451 UEP851920:UEP917451 UOL851920:UOL917451 UYH851920:UYH917451 VID851920:VID917451 VRZ851920:VRZ917451 WBV851920:WBV917451 WLR851920:WLR917451 WVN851920:WVN917451 JB917456:JB982987 SX917456:SX982987 ACT917456:ACT982987 AMP917456:AMP982987 AWL917456:AWL982987 BGH917456:BGH982987 BQD917456:BQD982987 BZZ917456:BZZ982987 CJV917456:CJV982987 CTR917456:CTR982987 DDN917456:DDN982987 DNJ917456:DNJ982987 DXF917456:DXF982987 EHB917456:EHB982987 EQX917456:EQX982987 FAT917456:FAT982987 FKP917456:FKP982987 FUL917456:FUL982987 GEH917456:GEH982987 GOD917456:GOD982987 GXZ917456:GXZ982987 HHV917456:HHV982987 HRR917456:HRR982987 IBN917456:IBN982987 ILJ917456:ILJ982987 IVF917456:IVF982987 JFB917456:JFB982987 JOX917456:JOX982987 JYT917456:JYT982987 KIP917456:KIP982987 KSL917456:KSL982987 LCH917456:LCH982987 LMD917456:LMD982987 LVZ917456:LVZ982987 MFV917456:MFV982987 MPR917456:MPR982987 MZN917456:MZN982987 NJJ917456:NJJ982987 NTF917456:NTF982987 ODB917456:ODB982987 OMX917456:OMX982987 OWT917456:OWT982987 PGP917456:PGP982987 PQL917456:PQL982987 QAH917456:QAH982987 QKD917456:QKD982987 QTZ917456:QTZ982987 RDV917456:RDV982987 RNR917456:RNR982987 RXN917456:RXN982987 SHJ917456:SHJ982987 SRF917456:SRF982987 TBB917456:TBB982987 TKX917456:TKX982987 TUT917456:TUT982987 UEP917456:UEP982987 UOL917456:UOL982987 UYH917456:UYH982987 VID917456:VID982987 VRZ917456:VRZ982987 WBV917456:WBV982987 WLR917456:WLR982987 WVN917456:WVN982987 JB982992:JB1048576 SX982992:SX1048576 ACT982992:ACT1048576 AMP982992:AMP1048576 AWL982992:AWL1048576 BGH982992:BGH1048576 BQD982992:BQD1048576 BZZ982992:BZZ1048576 CJV982992:CJV1048576 CTR982992:CTR1048576 DDN982992:DDN1048576 DNJ982992:DNJ1048576 DXF982992:DXF1048576 EHB982992:EHB1048576 EQX982992:EQX1048576 FAT982992:FAT1048576 FKP982992:FKP1048576 FUL982992:FUL1048576 GEH982992:GEH1048576 GOD982992:GOD1048576 GXZ982992:GXZ1048576 HHV982992:HHV1048576 HRR982992:HRR1048576 IBN982992:IBN1048576 ILJ982992:ILJ1048576 IVF982992:IVF1048576 JFB982992:JFB1048576 JOX982992:JOX1048576 JYT982992:JYT1048576 KIP982992:KIP1048576 KSL982992:KSL1048576 LCH982992:LCH1048576 LMD982992:LMD1048576 LVZ982992:LVZ1048576 MFV982992:MFV1048576 MPR982992:MPR1048576 MZN982992:MZN1048576 NJJ982992:NJJ1048576 NTF982992:NTF1048576 ODB982992:ODB1048576 OMX982992:OMX1048576 OWT982992:OWT1048576 PGP982992:PGP1048576 PQL982992:PQL1048576 QAH982992:QAH1048576 QKD982992:QKD1048576 QTZ982992:QTZ1048576 RDV982992:RDV1048576 RNR982992:RNR1048576 RXN982992:RXN1048576 SHJ982992:SHJ1048576 SRF982992:SRF1048576 TBB982992:TBB1048576 TKX982992:TKX1048576 TUT982992:TUT1048576 UEP982992:UEP1048576 UOL982992:UOL1048576 UYH982992:UYH1048576 VID982992:VID1048576 VRZ982992:VRZ1048576 WBV982992:WBV1048576 WLR982992:WLR1048576 JB5:JB65483 SX5:SX65483 ACT5:ACT65483 AMP5:AMP65483 AWL5:AWL65483 BGH5:BGH65483 BQD5:BQD65483 BZZ5:BZZ65483 CJV5:CJV65483 CTR5:CTR65483 DDN5:DDN65483 DNJ5:DNJ65483 DXF5:DXF65483 EHB5:EHB65483 EQX5:EQX65483 FAT5:FAT65483 FKP5:FKP65483 FUL5:FUL65483 GEH5:GEH65483 GOD5:GOD65483 GXZ5:GXZ65483 HHV5:HHV65483 HRR5:HRR65483 IBN5:IBN65483 ILJ5:ILJ65483 IVF5:IVF65483 JFB5:JFB65483 JOX5:JOX65483 JYT5:JYT65483 KIP5:KIP65483 KSL5:KSL65483 LCH5:LCH65483 LMD5:LMD65483 LVZ5:LVZ65483 MFV5:MFV65483 MPR5:MPR65483 MZN5:MZN65483 NJJ5:NJJ65483 NTF5:NTF65483 ODB5:ODB65483 OMX5:OMX65483 OWT5:OWT65483 PGP5:PGP65483 PQL5:PQL65483 QAH5:QAH65483 QKD5:QKD65483 QTZ5:QTZ65483 RDV5:RDV65483 RNR5:RNR65483 RXN5:RXN65483 SHJ5:SHJ65483 SRF5:SRF65483 TBB5:TBB65483 TKX5:TKX65483 TUT5:TUT65483 UEP5:UEP65483 UOL5:UOL65483 UYH5:UYH65483 VID5:VID65483 VRZ5:VRZ65483 WBV5:WBV65483 WLR5:WLR65483 WVN5:WVN65483">
       <formula1>"."</formula1>
     </dataValidation>
   </dataValidations>
@@ -2089,11 +2281,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="13.5"/>
@@ -2285,13 +2477,13 @@
         <v>42</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2299,13 +2491,13 @@
         <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>166</v>
+        <v>265</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2313,13 +2505,13 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2327,13 +2519,13 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2341,13 +2533,13 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2355,13 +2547,13 @@
         <v>42</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2369,13 +2561,13 @@
         <v>42</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2383,38 +2575,66 @@
         <v>42</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>270</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -2442,12 +2662,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F5" sqref="F5"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2564,7 +2784,7 @@
         <v>65</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2631,7 +2851,7 @@
         <v>95</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2686,7 +2906,7 @@
         <v>96</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2719,7 +2939,7 @@
         <v>126</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2757,7 +2977,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C33" t="s">
         <v>43</v>
@@ -2765,15 +2985,15 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>72</v>
@@ -2781,31 +3001,31 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="4" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>92</v>
@@ -2813,16 +3033,115 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="C40" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>261</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>262</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>260</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>266</v>
+      </c>
+      <c r="C44" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>267</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>274</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>275</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>276</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>277</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B52" t="s">
+        <v>244</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="textLength" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="数据长度错误" error="数据长度必须在6-35个字符之间" sqref="C26 C12:C13 C10 C5:C6 C21 C32:C37 C39">
+    <dataValidation type="textLength" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="数据长度错误" error="数据长度必须在6-35个字符之间" sqref="C26 C12:C13 C10 C5:C6 C21 C32:C37 C39 C41 C43 C45 C47:C52">
       <formula1>6</formula1>
       <formula2>35</formula2>
     </dataValidation>
@@ -2836,7 +3155,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
@@ -2894,7 +3213,7 @@
         <v>7771</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2905,7 +3224,7 @@
         <v>7772</v>
       </c>
       <c r="C7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2916,7 +3235,7 @@
         <v>7773</v>
       </c>
       <c r="C8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2927,7 +3246,7 @@
         <v>7774</v>
       </c>
       <c r="C9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2938,7 +3257,7 @@
         <v>7775</v>
       </c>
       <c r="C10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2949,7 +3268,7 @@
         <v>7776</v>
       </c>
       <c r="C11" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2960,7 +3279,7 @@
         <v>7777</v>
       </c>
       <c r="C12" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2971,7 +3290,7 @@
         <v>7778</v>
       </c>
       <c r="C13" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2982,7 +3301,7 @@
         <v>7779</v>
       </c>
       <c r="C14" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2993,7 +3312,7 @@
         <v>7780</v>
       </c>
       <c r="C15" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -3004,7 +3323,7 @@
         <v>7781</v>
       </c>
       <c r="C16" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3015,7 +3334,7 @@
         <v>7782</v>
       </c>
       <c r="C17" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3106,7 +3425,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3131,6 +3450,9 @@
       </c>
     </row>
     <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>255</v>
+      </c>
       <c r="B5" s="5" t="s">
         <v>110</v>
       </c>
@@ -3182,7 +3504,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3208,7 +3530,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>157</v>
+        <v>256</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>110</v>
@@ -3239,7 +3561,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3264,6 +3586,9 @@
       </c>
     </row>
     <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>256</v>
+      </c>
       <c r="B5" s="5" t="s">
         <v>110</v>
       </c>
@@ -3323,226 +3648,226 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="9"/>
+    <col min="1" max="1" width="14.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" s="8">
+        <v>7</v>
+      </c>
+      <c r="G5" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" s="8">
+        <v>7</v>
+      </c>
+      <c r="G6" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" s="8">
+        <v>7</v>
+      </c>
+      <c r="G7" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="D8" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="F8" s="8">
+        <v>7</v>
+      </c>
+      <c r="G8" s="8">
         <v>6</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="F5" s="9">
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="F9" s="8">
         <v>7</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G9" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="F6" s="9">
+    <row r="10" spans="1:7">
+      <c r="A10" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F10" s="8">
         <v>7</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G10" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="F7" s="9">
+    <row r="11" spans="1:7">
+      <c r="A11" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="F11" s="8">
         <v>7</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G11" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="F8" s="9">
+    <row r="12" spans="1:7">
+      <c r="A12" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F12" s="8">
         <v>7</v>
       </c>
-      <c r="G8" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="F9" s="9">
-        <v>7</v>
-      </c>
-      <c r="G9" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="F10" s="9">
-        <v>7</v>
-      </c>
-      <c r="G10" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="F11" s="9">
-        <v>7</v>
-      </c>
-      <c r="G11" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="F12" s="9">
-        <v>7</v>
-      </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
# add report xxbcrp.p.
</commit_message>
<xml_diff>
--- a/bookmg/initial/cim.xlsx
+++ b/bookmg/initial/cim.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="2505" windowWidth="14295" windowHeight="7020" tabRatio="944"/>
+    <workbookView xWindow="9555" yWindow="2505" windowWidth="14295" windowHeight="7020" tabRatio="944" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="00-mgmemt.p" sheetId="8" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="304">
   <si>
     <t>mgmsgmt.p</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1377,6 +1377,83 @@
   <si>
     <t>读者借阅统计</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_bctype</t>
+  </si>
+  <si>
+    <t>v_bcstat</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_latecnt</t>
+  </si>
+  <si>
+    <t>v_onhand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIMES_LATE </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>延迟次数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>延迟</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_bc1</t>
+  </si>
+  <si>
+    <t>TO</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ON_HAND_BOOK_COUNT</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>尚未归还</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>未还</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ON_HAND_LATE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>延迟未还</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_onlate</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_maxlate</t>
+  </si>
+  <si>
+    <t>MAX_LATE_DAYS</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>最长延迟天数</t>
+  </si>
+  <si>
+    <t>v_late</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_bkname</t>
   </si>
 </sst>
 </file>
@@ -1869,11 +1946,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5"/>
@@ -2281,11 +2358,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="13.5"/>
@@ -2637,6 +2714,59 @@
         <v>280</v>
       </c>
     </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>290</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>290</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>290</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C26" t="s">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="6">
@@ -2645,7 +2775,7 @@
       <formula1>"EN,CH,TW"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="数据有效" prompt="数据长度必须在6-35个字符之间，且不能包含汉字。" sqref="B4 IX4 ST4 ACP4 AML4 AWH4 BGD4 BPZ4 BZV4 CJR4 CTN4 DDJ4 DNF4 DXB4 EGX4 EQT4 FAP4 FKL4 FUH4 GED4 GNZ4 GXV4 HHR4 HRN4 IBJ4 ILF4 IVB4 JEX4 JOT4 JYP4 KIL4 KSH4 LCD4 LLZ4 LVV4 MFR4 MPN4 MZJ4 NJF4 NTB4 OCX4 OMT4 OWP4 PGL4 PQH4 QAD4 QJZ4 QTV4 RDR4 RNN4 RXJ4 SHF4 SRB4 TAX4 TKT4 TUP4 UEL4 UOH4 UYD4 VHZ4 VRV4 WBR4 WLN4 WVJ4 B65540 IX65540 ST65540 ACP65540 AML65540 AWH65540 BGD65540 BPZ65540 BZV65540 CJR65540 CTN65540 DDJ65540 DNF65540 DXB65540 EGX65540 EQT65540 FAP65540 FKL65540 FUH65540 GED65540 GNZ65540 GXV65540 HHR65540 HRN65540 IBJ65540 ILF65540 IVB65540 JEX65540 JOT65540 JYP65540 KIL65540 KSH65540 LCD65540 LLZ65540 LVV65540 MFR65540 MPN65540 MZJ65540 NJF65540 NTB65540 OCX65540 OMT65540 OWP65540 PGL65540 PQH65540 QAD65540 QJZ65540 QTV65540 RDR65540 RNN65540 RXJ65540 SHF65540 SRB65540 TAX65540 TKT65540 TUP65540 UEL65540 UOH65540 UYD65540 VHZ65540 VRV65540 WBR65540 WLN65540 WVJ65540 B131076 IX131076 ST131076 ACP131076 AML131076 AWH131076 BGD131076 BPZ131076 BZV131076 CJR131076 CTN131076 DDJ131076 DNF131076 DXB131076 EGX131076 EQT131076 FAP131076 FKL131076 FUH131076 GED131076 GNZ131076 GXV131076 HHR131076 HRN131076 IBJ131076 ILF131076 IVB131076 JEX131076 JOT131076 JYP131076 KIL131076 KSH131076 LCD131076 LLZ131076 LVV131076 MFR131076 MPN131076 MZJ131076 NJF131076 NTB131076 OCX131076 OMT131076 OWP131076 PGL131076 PQH131076 QAD131076 QJZ131076 QTV131076 RDR131076 RNN131076 RXJ131076 SHF131076 SRB131076 TAX131076 TKT131076 TUP131076 UEL131076 UOH131076 UYD131076 VHZ131076 VRV131076 WBR131076 WLN131076 WVJ131076 B196612 IX196612 ST196612 ACP196612 AML196612 AWH196612 BGD196612 BPZ196612 BZV196612 CJR196612 CTN196612 DDJ196612 DNF196612 DXB196612 EGX196612 EQT196612 FAP196612 FKL196612 FUH196612 GED196612 GNZ196612 GXV196612 HHR196612 HRN196612 IBJ196612 ILF196612 IVB196612 JEX196612 JOT196612 JYP196612 KIL196612 KSH196612 LCD196612 LLZ196612 LVV196612 MFR196612 MPN196612 MZJ196612 NJF196612 NTB196612 OCX196612 OMT196612 OWP196612 PGL196612 PQH196612 QAD196612 QJZ196612 QTV196612 RDR196612 RNN196612 RXJ196612 SHF196612 SRB196612 TAX196612 TKT196612 TUP196612 UEL196612 UOH196612 UYD196612 VHZ196612 VRV196612 WBR196612 WLN196612 WVJ196612 B262148 IX262148 ST262148 ACP262148 AML262148 AWH262148 BGD262148 BPZ262148 BZV262148 CJR262148 CTN262148 DDJ262148 DNF262148 DXB262148 EGX262148 EQT262148 FAP262148 FKL262148 FUH262148 GED262148 GNZ262148 GXV262148 HHR262148 HRN262148 IBJ262148 ILF262148 IVB262148 JEX262148 JOT262148 JYP262148 KIL262148 KSH262148 LCD262148 LLZ262148 LVV262148 MFR262148 MPN262148 MZJ262148 NJF262148 NTB262148 OCX262148 OMT262148 OWP262148 PGL262148 PQH262148 QAD262148 QJZ262148 QTV262148 RDR262148 RNN262148 RXJ262148 SHF262148 SRB262148 TAX262148 TKT262148 TUP262148 UEL262148 UOH262148 UYD262148 VHZ262148 VRV262148 WBR262148 WLN262148 WVJ262148 B327684 IX327684 ST327684 ACP327684 AML327684 AWH327684 BGD327684 BPZ327684 BZV327684 CJR327684 CTN327684 DDJ327684 DNF327684 DXB327684 EGX327684 EQT327684 FAP327684 FKL327684 FUH327684 GED327684 GNZ327684 GXV327684 HHR327684 HRN327684 IBJ327684 ILF327684 IVB327684 JEX327684 JOT327684 JYP327684 KIL327684 KSH327684 LCD327684 LLZ327684 LVV327684 MFR327684 MPN327684 MZJ327684 NJF327684 NTB327684 OCX327684 OMT327684 OWP327684 PGL327684 PQH327684 QAD327684 QJZ327684 QTV327684 RDR327684 RNN327684 RXJ327684 SHF327684 SRB327684 TAX327684 TKT327684 TUP327684 UEL327684 UOH327684 UYD327684 VHZ327684 VRV327684 WBR327684 WLN327684 WVJ327684 B393220 IX393220 ST393220 ACP393220 AML393220 AWH393220 BGD393220 BPZ393220 BZV393220 CJR393220 CTN393220 DDJ393220 DNF393220 DXB393220 EGX393220 EQT393220 FAP393220 FKL393220 FUH393220 GED393220 GNZ393220 GXV393220 HHR393220 HRN393220 IBJ393220 ILF393220 IVB393220 JEX393220 JOT393220 JYP393220 KIL393220 KSH393220 LCD393220 LLZ393220 LVV393220 MFR393220 MPN393220 MZJ393220 NJF393220 NTB393220 OCX393220 OMT393220 OWP393220 PGL393220 PQH393220 QAD393220 QJZ393220 QTV393220 RDR393220 RNN393220 RXJ393220 SHF393220 SRB393220 TAX393220 TKT393220 TUP393220 UEL393220 UOH393220 UYD393220 VHZ393220 VRV393220 WBR393220 WLN393220 WVJ393220 B458756 IX458756 ST458756 ACP458756 AML458756 AWH458756 BGD458756 BPZ458756 BZV458756 CJR458756 CTN458756 DDJ458756 DNF458756 DXB458756 EGX458756 EQT458756 FAP458756 FKL458756 FUH458756 GED458756 GNZ458756 GXV458756 HHR458756 HRN458756 IBJ458756 ILF458756 IVB458756 JEX458756 JOT458756 JYP458756 KIL458756 KSH458756 LCD458756 LLZ458756 LVV458756 MFR458756 MPN458756 MZJ458756 NJF458756 NTB458756 OCX458756 OMT458756 OWP458756 PGL458756 PQH458756 QAD458756 QJZ458756 QTV458756 RDR458756 RNN458756 RXJ458756 SHF458756 SRB458756 TAX458756 TKT458756 TUP458756 UEL458756 UOH458756 UYD458756 VHZ458756 VRV458756 WBR458756 WLN458756 WVJ458756 B524292 IX524292 ST524292 ACP524292 AML524292 AWH524292 BGD524292 BPZ524292 BZV524292 CJR524292 CTN524292 DDJ524292 DNF524292 DXB524292 EGX524292 EQT524292 FAP524292 FKL524292 FUH524292 GED524292 GNZ524292 GXV524292 HHR524292 HRN524292 IBJ524292 ILF524292 IVB524292 JEX524292 JOT524292 JYP524292 KIL524292 KSH524292 LCD524292 LLZ524292 LVV524292 MFR524292 MPN524292 MZJ524292 NJF524292 NTB524292 OCX524292 OMT524292 OWP524292 PGL524292 PQH524292 QAD524292 QJZ524292 QTV524292 RDR524292 RNN524292 RXJ524292 SHF524292 SRB524292 TAX524292 TKT524292 TUP524292 UEL524292 UOH524292 UYD524292 VHZ524292 VRV524292 WBR524292 WLN524292 WVJ524292 B589828 IX589828 ST589828 ACP589828 AML589828 AWH589828 BGD589828 BPZ589828 BZV589828 CJR589828 CTN589828 DDJ589828 DNF589828 DXB589828 EGX589828 EQT589828 FAP589828 FKL589828 FUH589828 GED589828 GNZ589828 GXV589828 HHR589828 HRN589828 IBJ589828 ILF589828 IVB589828 JEX589828 JOT589828 JYP589828 KIL589828 KSH589828 LCD589828 LLZ589828 LVV589828 MFR589828 MPN589828 MZJ589828 NJF589828 NTB589828 OCX589828 OMT589828 OWP589828 PGL589828 PQH589828 QAD589828 QJZ589828 QTV589828 RDR589828 RNN589828 RXJ589828 SHF589828 SRB589828 TAX589828 TKT589828 TUP589828 UEL589828 UOH589828 UYD589828 VHZ589828 VRV589828 WBR589828 WLN589828 WVJ589828 B655364 IX655364 ST655364 ACP655364 AML655364 AWH655364 BGD655364 BPZ655364 BZV655364 CJR655364 CTN655364 DDJ655364 DNF655364 DXB655364 EGX655364 EQT655364 FAP655364 FKL655364 FUH655364 GED655364 GNZ655364 GXV655364 HHR655364 HRN655364 IBJ655364 ILF655364 IVB655364 JEX655364 JOT655364 JYP655364 KIL655364 KSH655364 LCD655364 LLZ655364 LVV655364 MFR655364 MPN655364 MZJ655364 NJF655364 NTB655364 OCX655364 OMT655364 OWP655364 PGL655364 PQH655364 QAD655364 QJZ655364 QTV655364 RDR655364 RNN655364 RXJ655364 SHF655364 SRB655364 TAX655364 TKT655364 TUP655364 UEL655364 UOH655364 UYD655364 VHZ655364 VRV655364 WBR655364 WLN655364 WVJ655364 B720900 IX720900 ST720900 ACP720900 AML720900 AWH720900 BGD720900 BPZ720900 BZV720900 CJR720900 CTN720900 DDJ720900 DNF720900 DXB720900 EGX720900 EQT720900 FAP720900 FKL720900 FUH720900 GED720900 GNZ720900 GXV720900 HHR720900 HRN720900 IBJ720900 ILF720900 IVB720900 JEX720900 JOT720900 JYP720900 KIL720900 KSH720900 LCD720900 LLZ720900 LVV720900 MFR720900 MPN720900 MZJ720900 NJF720900 NTB720900 OCX720900 OMT720900 OWP720900 PGL720900 PQH720900 QAD720900 QJZ720900 QTV720900 RDR720900 RNN720900 RXJ720900 SHF720900 SRB720900 TAX720900 TKT720900 TUP720900 UEL720900 UOH720900 UYD720900 VHZ720900 VRV720900 WBR720900 WLN720900 WVJ720900 B786436 IX786436 ST786436 ACP786436 AML786436 AWH786436 BGD786436 BPZ786436 BZV786436 CJR786436 CTN786436 DDJ786436 DNF786436 DXB786436 EGX786436 EQT786436 FAP786436 FKL786436 FUH786436 GED786436 GNZ786436 GXV786436 HHR786436 HRN786436 IBJ786436 ILF786436 IVB786436 JEX786436 JOT786436 JYP786436 KIL786436 KSH786436 LCD786436 LLZ786436 LVV786436 MFR786436 MPN786436 MZJ786436 NJF786436 NTB786436 OCX786436 OMT786436 OWP786436 PGL786436 PQH786436 QAD786436 QJZ786436 QTV786436 RDR786436 RNN786436 RXJ786436 SHF786436 SRB786436 TAX786436 TKT786436 TUP786436 UEL786436 UOH786436 UYD786436 VHZ786436 VRV786436 WBR786436 WLN786436 WVJ786436 B851972 IX851972 ST851972 ACP851972 AML851972 AWH851972 BGD851972 BPZ851972 BZV851972 CJR851972 CTN851972 DDJ851972 DNF851972 DXB851972 EGX851972 EQT851972 FAP851972 FKL851972 FUH851972 GED851972 GNZ851972 GXV851972 HHR851972 HRN851972 IBJ851972 ILF851972 IVB851972 JEX851972 JOT851972 JYP851972 KIL851972 KSH851972 LCD851972 LLZ851972 LVV851972 MFR851972 MPN851972 MZJ851972 NJF851972 NTB851972 OCX851972 OMT851972 OWP851972 PGL851972 PQH851972 QAD851972 QJZ851972 QTV851972 RDR851972 RNN851972 RXJ851972 SHF851972 SRB851972 TAX851972 TKT851972 TUP851972 UEL851972 UOH851972 UYD851972 VHZ851972 VRV851972 WBR851972 WLN851972 WVJ851972 B917508 IX917508 ST917508 ACP917508 AML917508 AWH917508 BGD917508 BPZ917508 BZV917508 CJR917508 CTN917508 DDJ917508 DNF917508 DXB917508 EGX917508 EQT917508 FAP917508 FKL917508 FUH917508 GED917508 GNZ917508 GXV917508 HHR917508 HRN917508 IBJ917508 ILF917508 IVB917508 JEX917508 JOT917508 JYP917508 KIL917508 KSH917508 LCD917508 LLZ917508 LVV917508 MFR917508 MPN917508 MZJ917508 NJF917508 NTB917508 OCX917508 OMT917508 OWP917508 PGL917508 PQH917508 QAD917508 QJZ917508 QTV917508 RDR917508 RNN917508 RXJ917508 SHF917508 SRB917508 TAX917508 TKT917508 TUP917508 UEL917508 UOH917508 UYD917508 VHZ917508 VRV917508 WBR917508 WLN917508 WVJ917508 B983044 IX983044 ST983044 ACP983044 AML983044 AWH983044 BGD983044 BPZ983044 BZV983044 CJR983044 CTN983044 DDJ983044 DNF983044 DXB983044 EGX983044 EQT983044 FAP983044 FKL983044 FUH983044 GED983044 GNZ983044 GXV983044 HHR983044 HRN983044 IBJ983044 ILF983044 IVB983044 JEX983044 JOT983044 JYP983044 KIL983044 KSH983044 LCD983044 LLZ983044 LVV983044 MFR983044 MPN983044 MZJ983044 NJF983044 NTB983044 OCX983044 OMT983044 OWP983044 PGL983044 PQH983044 QAD983044 QJZ983044 QTV983044 RDR983044 RNN983044 RXJ983044 SHF983044 SRB983044 TAX983044 TKT983044 TUP983044 UEL983044 UOH983044 UYD983044 VHZ983044 VRV983044 WBR983044 WLN983044 WVJ983044"/>
-    <dataValidation type="textLength" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="数据长度错误" error="数据长度必须在6-35个字符之间" sqref="WVJ983045:WVJ1048576 IX5:IX65536 ST5:ST65536 ACP5:ACP65536 AML5:AML65536 AWH5:AWH65536 BGD5:BGD65536 BPZ5:BPZ65536 BZV5:BZV65536 CJR5:CJR65536 CTN5:CTN65536 DDJ5:DDJ65536 DNF5:DNF65536 DXB5:DXB65536 EGX5:EGX65536 EQT5:EQT65536 FAP5:FAP65536 FKL5:FKL65536 FUH5:FUH65536 GED5:GED65536 GNZ5:GNZ65536 GXV5:GXV65536 HHR5:HHR65536 HRN5:HRN65536 IBJ5:IBJ65536 ILF5:ILF65536 IVB5:IVB65536 JEX5:JEX65536 JOT5:JOT65536 JYP5:JYP65536 KIL5:KIL65536 KSH5:KSH65536 LCD5:LCD65536 LLZ5:LLZ65536 LVV5:LVV65536 MFR5:MFR65536 MPN5:MPN65536 MZJ5:MZJ65536 NJF5:NJF65536 NTB5:NTB65536 OCX5:OCX65536 OMT5:OMT65536 OWP5:OWP65536 PGL5:PGL65536 PQH5:PQH65536 QAD5:QAD65536 QJZ5:QJZ65536 QTV5:QTV65536 RDR5:RDR65536 RNN5:RNN65536 RXJ5:RXJ65536 SHF5:SHF65536 SRB5:SRB65536 TAX5:TAX65536 TKT5:TKT65536 TUP5:TUP65536 UEL5:UEL65536 UOH5:UOH65536 UYD5:UYD65536 VHZ5:VHZ65536 VRV5:VRV65536 WBR5:WBR65536 WLN5:WLN65536 WVJ5:WVJ65536 B65541:B131072 IX65541:IX131072 ST65541:ST131072 ACP65541:ACP131072 AML65541:AML131072 AWH65541:AWH131072 BGD65541:BGD131072 BPZ65541:BPZ131072 BZV65541:BZV131072 CJR65541:CJR131072 CTN65541:CTN131072 DDJ65541:DDJ131072 DNF65541:DNF131072 DXB65541:DXB131072 EGX65541:EGX131072 EQT65541:EQT131072 FAP65541:FAP131072 FKL65541:FKL131072 FUH65541:FUH131072 GED65541:GED131072 GNZ65541:GNZ131072 GXV65541:GXV131072 HHR65541:HHR131072 HRN65541:HRN131072 IBJ65541:IBJ131072 ILF65541:ILF131072 IVB65541:IVB131072 JEX65541:JEX131072 JOT65541:JOT131072 JYP65541:JYP131072 KIL65541:KIL131072 KSH65541:KSH131072 LCD65541:LCD131072 LLZ65541:LLZ131072 LVV65541:LVV131072 MFR65541:MFR131072 MPN65541:MPN131072 MZJ65541:MZJ131072 NJF65541:NJF131072 NTB65541:NTB131072 OCX65541:OCX131072 OMT65541:OMT131072 OWP65541:OWP131072 PGL65541:PGL131072 PQH65541:PQH131072 QAD65541:QAD131072 QJZ65541:QJZ131072 QTV65541:QTV131072 RDR65541:RDR131072 RNN65541:RNN131072 RXJ65541:RXJ131072 SHF65541:SHF131072 SRB65541:SRB131072 TAX65541:TAX131072 TKT65541:TKT131072 TUP65541:TUP131072 UEL65541:UEL131072 UOH65541:UOH131072 UYD65541:UYD131072 VHZ65541:VHZ131072 VRV65541:VRV131072 WBR65541:WBR131072 WLN65541:WLN131072 WVJ65541:WVJ131072 B131077:B196608 IX131077:IX196608 ST131077:ST196608 ACP131077:ACP196608 AML131077:AML196608 AWH131077:AWH196608 BGD131077:BGD196608 BPZ131077:BPZ196608 BZV131077:BZV196608 CJR131077:CJR196608 CTN131077:CTN196608 DDJ131077:DDJ196608 DNF131077:DNF196608 DXB131077:DXB196608 EGX131077:EGX196608 EQT131077:EQT196608 FAP131077:FAP196608 FKL131077:FKL196608 FUH131077:FUH196608 GED131077:GED196608 GNZ131077:GNZ196608 GXV131077:GXV196608 HHR131077:HHR196608 HRN131077:HRN196608 IBJ131077:IBJ196608 ILF131077:ILF196608 IVB131077:IVB196608 JEX131077:JEX196608 JOT131077:JOT196608 JYP131077:JYP196608 KIL131077:KIL196608 KSH131077:KSH196608 LCD131077:LCD196608 LLZ131077:LLZ196608 LVV131077:LVV196608 MFR131077:MFR196608 MPN131077:MPN196608 MZJ131077:MZJ196608 NJF131077:NJF196608 NTB131077:NTB196608 OCX131077:OCX196608 OMT131077:OMT196608 OWP131077:OWP196608 PGL131077:PGL196608 PQH131077:PQH196608 QAD131077:QAD196608 QJZ131077:QJZ196608 QTV131077:QTV196608 RDR131077:RDR196608 RNN131077:RNN196608 RXJ131077:RXJ196608 SHF131077:SHF196608 SRB131077:SRB196608 TAX131077:TAX196608 TKT131077:TKT196608 TUP131077:TUP196608 UEL131077:UEL196608 UOH131077:UOH196608 UYD131077:UYD196608 VHZ131077:VHZ196608 VRV131077:VRV196608 WBR131077:WBR196608 WLN131077:WLN196608 WVJ131077:WVJ196608 B196613:B262144 IX196613:IX262144 ST196613:ST262144 ACP196613:ACP262144 AML196613:AML262144 AWH196613:AWH262144 BGD196613:BGD262144 BPZ196613:BPZ262144 BZV196613:BZV262144 CJR196613:CJR262144 CTN196613:CTN262144 DDJ196613:DDJ262144 DNF196613:DNF262144 DXB196613:DXB262144 EGX196613:EGX262144 EQT196613:EQT262144 FAP196613:FAP262144 FKL196613:FKL262144 FUH196613:FUH262144 GED196613:GED262144 GNZ196613:GNZ262144 GXV196613:GXV262144 HHR196613:HHR262144 HRN196613:HRN262144 IBJ196613:IBJ262144 ILF196613:ILF262144 IVB196613:IVB262144 JEX196613:JEX262144 JOT196613:JOT262144 JYP196613:JYP262144 KIL196613:KIL262144 KSH196613:KSH262144 LCD196613:LCD262144 LLZ196613:LLZ262144 LVV196613:LVV262144 MFR196613:MFR262144 MPN196613:MPN262144 MZJ196613:MZJ262144 NJF196613:NJF262144 NTB196613:NTB262144 OCX196613:OCX262144 OMT196613:OMT262144 OWP196613:OWP262144 PGL196613:PGL262144 PQH196613:PQH262144 QAD196613:QAD262144 QJZ196613:QJZ262144 QTV196613:QTV262144 RDR196613:RDR262144 RNN196613:RNN262144 RXJ196613:RXJ262144 SHF196613:SHF262144 SRB196613:SRB262144 TAX196613:TAX262144 TKT196613:TKT262144 TUP196613:TUP262144 UEL196613:UEL262144 UOH196613:UOH262144 UYD196613:UYD262144 VHZ196613:VHZ262144 VRV196613:VRV262144 WBR196613:WBR262144 WLN196613:WLN262144 WVJ196613:WVJ262144 B262149:B327680 IX262149:IX327680 ST262149:ST327680 ACP262149:ACP327680 AML262149:AML327680 AWH262149:AWH327680 BGD262149:BGD327680 BPZ262149:BPZ327680 BZV262149:BZV327680 CJR262149:CJR327680 CTN262149:CTN327680 DDJ262149:DDJ327680 DNF262149:DNF327680 DXB262149:DXB327680 EGX262149:EGX327680 EQT262149:EQT327680 FAP262149:FAP327680 FKL262149:FKL327680 FUH262149:FUH327680 GED262149:GED327680 GNZ262149:GNZ327680 GXV262149:GXV327680 HHR262149:HHR327680 HRN262149:HRN327680 IBJ262149:IBJ327680 ILF262149:ILF327680 IVB262149:IVB327680 JEX262149:JEX327680 JOT262149:JOT327680 JYP262149:JYP327680 KIL262149:KIL327680 KSH262149:KSH327680 LCD262149:LCD327680 LLZ262149:LLZ327680 LVV262149:LVV327680 MFR262149:MFR327680 MPN262149:MPN327680 MZJ262149:MZJ327680 NJF262149:NJF327680 NTB262149:NTB327680 OCX262149:OCX327680 OMT262149:OMT327680 OWP262149:OWP327680 PGL262149:PGL327680 PQH262149:PQH327680 QAD262149:QAD327680 QJZ262149:QJZ327680 QTV262149:QTV327680 RDR262149:RDR327680 RNN262149:RNN327680 RXJ262149:RXJ327680 SHF262149:SHF327680 SRB262149:SRB327680 TAX262149:TAX327680 TKT262149:TKT327680 TUP262149:TUP327680 UEL262149:UEL327680 UOH262149:UOH327680 UYD262149:UYD327680 VHZ262149:VHZ327680 VRV262149:VRV327680 WBR262149:WBR327680 WLN262149:WLN327680 WVJ262149:WVJ327680 B327685:B393216 IX327685:IX393216 ST327685:ST393216 ACP327685:ACP393216 AML327685:AML393216 AWH327685:AWH393216 BGD327685:BGD393216 BPZ327685:BPZ393216 BZV327685:BZV393216 CJR327685:CJR393216 CTN327685:CTN393216 DDJ327685:DDJ393216 DNF327685:DNF393216 DXB327685:DXB393216 EGX327685:EGX393216 EQT327685:EQT393216 FAP327685:FAP393216 FKL327685:FKL393216 FUH327685:FUH393216 GED327685:GED393216 GNZ327685:GNZ393216 GXV327685:GXV393216 HHR327685:HHR393216 HRN327685:HRN393216 IBJ327685:IBJ393216 ILF327685:ILF393216 IVB327685:IVB393216 JEX327685:JEX393216 JOT327685:JOT393216 JYP327685:JYP393216 KIL327685:KIL393216 KSH327685:KSH393216 LCD327685:LCD393216 LLZ327685:LLZ393216 LVV327685:LVV393216 MFR327685:MFR393216 MPN327685:MPN393216 MZJ327685:MZJ393216 NJF327685:NJF393216 NTB327685:NTB393216 OCX327685:OCX393216 OMT327685:OMT393216 OWP327685:OWP393216 PGL327685:PGL393216 PQH327685:PQH393216 QAD327685:QAD393216 QJZ327685:QJZ393216 QTV327685:QTV393216 RDR327685:RDR393216 RNN327685:RNN393216 RXJ327685:RXJ393216 SHF327685:SHF393216 SRB327685:SRB393216 TAX327685:TAX393216 TKT327685:TKT393216 TUP327685:TUP393216 UEL327685:UEL393216 UOH327685:UOH393216 UYD327685:UYD393216 VHZ327685:VHZ393216 VRV327685:VRV393216 WBR327685:WBR393216 WLN327685:WLN393216 WVJ327685:WVJ393216 B393221:B458752 IX393221:IX458752 ST393221:ST458752 ACP393221:ACP458752 AML393221:AML458752 AWH393221:AWH458752 BGD393221:BGD458752 BPZ393221:BPZ458752 BZV393221:BZV458752 CJR393221:CJR458752 CTN393221:CTN458752 DDJ393221:DDJ458752 DNF393221:DNF458752 DXB393221:DXB458752 EGX393221:EGX458752 EQT393221:EQT458752 FAP393221:FAP458752 FKL393221:FKL458752 FUH393221:FUH458752 GED393221:GED458752 GNZ393221:GNZ458752 GXV393221:GXV458752 HHR393221:HHR458752 HRN393221:HRN458752 IBJ393221:IBJ458752 ILF393221:ILF458752 IVB393221:IVB458752 JEX393221:JEX458752 JOT393221:JOT458752 JYP393221:JYP458752 KIL393221:KIL458752 KSH393221:KSH458752 LCD393221:LCD458752 LLZ393221:LLZ458752 LVV393221:LVV458752 MFR393221:MFR458752 MPN393221:MPN458752 MZJ393221:MZJ458752 NJF393221:NJF458752 NTB393221:NTB458752 OCX393221:OCX458752 OMT393221:OMT458752 OWP393221:OWP458752 PGL393221:PGL458752 PQH393221:PQH458752 QAD393221:QAD458752 QJZ393221:QJZ458752 QTV393221:QTV458752 RDR393221:RDR458752 RNN393221:RNN458752 RXJ393221:RXJ458752 SHF393221:SHF458752 SRB393221:SRB458752 TAX393221:TAX458752 TKT393221:TKT458752 TUP393221:TUP458752 UEL393221:UEL458752 UOH393221:UOH458752 UYD393221:UYD458752 VHZ393221:VHZ458752 VRV393221:VRV458752 WBR393221:WBR458752 WLN393221:WLN458752 WVJ393221:WVJ458752 B458757:B524288 IX458757:IX524288 ST458757:ST524288 ACP458757:ACP524288 AML458757:AML524288 AWH458757:AWH524288 BGD458757:BGD524288 BPZ458757:BPZ524288 BZV458757:BZV524288 CJR458757:CJR524288 CTN458757:CTN524288 DDJ458757:DDJ524288 DNF458757:DNF524288 DXB458757:DXB524288 EGX458757:EGX524288 EQT458757:EQT524288 FAP458757:FAP524288 FKL458757:FKL524288 FUH458757:FUH524288 GED458757:GED524288 GNZ458757:GNZ524288 GXV458757:GXV524288 HHR458757:HHR524288 HRN458757:HRN524288 IBJ458757:IBJ524288 ILF458757:ILF524288 IVB458757:IVB524288 JEX458757:JEX524288 JOT458757:JOT524288 JYP458757:JYP524288 KIL458757:KIL524288 KSH458757:KSH524288 LCD458757:LCD524288 LLZ458757:LLZ524288 LVV458757:LVV524288 MFR458757:MFR524288 MPN458757:MPN524288 MZJ458757:MZJ524288 NJF458757:NJF524288 NTB458757:NTB524288 OCX458757:OCX524288 OMT458757:OMT524288 OWP458757:OWP524288 PGL458757:PGL524288 PQH458757:PQH524288 QAD458757:QAD524288 QJZ458757:QJZ524288 QTV458757:QTV524288 RDR458757:RDR524288 RNN458757:RNN524288 RXJ458757:RXJ524288 SHF458757:SHF524288 SRB458757:SRB524288 TAX458757:TAX524288 TKT458757:TKT524288 TUP458757:TUP524288 UEL458757:UEL524288 UOH458757:UOH524288 UYD458757:UYD524288 VHZ458757:VHZ524288 VRV458757:VRV524288 WBR458757:WBR524288 WLN458757:WLN524288 WVJ458757:WVJ524288 B524293:B589824 IX524293:IX589824 ST524293:ST589824 ACP524293:ACP589824 AML524293:AML589824 AWH524293:AWH589824 BGD524293:BGD589824 BPZ524293:BPZ589824 BZV524293:BZV589824 CJR524293:CJR589824 CTN524293:CTN589824 DDJ524293:DDJ589824 DNF524293:DNF589824 DXB524293:DXB589824 EGX524293:EGX589824 EQT524293:EQT589824 FAP524293:FAP589824 FKL524293:FKL589824 FUH524293:FUH589824 GED524293:GED589824 GNZ524293:GNZ589824 GXV524293:GXV589824 HHR524293:HHR589824 HRN524293:HRN589824 IBJ524293:IBJ589824 ILF524293:ILF589824 IVB524293:IVB589824 JEX524293:JEX589824 JOT524293:JOT589824 JYP524293:JYP589824 KIL524293:KIL589824 KSH524293:KSH589824 LCD524293:LCD589824 LLZ524293:LLZ589824 LVV524293:LVV589824 MFR524293:MFR589824 MPN524293:MPN589824 MZJ524293:MZJ589824 NJF524293:NJF589824 NTB524293:NTB589824 OCX524293:OCX589824 OMT524293:OMT589824 OWP524293:OWP589824 PGL524293:PGL589824 PQH524293:PQH589824 QAD524293:QAD589824 QJZ524293:QJZ589824 QTV524293:QTV589824 RDR524293:RDR589824 RNN524293:RNN589824 RXJ524293:RXJ589824 SHF524293:SHF589824 SRB524293:SRB589824 TAX524293:TAX589824 TKT524293:TKT589824 TUP524293:TUP589824 UEL524293:UEL589824 UOH524293:UOH589824 UYD524293:UYD589824 VHZ524293:VHZ589824 VRV524293:VRV589824 WBR524293:WBR589824 WLN524293:WLN589824 WVJ524293:WVJ589824 B589829:B655360 IX589829:IX655360 ST589829:ST655360 ACP589829:ACP655360 AML589829:AML655360 AWH589829:AWH655360 BGD589829:BGD655360 BPZ589829:BPZ655360 BZV589829:BZV655360 CJR589829:CJR655360 CTN589829:CTN655360 DDJ589829:DDJ655360 DNF589829:DNF655360 DXB589829:DXB655360 EGX589829:EGX655360 EQT589829:EQT655360 FAP589829:FAP655360 FKL589829:FKL655360 FUH589829:FUH655360 GED589829:GED655360 GNZ589829:GNZ655360 GXV589829:GXV655360 HHR589829:HHR655360 HRN589829:HRN655360 IBJ589829:IBJ655360 ILF589829:ILF655360 IVB589829:IVB655360 JEX589829:JEX655360 JOT589829:JOT655360 JYP589829:JYP655360 KIL589829:KIL655360 KSH589829:KSH655360 LCD589829:LCD655360 LLZ589829:LLZ655360 LVV589829:LVV655360 MFR589829:MFR655360 MPN589829:MPN655360 MZJ589829:MZJ655360 NJF589829:NJF655360 NTB589829:NTB655360 OCX589829:OCX655360 OMT589829:OMT655360 OWP589829:OWP655360 PGL589829:PGL655360 PQH589829:PQH655360 QAD589829:QAD655360 QJZ589829:QJZ655360 QTV589829:QTV655360 RDR589829:RDR655360 RNN589829:RNN655360 RXJ589829:RXJ655360 SHF589829:SHF655360 SRB589829:SRB655360 TAX589829:TAX655360 TKT589829:TKT655360 TUP589829:TUP655360 UEL589829:UEL655360 UOH589829:UOH655360 UYD589829:UYD655360 VHZ589829:VHZ655360 VRV589829:VRV655360 WBR589829:WBR655360 WLN589829:WLN655360 WVJ589829:WVJ655360 B655365:B720896 IX655365:IX720896 ST655365:ST720896 ACP655365:ACP720896 AML655365:AML720896 AWH655365:AWH720896 BGD655365:BGD720896 BPZ655365:BPZ720896 BZV655365:BZV720896 CJR655365:CJR720896 CTN655365:CTN720896 DDJ655365:DDJ720896 DNF655365:DNF720896 DXB655365:DXB720896 EGX655365:EGX720896 EQT655365:EQT720896 FAP655365:FAP720896 FKL655365:FKL720896 FUH655365:FUH720896 GED655365:GED720896 GNZ655365:GNZ720896 GXV655365:GXV720896 HHR655365:HHR720896 HRN655365:HRN720896 IBJ655365:IBJ720896 ILF655365:ILF720896 IVB655365:IVB720896 JEX655365:JEX720896 JOT655365:JOT720896 JYP655365:JYP720896 KIL655365:KIL720896 KSH655365:KSH720896 LCD655365:LCD720896 LLZ655365:LLZ720896 LVV655365:LVV720896 MFR655365:MFR720896 MPN655365:MPN720896 MZJ655365:MZJ720896 NJF655365:NJF720896 NTB655365:NTB720896 OCX655365:OCX720896 OMT655365:OMT720896 OWP655365:OWP720896 PGL655365:PGL720896 PQH655365:PQH720896 QAD655365:QAD720896 QJZ655365:QJZ720896 QTV655365:QTV720896 RDR655365:RDR720896 RNN655365:RNN720896 RXJ655365:RXJ720896 SHF655365:SHF720896 SRB655365:SRB720896 TAX655365:TAX720896 TKT655365:TKT720896 TUP655365:TUP720896 UEL655365:UEL720896 UOH655365:UOH720896 UYD655365:UYD720896 VHZ655365:VHZ720896 VRV655365:VRV720896 WBR655365:WBR720896 WLN655365:WLN720896 WVJ655365:WVJ720896 B720901:B786432 IX720901:IX786432 ST720901:ST786432 ACP720901:ACP786432 AML720901:AML786432 AWH720901:AWH786432 BGD720901:BGD786432 BPZ720901:BPZ786432 BZV720901:BZV786432 CJR720901:CJR786432 CTN720901:CTN786432 DDJ720901:DDJ786432 DNF720901:DNF786432 DXB720901:DXB786432 EGX720901:EGX786432 EQT720901:EQT786432 FAP720901:FAP786432 FKL720901:FKL786432 FUH720901:FUH786432 GED720901:GED786432 GNZ720901:GNZ786432 GXV720901:GXV786432 HHR720901:HHR786432 HRN720901:HRN786432 IBJ720901:IBJ786432 ILF720901:ILF786432 IVB720901:IVB786432 JEX720901:JEX786432 JOT720901:JOT786432 JYP720901:JYP786432 KIL720901:KIL786432 KSH720901:KSH786432 LCD720901:LCD786432 LLZ720901:LLZ786432 LVV720901:LVV786432 MFR720901:MFR786432 MPN720901:MPN786432 MZJ720901:MZJ786432 NJF720901:NJF786432 NTB720901:NTB786432 OCX720901:OCX786432 OMT720901:OMT786432 OWP720901:OWP786432 PGL720901:PGL786432 PQH720901:PQH786432 QAD720901:QAD786432 QJZ720901:QJZ786432 QTV720901:QTV786432 RDR720901:RDR786432 RNN720901:RNN786432 RXJ720901:RXJ786432 SHF720901:SHF786432 SRB720901:SRB786432 TAX720901:TAX786432 TKT720901:TKT786432 TUP720901:TUP786432 UEL720901:UEL786432 UOH720901:UOH786432 UYD720901:UYD786432 VHZ720901:VHZ786432 VRV720901:VRV786432 WBR720901:WBR786432 WLN720901:WLN786432 WVJ720901:WVJ786432 B786437:B851968 IX786437:IX851968 ST786437:ST851968 ACP786437:ACP851968 AML786437:AML851968 AWH786437:AWH851968 BGD786437:BGD851968 BPZ786437:BPZ851968 BZV786437:BZV851968 CJR786437:CJR851968 CTN786437:CTN851968 DDJ786437:DDJ851968 DNF786437:DNF851968 DXB786437:DXB851968 EGX786437:EGX851968 EQT786437:EQT851968 FAP786437:FAP851968 FKL786437:FKL851968 FUH786437:FUH851968 GED786437:GED851968 GNZ786437:GNZ851968 GXV786437:GXV851968 HHR786437:HHR851968 HRN786437:HRN851968 IBJ786437:IBJ851968 ILF786437:ILF851968 IVB786437:IVB851968 JEX786437:JEX851968 JOT786437:JOT851968 JYP786437:JYP851968 KIL786437:KIL851968 KSH786437:KSH851968 LCD786437:LCD851968 LLZ786437:LLZ851968 LVV786437:LVV851968 MFR786437:MFR851968 MPN786437:MPN851968 MZJ786437:MZJ851968 NJF786437:NJF851968 NTB786437:NTB851968 OCX786437:OCX851968 OMT786437:OMT851968 OWP786437:OWP851968 PGL786437:PGL851968 PQH786437:PQH851968 QAD786437:QAD851968 QJZ786437:QJZ851968 QTV786437:QTV851968 RDR786437:RDR851968 RNN786437:RNN851968 RXJ786437:RXJ851968 SHF786437:SHF851968 SRB786437:SRB851968 TAX786437:TAX851968 TKT786437:TKT851968 TUP786437:TUP851968 UEL786437:UEL851968 UOH786437:UOH851968 UYD786437:UYD851968 VHZ786437:VHZ851968 VRV786437:VRV851968 WBR786437:WBR851968 WLN786437:WLN851968 WVJ786437:WVJ851968 B851973:B917504 IX851973:IX917504 ST851973:ST917504 ACP851973:ACP917504 AML851973:AML917504 AWH851973:AWH917504 BGD851973:BGD917504 BPZ851973:BPZ917504 BZV851973:BZV917504 CJR851973:CJR917504 CTN851973:CTN917504 DDJ851973:DDJ917504 DNF851973:DNF917504 DXB851973:DXB917504 EGX851973:EGX917504 EQT851973:EQT917504 FAP851973:FAP917504 FKL851973:FKL917504 FUH851973:FUH917504 GED851973:GED917504 GNZ851973:GNZ917504 GXV851973:GXV917504 HHR851973:HHR917504 HRN851973:HRN917504 IBJ851973:IBJ917504 ILF851973:ILF917504 IVB851973:IVB917504 JEX851973:JEX917504 JOT851973:JOT917504 JYP851973:JYP917504 KIL851973:KIL917504 KSH851973:KSH917504 LCD851973:LCD917504 LLZ851973:LLZ917504 LVV851973:LVV917504 MFR851973:MFR917504 MPN851973:MPN917504 MZJ851973:MZJ917504 NJF851973:NJF917504 NTB851973:NTB917504 OCX851973:OCX917504 OMT851973:OMT917504 OWP851973:OWP917504 PGL851973:PGL917504 PQH851973:PQH917504 QAD851973:QAD917504 QJZ851973:QJZ917504 QTV851973:QTV917504 RDR851973:RDR917504 RNN851973:RNN917504 RXJ851973:RXJ917504 SHF851973:SHF917504 SRB851973:SRB917504 TAX851973:TAX917504 TKT851973:TKT917504 TUP851973:TUP917504 UEL851973:UEL917504 UOH851973:UOH917504 UYD851973:UYD917504 VHZ851973:VHZ917504 VRV851973:VRV917504 WBR851973:WBR917504 WLN851973:WLN917504 WVJ851973:WVJ917504 B917509:B983040 IX917509:IX983040 ST917509:ST983040 ACP917509:ACP983040 AML917509:AML983040 AWH917509:AWH983040 BGD917509:BGD983040 BPZ917509:BPZ983040 BZV917509:BZV983040 CJR917509:CJR983040 CTN917509:CTN983040 DDJ917509:DDJ983040 DNF917509:DNF983040 DXB917509:DXB983040 EGX917509:EGX983040 EQT917509:EQT983040 FAP917509:FAP983040 FKL917509:FKL983040 FUH917509:FUH983040 GED917509:GED983040 GNZ917509:GNZ983040 GXV917509:GXV983040 HHR917509:HHR983040 HRN917509:HRN983040 IBJ917509:IBJ983040 ILF917509:ILF983040 IVB917509:IVB983040 JEX917509:JEX983040 JOT917509:JOT983040 JYP917509:JYP983040 KIL917509:KIL983040 KSH917509:KSH983040 LCD917509:LCD983040 LLZ917509:LLZ983040 LVV917509:LVV983040 MFR917509:MFR983040 MPN917509:MPN983040 MZJ917509:MZJ983040 NJF917509:NJF983040 NTB917509:NTB983040 OCX917509:OCX983040 OMT917509:OMT983040 OWP917509:OWP983040 PGL917509:PGL983040 PQH917509:PQH983040 QAD917509:QAD983040 QJZ917509:QJZ983040 QTV917509:QTV983040 RDR917509:RDR983040 RNN917509:RNN983040 RXJ917509:RXJ983040 SHF917509:SHF983040 SRB917509:SRB983040 TAX917509:TAX983040 TKT917509:TKT983040 TUP917509:TUP983040 UEL917509:UEL983040 UOH917509:UOH983040 UYD917509:UYD983040 VHZ917509:VHZ983040 VRV917509:VRV983040 WBR917509:WBR983040 WLN917509:WLN983040 WVJ917509:WVJ983040 B983045:B1048576 IX983045:IX1048576 ST983045:ST1048576 ACP983045:ACP1048576 AML983045:AML1048576 AWH983045:AWH1048576 BGD983045:BGD1048576 BPZ983045:BPZ1048576 BZV983045:BZV1048576 CJR983045:CJR1048576 CTN983045:CTN1048576 DDJ983045:DDJ1048576 DNF983045:DNF1048576 DXB983045:DXB1048576 EGX983045:EGX1048576 EQT983045:EQT1048576 FAP983045:FAP1048576 FKL983045:FKL1048576 FUH983045:FUH1048576 GED983045:GED1048576 GNZ983045:GNZ1048576 GXV983045:GXV1048576 HHR983045:HHR1048576 HRN983045:HRN1048576 IBJ983045:IBJ1048576 ILF983045:ILF1048576 IVB983045:IVB1048576 JEX983045:JEX1048576 JOT983045:JOT1048576 JYP983045:JYP1048576 KIL983045:KIL1048576 KSH983045:KSH1048576 LCD983045:LCD1048576 LLZ983045:LLZ1048576 LVV983045:LVV1048576 MFR983045:MFR1048576 MPN983045:MPN1048576 MZJ983045:MZJ1048576 NJF983045:NJF1048576 NTB983045:NTB1048576 OCX983045:OCX1048576 OMT983045:OMT1048576 OWP983045:OWP1048576 PGL983045:PGL1048576 PQH983045:PQH1048576 QAD983045:QAD1048576 QJZ983045:QJZ1048576 QTV983045:QTV1048576 RDR983045:RDR1048576 RNN983045:RNN1048576 RXJ983045:RXJ1048576 SHF983045:SHF1048576 SRB983045:SRB1048576 TAX983045:TAX1048576 TKT983045:TKT1048576 TUP983045:TUP1048576 UEL983045:UEL1048576 UOH983045:UOH1048576 UYD983045:UYD1048576 VHZ983045:VHZ1048576 VRV983045:VRV1048576 WBR983045:WBR1048576 WLN983045:WLN1048576 B5:B8 B10:B65536">
+    <dataValidation type="textLength" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="数据长度错误" error="数据长度必须在6-35个字符之间" sqref="WVJ983045:WVJ1048576 IX5:IX65536 ST5:ST65536 ACP5:ACP65536 AML5:AML65536 AWH5:AWH65536 BGD5:BGD65536 BPZ5:BPZ65536 BZV5:BZV65536 CJR5:CJR65536 CTN5:CTN65536 DDJ5:DDJ65536 DNF5:DNF65536 DXB5:DXB65536 EGX5:EGX65536 EQT5:EQT65536 FAP5:FAP65536 FKL5:FKL65536 FUH5:FUH65536 GED5:GED65536 GNZ5:GNZ65536 GXV5:GXV65536 HHR5:HHR65536 HRN5:HRN65536 IBJ5:IBJ65536 ILF5:ILF65536 IVB5:IVB65536 JEX5:JEX65536 JOT5:JOT65536 JYP5:JYP65536 KIL5:KIL65536 KSH5:KSH65536 LCD5:LCD65536 LLZ5:LLZ65536 LVV5:LVV65536 MFR5:MFR65536 MPN5:MPN65536 MZJ5:MZJ65536 NJF5:NJF65536 NTB5:NTB65536 OCX5:OCX65536 OMT5:OMT65536 OWP5:OWP65536 PGL5:PGL65536 PQH5:PQH65536 QAD5:QAD65536 QJZ5:QJZ65536 QTV5:QTV65536 RDR5:RDR65536 RNN5:RNN65536 RXJ5:RXJ65536 SHF5:SHF65536 SRB5:SRB65536 TAX5:TAX65536 TKT5:TKT65536 TUP5:TUP65536 UEL5:UEL65536 UOH5:UOH65536 UYD5:UYD65536 VHZ5:VHZ65536 VRV5:VRV65536 WBR5:WBR65536 WLN5:WLN65536 WVJ5:WVJ65536 B65541:B131072 IX65541:IX131072 ST65541:ST131072 ACP65541:ACP131072 AML65541:AML131072 AWH65541:AWH131072 BGD65541:BGD131072 BPZ65541:BPZ131072 BZV65541:BZV131072 CJR65541:CJR131072 CTN65541:CTN131072 DDJ65541:DDJ131072 DNF65541:DNF131072 DXB65541:DXB131072 EGX65541:EGX131072 EQT65541:EQT131072 FAP65541:FAP131072 FKL65541:FKL131072 FUH65541:FUH131072 GED65541:GED131072 GNZ65541:GNZ131072 GXV65541:GXV131072 HHR65541:HHR131072 HRN65541:HRN131072 IBJ65541:IBJ131072 ILF65541:ILF131072 IVB65541:IVB131072 JEX65541:JEX131072 JOT65541:JOT131072 JYP65541:JYP131072 KIL65541:KIL131072 KSH65541:KSH131072 LCD65541:LCD131072 LLZ65541:LLZ131072 LVV65541:LVV131072 MFR65541:MFR131072 MPN65541:MPN131072 MZJ65541:MZJ131072 NJF65541:NJF131072 NTB65541:NTB131072 OCX65541:OCX131072 OMT65541:OMT131072 OWP65541:OWP131072 PGL65541:PGL131072 PQH65541:PQH131072 QAD65541:QAD131072 QJZ65541:QJZ131072 QTV65541:QTV131072 RDR65541:RDR131072 RNN65541:RNN131072 RXJ65541:RXJ131072 SHF65541:SHF131072 SRB65541:SRB131072 TAX65541:TAX131072 TKT65541:TKT131072 TUP65541:TUP131072 UEL65541:UEL131072 UOH65541:UOH131072 UYD65541:UYD131072 VHZ65541:VHZ131072 VRV65541:VRV131072 WBR65541:WBR131072 WLN65541:WLN131072 WVJ65541:WVJ131072 B131077:B196608 IX131077:IX196608 ST131077:ST196608 ACP131077:ACP196608 AML131077:AML196608 AWH131077:AWH196608 BGD131077:BGD196608 BPZ131077:BPZ196608 BZV131077:BZV196608 CJR131077:CJR196608 CTN131077:CTN196608 DDJ131077:DDJ196608 DNF131077:DNF196608 DXB131077:DXB196608 EGX131077:EGX196608 EQT131077:EQT196608 FAP131077:FAP196608 FKL131077:FKL196608 FUH131077:FUH196608 GED131077:GED196608 GNZ131077:GNZ196608 GXV131077:GXV196608 HHR131077:HHR196608 HRN131077:HRN196608 IBJ131077:IBJ196608 ILF131077:ILF196608 IVB131077:IVB196608 JEX131077:JEX196608 JOT131077:JOT196608 JYP131077:JYP196608 KIL131077:KIL196608 KSH131077:KSH196608 LCD131077:LCD196608 LLZ131077:LLZ196608 LVV131077:LVV196608 MFR131077:MFR196608 MPN131077:MPN196608 MZJ131077:MZJ196608 NJF131077:NJF196608 NTB131077:NTB196608 OCX131077:OCX196608 OMT131077:OMT196608 OWP131077:OWP196608 PGL131077:PGL196608 PQH131077:PQH196608 QAD131077:QAD196608 QJZ131077:QJZ196608 QTV131077:QTV196608 RDR131077:RDR196608 RNN131077:RNN196608 RXJ131077:RXJ196608 SHF131077:SHF196608 SRB131077:SRB196608 TAX131077:TAX196608 TKT131077:TKT196608 TUP131077:TUP196608 UEL131077:UEL196608 UOH131077:UOH196608 UYD131077:UYD196608 VHZ131077:VHZ196608 VRV131077:VRV196608 WBR131077:WBR196608 WLN131077:WLN196608 WVJ131077:WVJ196608 B196613:B262144 IX196613:IX262144 ST196613:ST262144 ACP196613:ACP262144 AML196613:AML262144 AWH196613:AWH262144 BGD196613:BGD262144 BPZ196613:BPZ262144 BZV196613:BZV262144 CJR196613:CJR262144 CTN196613:CTN262144 DDJ196613:DDJ262144 DNF196613:DNF262144 DXB196613:DXB262144 EGX196613:EGX262144 EQT196613:EQT262144 FAP196613:FAP262144 FKL196613:FKL262144 FUH196613:FUH262144 GED196613:GED262144 GNZ196613:GNZ262144 GXV196613:GXV262144 HHR196613:HHR262144 HRN196613:HRN262144 IBJ196613:IBJ262144 ILF196613:ILF262144 IVB196613:IVB262144 JEX196613:JEX262144 JOT196613:JOT262144 JYP196613:JYP262144 KIL196613:KIL262144 KSH196613:KSH262144 LCD196613:LCD262144 LLZ196613:LLZ262144 LVV196613:LVV262144 MFR196613:MFR262144 MPN196613:MPN262144 MZJ196613:MZJ262144 NJF196613:NJF262144 NTB196613:NTB262144 OCX196613:OCX262144 OMT196613:OMT262144 OWP196613:OWP262144 PGL196613:PGL262144 PQH196613:PQH262144 QAD196613:QAD262144 QJZ196613:QJZ262144 QTV196613:QTV262144 RDR196613:RDR262144 RNN196613:RNN262144 RXJ196613:RXJ262144 SHF196613:SHF262144 SRB196613:SRB262144 TAX196613:TAX262144 TKT196613:TKT262144 TUP196613:TUP262144 UEL196613:UEL262144 UOH196613:UOH262144 UYD196613:UYD262144 VHZ196613:VHZ262144 VRV196613:VRV262144 WBR196613:WBR262144 WLN196613:WLN262144 WVJ196613:WVJ262144 B262149:B327680 IX262149:IX327680 ST262149:ST327680 ACP262149:ACP327680 AML262149:AML327680 AWH262149:AWH327680 BGD262149:BGD327680 BPZ262149:BPZ327680 BZV262149:BZV327680 CJR262149:CJR327680 CTN262149:CTN327680 DDJ262149:DDJ327680 DNF262149:DNF327680 DXB262149:DXB327680 EGX262149:EGX327680 EQT262149:EQT327680 FAP262149:FAP327680 FKL262149:FKL327680 FUH262149:FUH327680 GED262149:GED327680 GNZ262149:GNZ327680 GXV262149:GXV327680 HHR262149:HHR327680 HRN262149:HRN327680 IBJ262149:IBJ327680 ILF262149:ILF327680 IVB262149:IVB327680 JEX262149:JEX327680 JOT262149:JOT327680 JYP262149:JYP327680 KIL262149:KIL327680 KSH262149:KSH327680 LCD262149:LCD327680 LLZ262149:LLZ327680 LVV262149:LVV327680 MFR262149:MFR327680 MPN262149:MPN327680 MZJ262149:MZJ327680 NJF262149:NJF327680 NTB262149:NTB327680 OCX262149:OCX327680 OMT262149:OMT327680 OWP262149:OWP327680 PGL262149:PGL327680 PQH262149:PQH327680 QAD262149:QAD327680 QJZ262149:QJZ327680 QTV262149:QTV327680 RDR262149:RDR327680 RNN262149:RNN327680 RXJ262149:RXJ327680 SHF262149:SHF327680 SRB262149:SRB327680 TAX262149:TAX327680 TKT262149:TKT327680 TUP262149:TUP327680 UEL262149:UEL327680 UOH262149:UOH327680 UYD262149:UYD327680 VHZ262149:VHZ327680 VRV262149:VRV327680 WBR262149:WBR327680 WLN262149:WLN327680 WVJ262149:WVJ327680 B327685:B393216 IX327685:IX393216 ST327685:ST393216 ACP327685:ACP393216 AML327685:AML393216 AWH327685:AWH393216 BGD327685:BGD393216 BPZ327685:BPZ393216 BZV327685:BZV393216 CJR327685:CJR393216 CTN327685:CTN393216 DDJ327685:DDJ393216 DNF327685:DNF393216 DXB327685:DXB393216 EGX327685:EGX393216 EQT327685:EQT393216 FAP327685:FAP393216 FKL327685:FKL393216 FUH327685:FUH393216 GED327685:GED393216 GNZ327685:GNZ393216 GXV327685:GXV393216 HHR327685:HHR393216 HRN327685:HRN393216 IBJ327685:IBJ393216 ILF327685:ILF393216 IVB327685:IVB393216 JEX327685:JEX393216 JOT327685:JOT393216 JYP327685:JYP393216 KIL327685:KIL393216 KSH327685:KSH393216 LCD327685:LCD393216 LLZ327685:LLZ393216 LVV327685:LVV393216 MFR327685:MFR393216 MPN327685:MPN393216 MZJ327685:MZJ393216 NJF327685:NJF393216 NTB327685:NTB393216 OCX327685:OCX393216 OMT327685:OMT393216 OWP327685:OWP393216 PGL327685:PGL393216 PQH327685:PQH393216 QAD327685:QAD393216 QJZ327685:QJZ393216 QTV327685:QTV393216 RDR327685:RDR393216 RNN327685:RNN393216 RXJ327685:RXJ393216 SHF327685:SHF393216 SRB327685:SRB393216 TAX327685:TAX393216 TKT327685:TKT393216 TUP327685:TUP393216 UEL327685:UEL393216 UOH327685:UOH393216 UYD327685:UYD393216 VHZ327685:VHZ393216 VRV327685:VRV393216 WBR327685:WBR393216 WLN327685:WLN393216 WVJ327685:WVJ393216 B393221:B458752 IX393221:IX458752 ST393221:ST458752 ACP393221:ACP458752 AML393221:AML458752 AWH393221:AWH458752 BGD393221:BGD458752 BPZ393221:BPZ458752 BZV393221:BZV458752 CJR393221:CJR458752 CTN393221:CTN458752 DDJ393221:DDJ458752 DNF393221:DNF458752 DXB393221:DXB458752 EGX393221:EGX458752 EQT393221:EQT458752 FAP393221:FAP458752 FKL393221:FKL458752 FUH393221:FUH458752 GED393221:GED458752 GNZ393221:GNZ458752 GXV393221:GXV458752 HHR393221:HHR458752 HRN393221:HRN458752 IBJ393221:IBJ458752 ILF393221:ILF458752 IVB393221:IVB458752 JEX393221:JEX458752 JOT393221:JOT458752 JYP393221:JYP458752 KIL393221:KIL458752 KSH393221:KSH458752 LCD393221:LCD458752 LLZ393221:LLZ458752 LVV393221:LVV458752 MFR393221:MFR458752 MPN393221:MPN458752 MZJ393221:MZJ458752 NJF393221:NJF458752 NTB393221:NTB458752 OCX393221:OCX458752 OMT393221:OMT458752 OWP393221:OWP458752 PGL393221:PGL458752 PQH393221:PQH458752 QAD393221:QAD458752 QJZ393221:QJZ458752 QTV393221:QTV458752 RDR393221:RDR458752 RNN393221:RNN458752 RXJ393221:RXJ458752 SHF393221:SHF458752 SRB393221:SRB458752 TAX393221:TAX458752 TKT393221:TKT458752 TUP393221:TUP458752 UEL393221:UEL458752 UOH393221:UOH458752 UYD393221:UYD458752 VHZ393221:VHZ458752 VRV393221:VRV458752 WBR393221:WBR458752 WLN393221:WLN458752 WVJ393221:WVJ458752 B458757:B524288 IX458757:IX524288 ST458757:ST524288 ACP458757:ACP524288 AML458757:AML524288 AWH458757:AWH524288 BGD458757:BGD524288 BPZ458757:BPZ524288 BZV458757:BZV524288 CJR458757:CJR524288 CTN458757:CTN524288 DDJ458757:DDJ524288 DNF458757:DNF524288 DXB458757:DXB524288 EGX458757:EGX524288 EQT458757:EQT524288 FAP458757:FAP524288 FKL458757:FKL524288 FUH458757:FUH524288 GED458757:GED524288 GNZ458757:GNZ524288 GXV458757:GXV524288 HHR458757:HHR524288 HRN458757:HRN524288 IBJ458757:IBJ524288 ILF458757:ILF524288 IVB458757:IVB524288 JEX458757:JEX524288 JOT458757:JOT524288 JYP458757:JYP524288 KIL458757:KIL524288 KSH458757:KSH524288 LCD458757:LCD524288 LLZ458757:LLZ524288 LVV458757:LVV524288 MFR458757:MFR524288 MPN458757:MPN524288 MZJ458757:MZJ524288 NJF458757:NJF524288 NTB458757:NTB524288 OCX458757:OCX524288 OMT458757:OMT524288 OWP458757:OWP524288 PGL458757:PGL524288 PQH458757:PQH524288 QAD458757:QAD524288 QJZ458757:QJZ524288 QTV458757:QTV524288 RDR458757:RDR524288 RNN458757:RNN524288 RXJ458757:RXJ524288 SHF458757:SHF524288 SRB458757:SRB524288 TAX458757:TAX524288 TKT458757:TKT524288 TUP458757:TUP524288 UEL458757:UEL524288 UOH458757:UOH524288 UYD458757:UYD524288 VHZ458757:VHZ524288 VRV458757:VRV524288 WBR458757:WBR524288 WLN458757:WLN524288 WVJ458757:WVJ524288 B524293:B589824 IX524293:IX589824 ST524293:ST589824 ACP524293:ACP589824 AML524293:AML589824 AWH524293:AWH589824 BGD524293:BGD589824 BPZ524293:BPZ589824 BZV524293:BZV589824 CJR524293:CJR589824 CTN524293:CTN589824 DDJ524293:DDJ589824 DNF524293:DNF589824 DXB524293:DXB589824 EGX524293:EGX589824 EQT524293:EQT589824 FAP524293:FAP589824 FKL524293:FKL589824 FUH524293:FUH589824 GED524293:GED589824 GNZ524293:GNZ589824 GXV524293:GXV589824 HHR524293:HHR589824 HRN524293:HRN589824 IBJ524293:IBJ589824 ILF524293:ILF589824 IVB524293:IVB589824 JEX524293:JEX589824 JOT524293:JOT589824 JYP524293:JYP589824 KIL524293:KIL589824 KSH524293:KSH589824 LCD524293:LCD589824 LLZ524293:LLZ589824 LVV524293:LVV589824 MFR524293:MFR589824 MPN524293:MPN589824 MZJ524293:MZJ589824 NJF524293:NJF589824 NTB524293:NTB589824 OCX524293:OCX589824 OMT524293:OMT589824 OWP524293:OWP589824 PGL524293:PGL589824 PQH524293:PQH589824 QAD524293:QAD589824 QJZ524293:QJZ589824 QTV524293:QTV589824 RDR524293:RDR589824 RNN524293:RNN589824 RXJ524293:RXJ589824 SHF524293:SHF589824 SRB524293:SRB589824 TAX524293:TAX589824 TKT524293:TKT589824 TUP524293:TUP589824 UEL524293:UEL589824 UOH524293:UOH589824 UYD524293:UYD589824 VHZ524293:VHZ589824 VRV524293:VRV589824 WBR524293:WBR589824 WLN524293:WLN589824 WVJ524293:WVJ589824 B589829:B655360 IX589829:IX655360 ST589829:ST655360 ACP589829:ACP655360 AML589829:AML655360 AWH589829:AWH655360 BGD589829:BGD655360 BPZ589829:BPZ655360 BZV589829:BZV655360 CJR589829:CJR655360 CTN589829:CTN655360 DDJ589829:DDJ655360 DNF589829:DNF655360 DXB589829:DXB655360 EGX589829:EGX655360 EQT589829:EQT655360 FAP589829:FAP655360 FKL589829:FKL655360 FUH589829:FUH655360 GED589829:GED655360 GNZ589829:GNZ655360 GXV589829:GXV655360 HHR589829:HHR655360 HRN589829:HRN655360 IBJ589829:IBJ655360 ILF589829:ILF655360 IVB589829:IVB655360 JEX589829:JEX655360 JOT589829:JOT655360 JYP589829:JYP655360 KIL589829:KIL655360 KSH589829:KSH655360 LCD589829:LCD655360 LLZ589829:LLZ655360 LVV589829:LVV655360 MFR589829:MFR655360 MPN589829:MPN655360 MZJ589829:MZJ655360 NJF589829:NJF655360 NTB589829:NTB655360 OCX589829:OCX655360 OMT589829:OMT655360 OWP589829:OWP655360 PGL589829:PGL655360 PQH589829:PQH655360 QAD589829:QAD655360 QJZ589829:QJZ655360 QTV589829:QTV655360 RDR589829:RDR655360 RNN589829:RNN655360 RXJ589829:RXJ655360 SHF589829:SHF655360 SRB589829:SRB655360 TAX589829:TAX655360 TKT589829:TKT655360 TUP589829:TUP655360 UEL589829:UEL655360 UOH589829:UOH655360 UYD589829:UYD655360 VHZ589829:VHZ655360 VRV589829:VRV655360 WBR589829:WBR655360 WLN589829:WLN655360 WVJ589829:WVJ655360 B655365:B720896 IX655365:IX720896 ST655365:ST720896 ACP655365:ACP720896 AML655365:AML720896 AWH655365:AWH720896 BGD655365:BGD720896 BPZ655365:BPZ720896 BZV655365:BZV720896 CJR655365:CJR720896 CTN655365:CTN720896 DDJ655365:DDJ720896 DNF655365:DNF720896 DXB655365:DXB720896 EGX655365:EGX720896 EQT655365:EQT720896 FAP655365:FAP720896 FKL655365:FKL720896 FUH655365:FUH720896 GED655365:GED720896 GNZ655365:GNZ720896 GXV655365:GXV720896 HHR655365:HHR720896 HRN655365:HRN720896 IBJ655365:IBJ720896 ILF655365:ILF720896 IVB655365:IVB720896 JEX655365:JEX720896 JOT655365:JOT720896 JYP655365:JYP720896 KIL655365:KIL720896 KSH655365:KSH720896 LCD655365:LCD720896 LLZ655365:LLZ720896 LVV655365:LVV720896 MFR655365:MFR720896 MPN655365:MPN720896 MZJ655365:MZJ720896 NJF655365:NJF720896 NTB655365:NTB720896 OCX655365:OCX720896 OMT655365:OMT720896 OWP655365:OWP720896 PGL655365:PGL720896 PQH655365:PQH720896 QAD655365:QAD720896 QJZ655365:QJZ720896 QTV655365:QTV720896 RDR655365:RDR720896 RNN655365:RNN720896 RXJ655365:RXJ720896 SHF655365:SHF720896 SRB655365:SRB720896 TAX655365:TAX720896 TKT655365:TKT720896 TUP655365:TUP720896 UEL655365:UEL720896 UOH655365:UOH720896 UYD655365:UYD720896 VHZ655365:VHZ720896 VRV655365:VRV720896 WBR655365:WBR720896 WLN655365:WLN720896 WVJ655365:WVJ720896 B720901:B786432 IX720901:IX786432 ST720901:ST786432 ACP720901:ACP786432 AML720901:AML786432 AWH720901:AWH786432 BGD720901:BGD786432 BPZ720901:BPZ786432 BZV720901:BZV786432 CJR720901:CJR786432 CTN720901:CTN786432 DDJ720901:DDJ786432 DNF720901:DNF786432 DXB720901:DXB786432 EGX720901:EGX786432 EQT720901:EQT786432 FAP720901:FAP786432 FKL720901:FKL786432 FUH720901:FUH786432 GED720901:GED786432 GNZ720901:GNZ786432 GXV720901:GXV786432 HHR720901:HHR786432 HRN720901:HRN786432 IBJ720901:IBJ786432 ILF720901:ILF786432 IVB720901:IVB786432 JEX720901:JEX786432 JOT720901:JOT786432 JYP720901:JYP786432 KIL720901:KIL786432 KSH720901:KSH786432 LCD720901:LCD786432 LLZ720901:LLZ786432 LVV720901:LVV786432 MFR720901:MFR786432 MPN720901:MPN786432 MZJ720901:MZJ786432 NJF720901:NJF786432 NTB720901:NTB786432 OCX720901:OCX786432 OMT720901:OMT786432 OWP720901:OWP786432 PGL720901:PGL786432 PQH720901:PQH786432 QAD720901:QAD786432 QJZ720901:QJZ786432 QTV720901:QTV786432 RDR720901:RDR786432 RNN720901:RNN786432 RXJ720901:RXJ786432 SHF720901:SHF786432 SRB720901:SRB786432 TAX720901:TAX786432 TKT720901:TKT786432 TUP720901:TUP786432 UEL720901:UEL786432 UOH720901:UOH786432 UYD720901:UYD786432 VHZ720901:VHZ786432 VRV720901:VRV786432 WBR720901:WBR786432 WLN720901:WLN786432 WVJ720901:WVJ786432 B786437:B851968 IX786437:IX851968 ST786437:ST851968 ACP786437:ACP851968 AML786437:AML851968 AWH786437:AWH851968 BGD786437:BGD851968 BPZ786437:BPZ851968 BZV786437:BZV851968 CJR786437:CJR851968 CTN786437:CTN851968 DDJ786437:DDJ851968 DNF786437:DNF851968 DXB786437:DXB851968 EGX786437:EGX851968 EQT786437:EQT851968 FAP786437:FAP851968 FKL786437:FKL851968 FUH786437:FUH851968 GED786437:GED851968 GNZ786437:GNZ851968 GXV786437:GXV851968 HHR786437:HHR851968 HRN786437:HRN851968 IBJ786437:IBJ851968 ILF786437:ILF851968 IVB786437:IVB851968 JEX786437:JEX851968 JOT786437:JOT851968 JYP786437:JYP851968 KIL786437:KIL851968 KSH786437:KSH851968 LCD786437:LCD851968 LLZ786437:LLZ851968 LVV786437:LVV851968 MFR786437:MFR851968 MPN786437:MPN851968 MZJ786437:MZJ851968 NJF786437:NJF851968 NTB786437:NTB851968 OCX786437:OCX851968 OMT786437:OMT851968 OWP786437:OWP851968 PGL786437:PGL851968 PQH786437:PQH851968 QAD786437:QAD851968 QJZ786437:QJZ851968 QTV786437:QTV851968 RDR786437:RDR851968 RNN786437:RNN851968 RXJ786437:RXJ851968 SHF786437:SHF851968 SRB786437:SRB851968 TAX786437:TAX851968 TKT786437:TKT851968 TUP786437:TUP851968 UEL786437:UEL851968 UOH786437:UOH851968 UYD786437:UYD851968 VHZ786437:VHZ851968 VRV786437:VRV851968 WBR786437:WBR851968 WLN786437:WLN851968 WVJ786437:WVJ851968 B851973:B917504 IX851973:IX917504 ST851973:ST917504 ACP851973:ACP917504 AML851973:AML917504 AWH851973:AWH917504 BGD851973:BGD917504 BPZ851973:BPZ917504 BZV851973:BZV917504 CJR851973:CJR917504 CTN851973:CTN917504 DDJ851973:DDJ917504 DNF851973:DNF917504 DXB851973:DXB917504 EGX851973:EGX917504 EQT851973:EQT917504 FAP851973:FAP917504 FKL851973:FKL917504 FUH851973:FUH917504 GED851973:GED917504 GNZ851973:GNZ917504 GXV851973:GXV917504 HHR851973:HHR917504 HRN851973:HRN917504 IBJ851973:IBJ917504 ILF851973:ILF917504 IVB851973:IVB917504 JEX851973:JEX917504 JOT851973:JOT917504 JYP851973:JYP917504 KIL851973:KIL917504 KSH851973:KSH917504 LCD851973:LCD917504 LLZ851973:LLZ917504 LVV851973:LVV917504 MFR851973:MFR917504 MPN851973:MPN917504 MZJ851973:MZJ917504 NJF851973:NJF917504 NTB851973:NTB917504 OCX851973:OCX917504 OMT851973:OMT917504 OWP851973:OWP917504 PGL851973:PGL917504 PQH851973:PQH917504 QAD851973:QAD917504 QJZ851973:QJZ917504 QTV851973:QTV917504 RDR851973:RDR917504 RNN851973:RNN917504 RXJ851973:RXJ917504 SHF851973:SHF917504 SRB851973:SRB917504 TAX851973:TAX917504 TKT851973:TKT917504 TUP851973:TUP917504 UEL851973:UEL917504 UOH851973:UOH917504 UYD851973:UYD917504 VHZ851973:VHZ917504 VRV851973:VRV917504 WBR851973:WBR917504 WLN851973:WLN917504 WVJ851973:WVJ917504 B917509:B983040 IX917509:IX983040 ST917509:ST983040 ACP917509:ACP983040 AML917509:AML983040 AWH917509:AWH983040 BGD917509:BGD983040 BPZ917509:BPZ983040 BZV917509:BZV983040 CJR917509:CJR983040 CTN917509:CTN983040 DDJ917509:DDJ983040 DNF917509:DNF983040 DXB917509:DXB983040 EGX917509:EGX983040 EQT917509:EQT983040 FAP917509:FAP983040 FKL917509:FKL983040 FUH917509:FUH983040 GED917509:GED983040 GNZ917509:GNZ983040 GXV917509:GXV983040 HHR917509:HHR983040 HRN917509:HRN983040 IBJ917509:IBJ983040 ILF917509:ILF983040 IVB917509:IVB983040 JEX917509:JEX983040 JOT917509:JOT983040 JYP917509:JYP983040 KIL917509:KIL983040 KSH917509:KSH983040 LCD917509:LCD983040 LLZ917509:LLZ983040 LVV917509:LVV983040 MFR917509:MFR983040 MPN917509:MPN983040 MZJ917509:MZJ983040 NJF917509:NJF983040 NTB917509:NTB983040 OCX917509:OCX983040 OMT917509:OMT983040 OWP917509:OWP983040 PGL917509:PGL983040 PQH917509:PQH983040 QAD917509:QAD983040 QJZ917509:QJZ983040 QTV917509:QTV983040 RDR917509:RDR983040 RNN917509:RNN983040 RXJ917509:RXJ983040 SHF917509:SHF983040 SRB917509:SRB983040 TAX917509:TAX983040 TKT917509:TKT983040 TUP917509:TUP983040 UEL917509:UEL983040 UOH917509:UOH983040 UYD917509:UYD983040 VHZ917509:VHZ983040 VRV917509:VRV983040 WBR917509:WBR983040 WLN917509:WLN983040 WVJ917509:WVJ983040 B983045:B1048576 IX983045:IX1048576 ST983045:ST1048576 ACP983045:ACP1048576 AML983045:AML1048576 AWH983045:AWH1048576 BGD983045:BGD1048576 BPZ983045:BPZ1048576 BZV983045:BZV1048576 CJR983045:CJR1048576 CTN983045:CTN1048576 DDJ983045:DDJ1048576 DNF983045:DNF1048576 DXB983045:DXB1048576 EGX983045:EGX1048576 EQT983045:EQT1048576 FAP983045:FAP1048576 FKL983045:FKL1048576 FUH983045:FUH1048576 GED983045:GED1048576 GNZ983045:GNZ1048576 GXV983045:GXV1048576 HHR983045:HHR1048576 HRN983045:HRN1048576 IBJ983045:IBJ1048576 ILF983045:ILF1048576 IVB983045:IVB1048576 JEX983045:JEX1048576 JOT983045:JOT1048576 JYP983045:JYP1048576 KIL983045:KIL1048576 KSH983045:KSH1048576 LCD983045:LCD1048576 LLZ983045:LLZ1048576 LVV983045:LVV1048576 MFR983045:MFR1048576 MPN983045:MPN1048576 MZJ983045:MZJ1048576 NJF983045:NJF1048576 NTB983045:NTB1048576 OCX983045:OCX1048576 OMT983045:OMT1048576 OWP983045:OWP1048576 PGL983045:PGL1048576 PQH983045:PQH1048576 QAD983045:QAD1048576 QJZ983045:QJZ1048576 QTV983045:QTV1048576 RDR983045:RDR1048576 RNN983045:RNN1048576 RXJ983045:RXJ1048576 SHF983045:SHF1048576 SRB983045:SRB1048576 TAX983045:TAX1048576 TKT983045:TKT1048576 TUP983045:TUP1048576 UEL983045:UEL1048576 UOH983045:UOH1048576 UYD983045:UYD1048576 VHZ983045:VHZ1048576 VRV983045:VRV1048576 WBR983045:WBR1048576 WLN983045:WLN1048576 B5:B8 B10:B25 B27:B65536">
       <formula1>6</formula1>
       <formula2>35</formula2>
     </dataValidation>
@@ -2662,12 +2792,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F5" sqref="F5"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3138,10 +3268,93 @@
         <v>278</v>
       </c>
     </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>283</v>
+      </c>
+      <c r="C53" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>284</v>
+      </c>
+      <c r="C54" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B55" t="s">
+        <v>243</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>291</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>285</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>286</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>298</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>299</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>302</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>303</v>
+      </c>
+      <c r="C62" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="textLength" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="数据长度错误" error="数据长度必须在6-35个字符之间" sqref="C26 C12:C13 C10 C5:C6 C21 C32:C37 C39 C41 C43 C45 C47:C52">
+    <dataValidation type="textLength" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="数据长度错误" error="数据长度必须在6-35个字符之间" sqref="C26 C47:C55 C45 C43 C41 C39 C32:C37 C21 C5:C6 C10 C12:C13 C57:C59 C61:C62">
       <formula1>6</formula1>
       <formula2>35</formula2>
     </dataValidation>
@@ -3643,7 +3856,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
# fix bug program bug.
</commit_message>
<xml_diff>
--- a/bookmg/initial/cim.xlsx
+++ b/bookmg/initial/cim.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="2505" windowWidth="14295" windowHeight="7020" tabRatio="944" activeTab="2"/>
+    <workbookView xWindow="9555" yWindow="2505" windowWidth="14295" windowHeight="7020" tabRatio="944"/>
   </bookViews>
   <sheets>
     <sheet name="00-mgmemt.p" sheetId="8" r:id="rId1"/>
@@ -1371,14 +1371,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>图书借阅报表</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>读者借阅统计</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>v_bctype</t>
   </si>
   <si>
@@ -1454,6 +1446,14 @@
   </si>
   <si>
     <t>v_bkname</t>
+  </si>
+  <si>
+    <t>员工借阅统计报表</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>图书借阅统计报表</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1946,11 +1946,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5"/>
@@ -2136,7 +2136,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>281</v>
+        <v>303</v>
       </c>
       <c r="F9" t="s">
         <v>244</v>
@@ -2162,7 +2162,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="F10" t="s">
         <v>243</v>
@@ -2719,52 +2719,52 @@
         <v>42</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>287</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>293</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C26" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -2794,7 +2794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F5" sqref="F5"/>
       <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
@@ -3270,7 +3270,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C53" t="s">
         <v>166</v>
@@ -3278,7 +3278,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C54" t="s">
         <v>167</v>
@@ -3297,55 +3297,55 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
+        <v>283</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>285</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C62" t="s">
         <v>47</v>

</xml_diff>